<commit_message>
added a sample with corrupted gzip for testing
</commit_message>
<xml_diff>
--- a/tests/data/sftp_handle/datatest1/metadata_validation_test.xlsx
+++ b/tests/data/sftp_handle/datatest1/metadata_validation_test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1525" uniqueCount="797">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="800">
   <si>
     <t xml:space="preserve">Label name</t>
   </si>
@@ -884,6 +884,18 @@
     <t xml:space="preserve">SAMPLE6_R2.fastq.gz</t>
   </si>
   <si>
+    <t xml:space="preserve">corrupted-gzip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Illumina NextSeq 2000</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMPLE7.R1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMPLE7.R2.fastq.gz</t>
+  </si>
+  <si>
     <t xml:space="preserve">ARTIC v.4</t>
   </si>
   <si>
@@ -1377,9 +1389,6 @@
   </si>
   <si>
     <t xml:space="preserve">Bacteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Illumina NextSeq 2000</t>
   </si>
   <si>
     <t xml:space="preserve">TG HiSeq Rapid PE Cluster Kit v2</t>
@@ -3485,18 +3494,18 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="AV12 C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="72.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="111.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6388,10 +6397,10 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
@@ -6439,10 +6448,10 @@
         <v>27</v>
       </c>
       <c r="C2" s="59" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="E2" s="59" t="s">
         <v>193</v>
@@ -6473,13 +6482,13 @@
         <v>194</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="C3" s="117" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="D3" s="117" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="E3" s="117" t="s">
         <v>171</v>
@@ -7521,10 +7530,10 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
@@ -7565,7 +7574,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>176</v>
@@ -8591,18 +8600,18 @@
   </sheetPr>
   <dimension ref="A1:AV1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AN1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AU23" activeCellId="0" sqref="AU23"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="AV12" activeCellId="0" sqref="AV12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="42.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="40.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="48.7"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="48.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="22.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="29.86"/>
@@ -8619,20 +8628,20 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="23.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="20.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="19.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="28.99"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="28.98"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="38.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="26.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="21.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="36"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="30.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="30.02"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="38.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="32"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="34" min="34" style="0" width="26"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="28.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="33.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="33.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="33.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="24.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="24.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="27.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="14.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="13.29"/>
@@ -9808,52 +9817,96 @@
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="44"/>
       <c r="B12" s="34"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
+      <c r="C12" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="D12" s="41" t="s">
+        <v>283</v>
+      </c>
+      <c r="E12" s="41" t="s">
+        <v>283</v>
+      </c>
       <c r="F12" s="41"/>
-      <c r="G12" s="41"/>
+      <c r="G12" s="41" t="s">
+        <v>283</v>
+      </c>
       <c r="H12" s="41"/>
       <c r="I12" s="41"/>
       <c r="J12" s="41"/>
-      <c r="K12" s="41"/>
-      <c r="L12" s="41"/>
-      <c r="M12" s="41"/>
-      <c r="N12" s="41"/>
-      <c r="O12" s="41"/>
-      <c r="P12" s="41"/>
+      <c r="K12" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="L12" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="N12" s="39" t="s">
+        <v>277</v>
+      </c>
+      <c r="O12" s="39" t="s">
+        <v>278</v>
+      </c>
+      <c r="P12" s="41" t="s">
+        <v>60</v>
+      </c>
       <c r="Q12" s="41"/>
       <c r="R12" s="41"/>
       <c r="S12" s="41"/>
       <c r="T12" s="41"/>
       <c r="U12" s="41"/>
-      <c r="V12" s="41"/>
+      <c r="V12" s="41" t="s">
+        <v>85</v>
+      </c>
       <c r="W12" s="41"/>
       <c r="X12" s="41"/>
-      <c r="Y12" s="41"/>
+      <c r="Y12" s="39" t="s">
+        <v>280</v>
+      </c>
       <c r="Z12" s="41"/>
       <c r="AA12" s="41"/>
       <c r="AB12" s="41"/>
-      <c r="AC12" s="41"/>
+      <c r="AC12" s="41" t="s">
+        <v>111</v>
+      </c>
       <c r="AD12" s="41"/>
-      <c r="AE12" s="41"/>
+      <c r="AE12" s="41" t="s">
+        <v>207</v>
+      </c>
       <c r="AF12" s="41"/>
-      <c r="AG12" s="41"/>
+      <c r="AG12" s="41" t="s">
+        <v>208</v>
+      </c>
       <c r="AH12" s="41"/>
       <c r="AI12" s="41"/>
-      <c r="AJ12" s="41"/>
+      <c r="AJ12" s="41" t="s">
+        <v>284</v>
+      </c>
       <c r="AK12" s="41"/>
-      <c r="AL12" s="41"/>
-      <c r="AM12" s="41"/>
-      <c r="AN12" s="41"/>
-      <c r="AO12" s="41"/>
+      <c r="AL12" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM12" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="AN12" s="41" t="s">
+        <v>111</v>
+      </c>
+      <c r="AO12" s="41" t="s">
+        <v>210</v>
+      </c>
       <c r="AP12" s="41"/>
       <c r="AQ12" s="41"/>
       <c r="AR12" s="41"/>
       <c r="AS12" s="41"/>
       <c r="AT12" s="41"/>
-      <c r="AU12" s="41"/>
-      <c r="AV12" s="41"/>
+      <c r="AU12" s="41" t="s">
+        <v>285</v>
+      </c>
+      <c r="AV12" s="41" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="44"/>
@@ -12421,47 +12474,47 @@
   <dimension ref="A1:AV1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG15" activeCellId="0" sqref="AG15"/>
+      <selection pane="topLeft" activeCell="AG15" activeCellId="1" sqref="AV12 AG15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="2" style="0" width="0.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="2" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="60"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="61.29"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="13" style="0" width="0.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="60.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="61.3"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="13" style="0" width="0.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="60.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="38.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="40.42"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="0" width="0.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="18" min="18" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="41.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="56.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="32.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="23" min="23" style="0" width="0.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="23" min="23" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="10.71"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="25" style="0" width="0.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="25" min="25" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="25.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="95.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="62.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="24.29"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="0.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="30" min="30" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="67.86"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="32" min="32" style="0" width="0.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="32" min="32" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="33" min="33" style="0" width="27"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="34" style="0" width="0.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="34" min="34" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="35" min="35" style="0" width="32.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="32.86"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="71.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="44.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="44.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="43" min="43" style="0" width="0.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="43" min="43" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="44" min="44" style="0" width="15.71"/>
-    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="48" min="45" style="0" width="0.14"/>
+    <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="48" min="45" style="0" width="0.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -12608,7 +12661,7 @@
       </c>
       <c r="AF2" s="50"/>
       <c r="AG2" s="50" t="s">
-        <v>283</v>
+        <v>287</v>
       </c>
       <c r="AH2" s="50" t="n">
         <v>96</v>
@@ -12617,7 +12670,7 @@
         <v>131</v>
       </c>
       <c r="AJ2" s="50" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="AK2" s="50" t="s">
         <v>139</v>
@@ -12707,7 +12760,7 @@
         <v>71</v>
       </c>
       <c r="T3" s="56" t="s">
-        <v>285</v>
+        <v>289</v>
       </c>
       <c r="U3" s="56" t="s">
         <v>79</v>
@@ -12716,7 +12769,7 @@
         <v>84</v>
       </c>
       <c r="W3" s="56" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="X3" s="56" t="s">
         <v>91</v>
@@ -12783,10 +12836,10 @@
         <v>168</v>
       </c>
       <c r="AT3" s="59" t="s">
-        <v>287</v>
+        <v>291</v>
       </c>
       <c r="AU3" s="59" t="s">
-        <v>288</v>
+        <v>292</v>
       </c>
       <c r="AV3" s="59" t="s">
         <v>193</v>
@@ -12827,7 +12880,7 @@
         <v>42</v>
       </c>
       <c r="L4" s="28" t="s">
-        <v>289</v>
+        <v>293</v>
       </c>
       <c r="M4" s="28" t="s">
         <v>53</v>
@@ -12839,13 +12892,13 @@
         <v>58</v>
       </c>
       <c r="P4" s="28" t="s">
-        <v>290</v>
+        <v>294</v>
       </c>
       <c r="Q4" s="28" t="s">
         <v>66</v>
       </c>
       <c r="R4" s="28" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="S4" s="28" t="s">
         <v>70</v>
@@ -12884,13 +12937,13 @@
         <v>113</v>
       </c>
       <c r="AE4" s="28" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="AF4" s="28" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="AG4" s="28" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="AH4" s="28" t="s">
         <v>126</v>
@@ -12929,10 +12982,10 @@
         <v>167</v>
       </c>
       <c r="AT4" s="63" t="s">
-        <v>295</v>
+        <v>299</v>
       </c>
       <c r="AU4" s="63" t="s">
-        <v>296</v>
+        <v>300</v>
       </c>
       <c r="AV4" s="63" t="s">
         <v>171</v>
@@ -13012,11 +13065,11 @@
       </c>
       <c r="P6" s="67"/>
       <c r="Q6" s="67" t="s">
-        <v>297</v>
+        <v>301</v>
       </c>
       <c r="R6" s="67"/>
       <c r="S6" s="67" t="s">
-        <v>298</v>
+        <v>302</v>
       </c>
       <c r="T6" s="67" t="s">
         <v>76</v>
@@ -13029,15 +13082,15 @@
       </c>
       <c r="W6" s="67"/>
       <c r="X6" s="67" t="s">
-        <v>299</v>
+        <v>303</v>
       </c>
       <c r="Y6" s="67"/>
       <c r="Z6" s="67"/>
       <c r="AA6" s="67" t="s">
-        <v>300</v>
+        <v>304</v>
       </c>
       <c r="AB6" s="67" t="s">
-        <v>301</v>
+        <v>305</v>
       </c>
       <c r="AC6" s="67" t="s">
         <v>111</v>
@@ -13048,21 +13101,21 @@
       </c>
       <c r="AF6" s="67"/>
       <c r="AG6" s="67" t="s">
-        <v>302</v>
+        <v>306</v>
       </c>
       <c r="AH6" s="67"/>
       <c r="AI6" s="67"/>
       <c r="AJ6" s="67" t="s">
-        <v>303</v>
+        <v>307</v>
       </c>
       <c r="AK6" s="67" t="s">
-        <v>304</v>
+        <v>308</v>
       </c>
       <c r="AL6" s="67" t="s">
         <v>235</v>
       </c>
       <c r="AM6" s="67" t="s">
-        <v>305</v>
+        <v>309</v>
       </c>
       <c r="AN6" s="67" t="s">
         <v>151</v>
@@ -13071,11 +13124,11 @@
         <v>237</v>
       </c>
       <c r="AP6" s="67" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
       <c r="AQ6" s="67"/>
       <c r="AR6" s="67" t="s">
-        <v>306</v>
+        <v>310</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13090,10 +13143,10 @@
       <c r="I7" s="67"/>
       <c r="J7" s="67"/>
       <c r="K7" s="67" t="s">
-        <v>307</v>
+        <v>311</v>
       </c>
       <c r="L7" s="67" t="s">
-        <v>308</v>
+        <v>312</v>
       </c>
       <c r="M7" s="67"/>
       <c r="N7" s="67"/>
@@ -13102,54 +13155,54 @@
       </c>
       <c r="P7" s="67"/>
       <c r="Q7" s="67" t="s">
-        <v>309</v>
+        <v>313</v>
       </c>
       <c r="R7" s="67"/>
       <c r="S7" s="67" t="s">
-        <v>310</v>
+        <v>314</v>
       </c>
       <c r="T7" s="67" t="s">
-        <v>311</v>
+        <v>315</v>
       </c>
       <c r="U7" s="67" t="s">
         <v>202</v>
       </c>
       <c r="V7" s="67" t="s">
-        <v>312</v>
+        <v>316</v>
       </c>
       <c r="W7" s="67"/>
       <c r="X7" s="67" t="s">
-        <v>313</v>
+        <v>317</v>
       </c>
       <c r="Y7" s="67"/>
       <c r="Z7" s="67"/>
       <c r="AA7" s="67" t="s">
-        <v>314</v>
+        <v>318</v>
       </c>
       <c r="AB7" s="67" t="s">
         <v>233</v>
       </c>
       <c r="AC7" s="67" t="s">
-        <v>315</v>
+        <v>319</v>
       </c>
       <c r="AD7" s="67"/>
       <c r="AE7" s="67" t="s">
-        <v>316</v>
+        <v>320</v>
       </c>
       <c r="AF7" s="67"/>
       <c r="AG7" s="67" t="s">
-        <v>317</v>
+        <v>321</v>
       </c>
       <c r="AH7" s="67"/>
       <c r="AI7" s="67"/>
       <c r="AJ7" s="67" t="s">
-        <v>318</v>
+        <v>322</v>
       </c>
       <c r="AK7" s="67" t="s">
-        <v>319</v>
+        <v>323</v>
       </c>
       <c r="AL7" s="67" t="s">
-        <v>320</v>
+        <v>324</v>
       </c>
       <c r="AM7" s="67" t="s">
         <v>270</v>
@@ -13161,11 +13214,11 @@
         <v>210</v>
       </c>
       <c r="AP7" s="67" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
       <c r="AQ7" s="67"/>
       <c r="AR7" s="67" t="s">
-        <v>321</v>
+        <v>325</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13180,47 +13233,47 @@
       <c r="I8" s="67"/>
       <c r="J8" s="67"/>
       <c r="K8" s="67" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="L8" s="67" t="s">
-        <v>322</v>
+        <v>326</v>
       </c>
       <c r="M8" s="67"/>
       <c r="N8" s="67"/>
       <c r="O8" s="68"/>
       <c r="P8" s="67"/>
       <c r="Q8" s="67" t="s">
-        <v>323</v>
+        <v>327</v>
       </c>
       <c r="R8" s="67"/>
       <c r="S8" s="67" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="T8" s="67" t="s">
-        <v>325</v>
+        <v>329</v>
       </c>
       <c r="U8" s="67"/>
       <c r="V8" s="67" t="s">
-        <v>326</v>
+        <v>330</v>
       </c>
       <c r="W8" s="67"/>
       <c r="X8" s="67" t="s">
-        <v>327</v>
+        <v>331</v>
       </c>
       <c r="Y8" s="67"/>
       <c r="Z8" s="67"/>
       <c r="AA8" s="67" t="s">
-        <v>328</v>
+        <v>332</v>
       </c>
       <c r="AB8" s="67" t="s">
-        <v>329</v>
+        <v>333</v>
       </c>
       <c r="AC8" s="67" t="s">
-        <v>330</v>
+        <v>334</v>
       </c>
       <c r="AD8" s="67"/>
       <c r="AE8" s="67" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="AF8" s="67"/>
       <c r="AG8" s="67" t="s">
@@ -13229,27 +13282,27 @@
       <c r="AH8" s="67"/>
       <c r="AI8" s="67"/>
       <c r="AJ8" s="67" t="s">
-        <v>332</v>
+        <v>336</v>
       </c>
       <c r="AK8" s="67" t="s">
-        <v>333</v>
+        <v>337</v>
       </c>
       <c r="AL8" s="67" t="s">
-        <v>334</v>
+        <v>338</v>
       </c>
       <c r="AM8" s="67" t="s">
-        <v>335</v>
+        <v>339</v>
       </c>
       <c r="AN8" s="67" t="s">
-        <v>336</v>
+        <v>340</v>
       </c>
       <c r="AO8" s="67"/>
       <c r="AP8" s="67" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
       <c r="AQ8" s="67"/>
       <c r="AR8" s="67" t="s">
-        <v>337</v>
+        <v>341</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13264,28 +13317,28 @@
       <c r="I9" s="67"/>
       <c r="J9" s="67"/>
       <c r="K9" s="67" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="L9" s="67" t="s">
-        <v>338</v>
+        <v>342</v>
       </c>
       <c r="M9" s="67"/>
       <c r="N9" s="67"/>
       <c r="O9" s="68"/>
       <c r="P9" s="67"/>
       <c r="Q9" s="67" t="s">
-        <v>339</v>
+        <v>343</v>
       </c>
       <c r="R9" s="67"/>
       <c r="S9" s="67" t="s">
-        <v>340</v>
+        <v>344</v>
       </c>
       <c r="T9" s="67" t="s">
-        <v>341</v>
+        <v>345</v>
       </c>
       <c r="U9" s="67"/>
       <c r="V9" s="67" t="s">
-        <v>342</v>
+        <v>346</v>
       </c>
       <c r="W9" s="67"/>
       <c r="X9" s="67" t="s">
@@ -13294,13 +13347,13 @@
       <c r="Y9" s="67"/>
       <c r="Z9" s="67"/>
       <c r="AA9" s="67" t="s">
-        <v>343</v>
+        <v>347</v>
       </c>
       <c r="AB9" s="67" t="s">
-        <v>344</v>
+        <v>348</v>
       </c>
       <c r="AC9" s="67" t="s">
-        <v>345</v>
+        <v>349</v>
       </c>
       <c r="AD9" s="67"/>
       <c r="AE9" s="67" t="s">
@@ -13313,13 +13366,13 @@
       <c r="AH9" s="67"/>
       <c r="AI9" s="67"/>
       <c r="AJ9" s="67" t="s">
-        <v>346</v>
+        <v>350</v>
       </c>
       <c r="AK9" s="67" t="s">
-        <v>347</v>
+        <v>351</v>
       </c>
       <c r="AL9" s="67" t="s">
-        <v>348</v>
+        <v>352</v>
       </c>
       <c r="AM9" s="67" t="s">
         <v>99</v>
@@ -13329,11 +13382,11 @@
       </c>
       <c r="AO9" s="67"/>
       <c r="AP9" s="67" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
       <c r="AQ9" s="67"/>
       <c r="AR9" s="67" t="s">
-        <v>349</v>
+        <v>353</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13348,21 +13401,21 @@
       <c r="I10" s="67"/>
       <c r="J10" s="67"/>
       <c r="K10" s="67" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="L10" s="67" t="s">
-        <v>350</v>
+        <v>354</v>
       </c>
       <c r="M10" s="67"/>
       <c r="N10" s="67"/>
       <c r="O10" s="68"/>
       <c r="P10" s="67"/>
       <c r="Q10" s="67" t="s">
-        <v>351</v>
+        <v>355</v>
       </c>
       <c r="R10" s="67"/>
       <c r="S10" s="67" t="s">
-        <v>352</v>
+        <v>356</v>
       </c>
       <c r="T10" s="67" t="s">
         <v>202</v>
@@ -13376,13 +13429,13 @@
       <c r="Y10" s="67"/>
       <c r="Z10" s="67"/>
       <c r="AA10" s="67" t="s">
-        <v>353</v>
+        <v>357</v>
       </c>
       <c r="AB10" s="67" t="s">
-        <v>354</v>
+        <v>358</v>
       </c>
       <c r="AC10" s="67" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="AD10" s="67"/>
       <c r="AE10" s="67" t="s">
@@ -13395,27 +13448,27 @@
       <c r="AH10" s="67"/>
       <c r="AI10" s="67"/>
       <c r="AJ10" s="67" t="s">
-        <v>356</v>
+        <v>360</v>
       </c>
       <c r="AK10" s="67" t="s">
-        <v>357</v>
+        <v>361</v>
       </c>
       <c r="AL10" s="67" t="s">
-        <v>358</v>
+        <v>362</v>
       </c>
       <c r="AM10" s="67" t="s">
-        <v>359</v>
+        <v>363</v>
       </c>
       <c r="AN10" s="67" t="s">
-        <v>360</v>
+        <v>364</v>
       </c>
       <c r="AO10" s="67"/>
       <c r="AP10" s="67" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
       <c r="AQ10" s="67"/>
       <c r="AR10" s="67" t="s">
-        <v>361</v>
+        <v>365</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13430,21 +13483,21 @@
       <c r="I11" s="67"/>
       <c r="J11" s="67"/>
       <c r="K11" s="67" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="L11" s="67" t="s">
-        <v>362</v>
+        <v>366</v>
       </c>
       <c r="M11" s="67"/>
       <c r="N11" s="67"/>
       <c r="O11" s="68"/>
       <c r="P11" s="67"/>
       <c r="Q11" s="67" t="s">
-        <v>363</v>
+        <v>367</v>
       </c>
       <c r="R11" s="67"/>
       <c r="S11" s="67" t="s">
-        <v>364</v>
+        <v>368</v>
       </c>
       <c r="T11" s="67"/>
       <c r="U11" s="67"/>
@@ -13454,46 +13507,46 @@
       <c r="Y11" s="67"/>
       <c r="Z11" s="67"/>
       <c r="AA11" s="67" t="s">
-        <v>365</v>
+        <v>369</v>
       </c>
       <c r="AB11" s="67" t="s">
-        <v>366</v>
+        <v>370</v>
       </c>
       <c r="AC11" s="67" t="s">
         <v>202</v>
       </c>
       <c r="AD11" s="67"/>
       <c r="AE11" s="67" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="AF11" s="67"/>
       <c r="AG11" s="67" t="s">
-        <v>331</v>
+        <v>335</v>
       </c>
       <c r="AH11" s="67"/>
       <c r="AI11" s="67"/>
       <c r="AJ11" s="67" t="s">
-        <v>368</v>
+        <v>372</v>
       </c>
       <c r="AK11" s="67" t="s">
-        <v>369</v>
+        <v>373</v>
       </c>
       <c r="AL11" s="67" t="s">
         <v>209</v>
       </c>
       <c r="AM11" s="67" t="s">
-        <v>370</v>
+        <v>374</v>
       </c>
       <c r="AN11" s="67" t="s">
-        <v>371</v>
+        <v>375</v>
       </c>
       <c r="AO11" s="67"/>
       <c r="AP11" s="67" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
       <c r="AQ11" s="67"/>
       <c r="AR11" s="67" t="s">
-        <v>372</v>
+        <v>376</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13508,21 +13561,21 @@
       <c r="I12" s="67"/>
       <c r="J12" s="67"/>
       <c r="K12" s="67" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="L12" s="67" t="s">
-        <v>373</v>
+        <v>377</v>
       </c>
       <c r="M12" s="67"/>
       <c r="N12" s="67"/>
       <c r="O12" s="68"/>
       <c r="P12" s="67"/>
       <c r="Q12" s="67" t="s">
-        <v>374</v>
+        <v>378</v>
       </c>
       <c r="R12" s="67"/>
       <c r="S12" s="67" t="s">
-        <v>375</v>
+        <v>379</v>
       </c>
       <c r="T12" s="67"/>
       <c r="U12" s="67"/>
@@ -13535,12 +13588,12 @@
         <v>206</v>
       </c>
       <c r="AB12" s="67" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="AC12" s="67"/>
       <c r="AD12" s="67"/>
       <c r="AE12" s="67" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="AF12" s="67"/>
       <c r="AG12" s="67" t="s">
@@ -13549,27 +13602,27 @@
       <c r="AH12" s="67"/>
       <c r="AI12" s="67"/>
       <c r="AJ12" s="67" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="AK12" s="67" t="s">
-        <v>379</v>
+        <v>383</v>
       </c>
       <c r="AL12" s="67" t="s">
-        <v>380</v>
+        <v>384</v>
       </c>
       <c r="AM12" s="67" t="s">
-        <v>381</v>
+        <v>385</v>
       </c>
       <c r="AN12" s="67" t="s">
-        <v>382</v>
+        <v>386</v>
       </c>
       <c r="AO12" s="67"/>
       <c r="AP12" s="67" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
       <c r="AQ12" s="67"/>
       <c r="AR12" s="67" t="s">
-        <v>383</v>
+        <v>387</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13584,21 +13637,21 @@
       <c r="I13" s="67"/>
       <c r="J13" s="67"/>
       <c r="K13" s="67" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="L13" s="67" t="s">
-        <v>384</v>
+        <v>388</v>
       </c>
       <c r="M13" s="67"/>
       <c r="N13" s="67"/>
       <c r="O13" s="68"/>
       <c r="P13" s="67"/>
       <c r="Q13" s="67" t="s">
-        <v>385</v>
+        <v>389</v>
       </c>
       <c r="R13" s="67"/>
       <c r="S13" s="67" t="s">
-        <v>386</v>
+        <v>390</v>
       </c>
       <c r="T13" s="67"/>
       <c r="U13" s="67"/>
@@ -13608,44 +13661,44 @@
       <c r="Y13" s="67"/>
       <c r="Z13" s="67"/>
       <c r="AA13" s="67" t="s">
-        <v>387</v>
+        <v>391</v>
       </c>
       <c r="AB13" s="67" t="s">
-        <v>388</v>
+        <v>392</v>
       </c>
       <c r="AC13" s="67"/>
       <c r="AD13" s="67"/>
       <c r="AE13" s="67" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="AF13" s="67"/>
       <c r="AG13" s="67" t="s">
-        <v>390</v>
+        <v>394</v>
       </c>
       <c r="AH13" s="67"/>
       <c r="AI13" s="67"/>
       <c r="AJ13" s="67" t="s">
-        <v>391</v>
+        <v>395</v>
       </c>
       <c r="AK13" s="67" t="s">
-        <v>392</v>
+        <v>396</v>
       </c>
       <c r="AL13" s="67" t="s">
-        <v>393</v>
+        <v>397</v>
       </c>
       <c r="AM13" s="67" t="s">
-        <v>394</v>
+        <v>398</v>
       </c>
       <c r="AN13" s="67" t="s">
-        <v>395</v>
+        <v>399</v>
       </c>
       <c r="AO13" s="67"/>
       <c r="AP13" s="67" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
       <c r="AQ13" s="67"/>
       <c r="AR13" s="67" t="s">
-        <v>396</v>
+        <v>400</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13660,21 +13713,21 @@
       <c r="I14" s="67"/>
       <c r="J14" s="67"/>
       <c r="K14" s="67" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="L14" s="67" t="s">
-        <v>397</v>
+        <v>401</v>
       </c>
       <c r="M14" s="67"/>
       <c r="N14" s="67"/>
       <c r="O14" s="68"/>
       <c r="P14" s="67"/>
       <c r="Q14" s="67" t="s">
-        <v>398</v>
+        <v>402</v>
       </c>
       <c r="R14" s="67"/>
       <c r="S14" s="67" t="s">
-        <v>399</v>
+        <v>403</v>
       </c>
       <c r="T14" s="67"/>
       <c r="U14" s="67"/>
@@ -13687,7 +13740,7 @@
         <v>202</v>
       </c>
       <c r="AB14" s="67" t="s">
-        <v>400</v>
+        <v>404</v>
       </c>
       <c r="AC14" s="67"/>
       <c r="AD14" s="67"/>
@@ -13696,32 +13749,32 @@
       </c>
       <c r="AF14" s="67"/>
       <c r="AG14" s="67" t="s">
-        <v>401</v>
+        <v>405</v>
       </c>
       <c r="AH14" s="67"/>
       <c r="AI14" s="67"/>
       <c r="AJ14" s="67" t="s">
-        <v>402</v>
+        <v>406</v>
       </c>
       <c r="AK14" s="67" t="s">
-        <v>403</v>
+        <v>407</v>
       </c>
       <c r="AL14" s="67" t="s">
-        <v>404</v>
+        <v>408</v>
       </c>
       <c r="AM14" s="67" t="s">
-        <v>405</v>
+        <v>409</v>
       </c>
       <c r="AN14" s="67" t="s">
-        <v>406</v>
+        <v>410</v>
       </c>
       <c r="AO14" s="67"/>
       <c r="AP14" s="67" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
       <c r="AQ14" s="67"/>
       <c r="AR14" s="67" t="s">
-        <v>407</v>
+        <v>411</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13736,21 +13789,21 @@
       <c r="I15" s="67"/>
       <c r="J15" s="67"/>
       <c r="K15" s="67" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="L15" s="67" t="s">
-        <v>408</v>
+        <v>412</v>
       </c>
       <c r="M15" s="67"/>
       <c r="N15" s="67"/>
       <c r="O15" s="68"/>
       <c r="P15" s="67"/>
       <c r="Q15" s="67" t="s">
-        <v>409</v>
+        <v>413</v>
       </c>
       <c r="R15" s="67"/>
       <c r="S15" s="67" t="s">
-        <v>410</v>
+        <v>414</v>
       </c>
       <c r="T15" s="67"/>
       <c r="U15" s="67"/>
@@ -13761,7 +13814,7 @@
       <c r="Z15" s="67"/>
       <c r="AA15" s="67"/>
       <c r="AB15" s="67" t="s">
-        <v>411</v>
+        <v>415</v>
       </c>
       <c r="AC15" s="67"/>
       <c r="AD15" s="67"/>
@@ -13773,25 +13826,25 @@
       <c r="AH15" s="67"/>
       <c r="AI15" s="67"/>
       <c r="AJ15" s="67" t="s">
-        <v>412</v>
+        <v>416</v>
       </c>
       <c r="AK15" s="67" t="s">
-        <v>413</v>
+        <v>417</v>
       </c>
       <c r="AL15" s="67"/>
       <c r="AM15" s="67" t="s">
-        <v>414</v>
+        <v>418</v>
       </c>
       <c r="AN15" s="67" t="s">
-        <v>415</v>
+        <v>419</v>
       </c>
       <c r="AO15" s="67"/>
       <c r="AP15" s="67" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
       <c r="AQ15" s="67"/>
       <c r="AR15" s="67" t="s">
-        <v>416</v>
+        <v>420</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13806,17 +13859,17 @@
       <c r="I16" s="67"/>
       <c r="J16" s="67"/>
       <c r="K16" s="67" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="L16" s="67" t="s">
-        <v>417</v>
+        <v>421</v>
       </c>
       <c r="M16" s="67"/>
       <c r="N16" s="67"/>
       <c r="O16" s="68"/>
       <c r="P16" s="67"/>
       <c r="Q16" s="67" t="s">
-        <v>418</v>
+        <v>422</v>
       </c>
       <c r="R16" s="67"/>
       <c r="S16" s="67" t="s">
@@ -13831,29 +13884,29 @@
       <c r="Z16" s="67"/>
       <c r="AA16" s="67"/>
       <c r="AB16" s="67" t="s">
-        <v>419</v>
+        <v>423</v>
       </c>
       <c r="AC16" s="67"/>
       <c r="AD16" s="67"/>
       <c r="AE16" s="67"/>
       <c r="AF16" s="67"/>
       <c r="AG16" s="67" t="s">
-        <v>367</v>
+        <v>371</v>
       </c>
       <c r="AH16" s="67"/>
       <c r="AI16" s="67"/>
       <c r="AJ16" s="67" t="s">
-        <v>420</v>
+        <v>424</v>
       </c>
       <c r="AK16" s="67" t="s">
-        <v>421</v>
+        <v>425</v>
       </c>
       <c r="AL16" s="67"/>
       <c r="AM16" s="67" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="AN16" s="67" t="s">
-        <v>423</v>
+        <v>427</v>
       </c>
       <c r="AO16" s="67"/>
       <c r="AP16" s="67" t="s">
@@ -13876,21 +13929,21 @@
       <c r="I17" s="67"/>
       <c r="J17" s="67"/>
       <c r="K17" s="67" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="L17" s="67" t="s">
-        <v>424</v>
+        <v>428</v>
       </c>
       <c r="M17" s="67"/>
       <c r="N17" s="67"/>
       <c r="O17" s="68"/>
       <c r="P17" s="67"/>
       <c r="Q17" s="67" t="s">
-        <v>425</v>
+        <v>429</v>
       </c>
       <c r="R17" s="67"/>
       <c r="S17" s="67" t="s">
-        <v>426</v>
+        <v>430</v>
       </c>
       <c r="T17" s="67"/>
       <c r="U17" s="67"/>
@@ -13901,29 +13954,29 @@
       <c r="Z17" s="67"/>
       <c r="AA17" s="67"/>
       <c r="AB17" s="67" t="s">
-        <v>427</v>
+        <v>431</v>
       </c>
       <c r="AC17" s="67"/>
       <c r="AD17" s="67"/>
       <c r="AE17" s="67"/>
       <c r="AF17" s="67"/>
       <c r="AG17" s="67" t="s">
-        <v>377</v>
+        <v>381</v>
       </c>
       <c r="AH17" s="67"/>
       <c r="AI17" s="67"/>
       <c r="AJ17" s="67" t="s">
-        <v>284</v>
+        <v>288</v>
       </c>
       <c r="AK17" s="67" t="s">
-        <v>428</v>
+        <v>432</v>
       </c>
       <c r="AL17" s="67"/>
       <c r="AM17" s="67" t="s">
-        <v>429</v>
+        <v>433</v>
       </c>
       <c r="AN17" s="67" t="s">
-        <v>430</v>
+        <v>434</v>
       </c>
       <c r="AO17" s="67"/>
       <c r="AP17" s="67"/>
@@ -13942,21 +13995,21 @@
       <c r="I18" s="67"/>
       <c r="J18" s="67"/>
       <c r="K18" s="67" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="L18" s="67" t="s">
-        <v>431</v>
+        <v>435</v>
       </c>
       <c r="M18" s="67"/>
       <c r="N18" s="67"/>
       <c r="O18" s="68"/>
       <c r="P18" s="67"/>
       <c r="Q18" s="67" t="s">
-        <v>432</v>
+        <v>436</v>
       </c>
       <c r="R18" s="67"/>
       <c r="S18" s="67" t="s">
-        <v>433</v>
+        <v>437</v>
       </c>
       <c r="T18" s="67"/>
       <c r="U18" s="67"/>
@@ -13974,7 +14027,7 @@
       <c r="AE18" s="67"/>
       <c r="AF18" s="67"/>
       <c r="AG18" s="67" t="s">
-        <v>389</v>
+        <v>393</v>
       </c>
       <c r="AH18" s="67"/>
       <c r="AI18" s="67"/>
@@ -13982,14 +14035,14 @@
         <v>187</v>
       </c>
       <c r="AK18" s="67" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
       <c r="AL18" s="67"/>
       <c r="AM18" s="67" t="s">
-        <v>435</v>
+        <v>439</v>
       </c>
       <c r="AN18" s="67" t="s">
-        <v>436</v>
+        <v>440</v>
       </c>
       <c r="AO18" s="67"/>
       <c r="AP18" s="67"/>
@@ -14008,21 +14061,21 @@
       <c r="I19" s="67"/>
       <c r="J19" s="67"/>
       <c r="K19" s="67" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="L19" s="67" t="s">
-        <v>437</v>
+        <v>441</v>
       </c>
       <c r="M19" s="67"/>
       <c r="N19" s="67"/>
       <c r="O19" s="68"/>
       <c r="P19" s="67"/>
       <c r="Q19" s="67" t="s">
-        <v>438</v>
+        <v>442</v>
       </c>
       <c r="R19" s="67"/>
       <c r="S19" s="67" t="s">
-        <v>439</v>
+        <v>443</v>
       </c>
       <c r="T19" s="67"/>
       <c r="U19" s="67"/>
@@ -14033,7 +14086,7 @@
       <c r="Z19" s="67"/>
       <c r="AA19" s="67"/>
       <c r="AB19" s="67" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="AC19" s="67"/>
       <c r="AD19" s="67"/>
@@ -14045,17 +14098,17 @@
       <c r="AH19" s="67"/>
       <c r="AI19" s="67"/>
       <c r="AJ19" s="67" t="s">
-        <v>441</v>
+        <v>445</v>
       </c>
       <c r="AK19" s="67" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
       <c r="AL19" s="67"/>
       <c r="AM19" s="67" t="s">
-        <v>443</v>
+        <v>447</v>
       </c>
       <c r="AN19" s="67" t="s">
-        <v>444</v>
+        <v>448</v>
       </c>
       <c r="AO19" s="67"/>
       <c r="AP19" s="67"/>
@@ -14074,21 +14127,21 @@
       <c r="I20" s="67"/>
       <c r="J20" s="67"/>
       <c r="K20" s="67" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="L20" s="67" t="s">
-        <v>445</v>
+        <v>449</v>
       </c>
       <c r="M20" s="67"/>
       <c r="N20" s="67"/>
       <c r="O20" s="68"/>
       <c r="P20" s="67"/>
       <c r="Q20" s="67" t="s">
-        <v>446</v>
+        <v>450</v>
       </c>
       <c r="R20" s="67"/>
       <c r="S20" s="67" t="s">
-        <v>447</v>
+        <v>451</v>
       </c>
       <c r="T20" s="67"/>
       <c r="U20" s="67"/>
@@ -14099,7 +14152,7 @@
       <c r="Z20" s="67"/>
       <c r="AA20" s="67"/>
       <c r="AB20" s="67" t="s">
-        <v>440</v>
+        <v>444</v>
       </c>
       <c r="AC20" s="67"/>
       <c r="AD20" s="67"/>
@@ -14109,17 +14162,17 @@
       <c r="AH20" s="67"/>
       <c r="AI20" s="67"/>
       <c r="AJ20" s="67" t="s">
-        <v>448</v>
+        <v>284</v>
       </c>
       <c r="AK20" s="67" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
       <c r="AL20" s="67"/>
       <c r="AM20" s="67" t="s">
-        <v>450</v>
+        <v>453</v>
       </c>
       <c r="AN20" s="67" t="s">
-        <v>451</v>
+        <v>454</v>
       </c>
       <c r="AO20" s="67"/>
       <c r="AP20" s="67"/>
@@ -14138,21 +14191,21 @@
       <c r="I21" s="67"/>
       <c r="J21" s="67"/>
       <c r="K21" s="69" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="L21" s="69" t="s">
-        <v>452</v>
+        <v>455</v>
       </c>
       <c r="M21" s="67"/>
       <c r="N21" s="67"/>
       <c r="O21" s="68"/>
       <c r="P21" s="67"/>
       <c r="Q21" s="67" t="s">
-        <v>453</v>
+        <v>456</v>
       </c>
       <c r="R21" s="67"/>
       <c r="S21" s="67" t="s">
-        <v>454</v>
+        <v>457</v>
       </c>
       <c r="T21" s="67"/>
       <c r="U21" s="67"/>
@@ -14163,7 +14216,7 @@
       <c r="Z21" s="67"/>
       <c r="AA21" s="67"/>
       <c r="AB21" s="67" t="s">
-        <v>455</v>
+        <v>458</v>
       </c>
       <c r="AC21" s="67"/>
       <c r="AD21" s="67"/>
@@ -14173,14 +14226,14 @@
       <c r="AH21" s="67"/>
       <c r="AI21" s="67"/>
       <c r="AJ21" s="67" t="s">
-        <v>456</v>
+        <v>459</v>
       </c>
       <c r="AK21" s="67" t="s">
-        <v>457</v>
+        <v>460</v>
       </c>
       <c r="AL21" s="67"/>
       <c r="AM21" s="67" t="s">
-        <v>458</v>
+        <v>461</v>
       </c>
       <c r="AN21" s="67" t="s">
         <v>222</v>
@@ -14202,21 +14255,21 @@
       <c r="I22" s="67"/>
       <c r="J22" s="67"/>
       <c r="K22" s="67" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="L22" s="67" t="s">
-        <v>459</v>
+        <v>462</v>
       </c>
       <c r="M22" s="67"/>
       <c r="N22" s="67"/>
       <c r="O22" s="68"/>
       <c r="P22" s="67"/>
       <c r="Q22" s="67" t="s">
-        <v>460</v>
+        <v>463</v>
       </c>
       <c r="R22" s="67"/>
       <c r="S22" s="67" t="s">
-        <v>461</v>
+        <v>464</v>
       </c>
       <c r="T22" s="67"/>
       <c r="U22" s="67"/>
@@ -14237,17 +14290,17 @@
       <c r="AH22" s="67"/>
       <c r="AI22" s="67"/>
       <c r="AJ22" s="67" t="s">
-        <v>462</v>
+        <v>465</v>
       </c>
       <c r="AK22" s="67" t="s">
-        <v>463</v>
+        <v>466</v>
       </c>
       <c r="AL22" s="67"/>
       <c r="AM22" s="67" t="s">
-        <v>464</v>
+        <v>467</v>
       </c>
       <c r="AN22" s="67" t="s">
-        <v>465</v>
+        <v>468</v>
       </c>
       <c r="AO22" s="67"/>
       <c r="AP22" s="67"/>
@@ -14266,21 +14319,21 @@
       <c r="I23" s="67"/>
       <c r="J23" s="67"/>
       <c r="K23" s="67" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="L23" s="67" t="s">
-        <v>466</v>
+        <v>469</v>
       </c>
       <c r="M23" s="67"/>
       <c r="N23" s="67"/>
       <c r="O23" s="68"/>
       <c r="P23" s="67"/>
       <c r="Q23" s="67" t="s">
-        <v>467</v>
+        <v>470</v>
       </c>
       <c r="R23" s="67"/>
       <c r="S23" s="67" t="s">
-        <v>468</v>
+        <v>471</v>
       </c>
       <c r="T23" s="70"/>
       <c r="U23" s="67"/>
@@ -14291,7 +14344,7 @@
       <c r="Z23" s="67"/>
       <c r="AA23" s="67"/>
       <c r="AB23" s="67" t="s">
-        <v>469</v>
+        <v>472</v>
       </c>
       <c r="AC23" s="67"/>
       <c r="AD23" s="67"/>
@@ -14301,17 +14354,17 @@
       <c r="AH23" s="67"/>
       <c r="AI23" s="67"/>
       <c r="AJ23" s="67" t="s">
-        <v>470</v>
+        <v>473</v>
       </c>
       <c r="AK23" s="67" t="s">
-        <v>471</v>
+        <v>474</v>
       </c>
       <c r="AL23" s="67"/>
       <c r="AM23" s="67" t="s">
-        <v>472</v>
+        <v>475</v>
       </c>
       <c r="AN23" s="67" t="s">
-        <v>473</v>
+        <v>476</v>
       </c>
       <c r="AO23" s="67"/>
       <c r="AP23" s="67"/>
@@ -14330,21 +14383,21 @@
       <c r="I24" s="67"/>
       <c r="J24" s="67"/>
       <c r="K24" s="67" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="L24" s="67" t="s">
-        <v>474</v>
+        <v>477</v>
       </c>
       <c r="M24" s="67"/>
       <c r="N24" s="67"/>
       <c r="O24" s="68"/>
       <c r="P24" s="67"/>
       <c r="Q24" s="67" t="s">
-        <v>475</v>
+        <v>478</v>
       </c>
       <c r="R24" s="67"/>
       <c r="S24" s="67" t="s">
-        <v>476</v>
+        <v>479</v>
       </c>
       <c r="T24" s="70"/>
       <c r="U24" s="67"/>
@@ -14355,7 +14408,7 @@
       <c r="Z24" s="67"/>
       <c r="AA24" s="67"/>
       <c r="AB24" s="67" t="s">
-        <v>477</v>
+        <v>480</v>
       </c>
       <c r="AC24" s="67"/>
       <c r="AD24" s="67"/>
@@ -14365,17 +14418,17 @@
       <c r="AH24" s="67"/>
       <c r="AI24" s="67"/>
       <c r="AJ24" s="67" t="s">
-        <v>478</v>
+        <v>481</v>
       </c>
       <c r="AK24" s="67" t="s">
-        <v>479</v>
+        <v>482</v>
       </c>
       <c r="AL24" s="67"/>
       <c r="AM24" s="67" t="s">
-        <v>480</v>
+        <v>483</v>
       </c>
       <c r="AN24" s="67" t="s">
-        <v>481</v>
+        <v>484</v>
       </c>
       <c r="AO24" s="67"/>
       <c r="AP24" s="67"/>
@@ -14394,21 +14447,21 @@
       <c r="I25" s="67"/>
       <c r="J25" s="67"/>
       <c r="K25" s="67" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="L25" s="67" t="s">
-        <v>482</v>
+        <v>485</v>
       </c>
       <c r="M25" s="67"/>
       <c r="N25" s="67"/>
       <c r="O25" s="68"/>
       <c r="P25" s="67"/>
       <c r="Q25" s="67" t="s">
-        <v>483</v>
+        <v>486</v>
       </c>
       <c r="R25" s="67"/>
       <c r="S25" s="67" t="s">
-        <v>484</v>
+        <v>487</v>
       </c>
       <c r="T25" s="70"/>
       <c r="U25" s="67"/>
@@ -14419,7 +14472,7 @@
       <c r="Z25" s="67"/>
       <c r="AA25" s="67"/>
       <c r="AB25" s="67" t="s">
-        <v>485</v>
+        <v>488</v>
       </c>
       <c r="AC25" s="67"/>
       <c r="AD25" s="67"/>
@@ -14429,14 +14482,14 @@
       <c r="AH25" s="67"/>
       <c r="AI25" s="67"/>
       <c r="AJ25" s="67" t="s">
-        <v>486</v>
+        <v>489</v>
       </c>
       <c r="AK25" s="67" t="s">
-        <v>487</v>
+        <v>490</v>
       </c>
       <c r="AL25" s="67"/>
       <c r="AM25" s="67" t="s">
-        <v>488</v>
+        <v>491</v>
       </c>
       <c r="AN25" s="67"/>
       <c r="AO25" s="67"/>
@@ -14456,21 +14509,21 @@
       <c r="I26" s="67"/>
       <c r="J26" s="67"/>
       <c r="K26" s="67" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="L26" s="67" t="s">
-        <v>489</v>
+        <v>492</v>
       </c>
       <c r="M26" s="67"/>
       <c r="N26" s="67"/>
       <c r="O26" s="68"/>
       <c r="P26" s="67"/>
       <c r="Q26" s="67" t="s">
-        <v>490</v>
+        <v>493</v>
       </c>
       <c r="R26" s="67"/>
       <c r="S26" s="67" t="s">
-        <v>491</v>
+        <v>494</v>
       </c>
       <c r="T26" s="70"/>
       <c r="U26" s="67"/>
@@ -14481,7 +14534,7 @@
       <c r="Z26" s="67"/>
       <c r="AA26" s="67"/>
       <c r="AB26" s="67" t="s">
-        <v>492</v>
+        <v>495</v>
       </c>
       <c r="AC26" s="67"/>
       <c r="AD26" s="67"/>
@@ -14491,14 +14544,14 @@
       <c r="AH26" s="67"/>
       <c r="AI26" s="67"/>
       <c r="AJ26" s="67" t="s">
-        <v>493</v>
+        <v>496</v>
       </c>
       <c r="AK26" s="67" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="AL26" s="67"/>
       <c r="AM26" s="67" t="s">
-        <v>495</v>
+        <v>498</v>
       </c>
       <c r="AN26" s="67"/>
       <c r="AO26" s="67"/>
@@ -14518,21 +14571,21 @@
       <c r="I27" s="67"/>
       <c r="J27" s="67"/>
       <c r="K27" s="67" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="L27" s="67" t="s">
-        <v>496</v>
+        <v>499</v>
       </c>
       <c r="M27" s="67"/>
       <c r="N27" s="67"/>
       <c r="O27" s="68"/>
       <c r="P27" s="67"/>
       <c r="Q27" s="67" t="s">
-        <v>497</v>
+        <v>500</v>
       </c>
       <c r="R27" s="67"/>
       <c r="S27" s="67" t="s">
-        <v>498</v>
+        <v>501</v>
       </c>
       <c r="T27" s="67"/>
       <c r="U27" s="67"/>
@@ -14543,7 +14596,7 @@
       <c r="Z27" s="67"/>
       <c r="AA27" s="67"/>
       <c r="AB27" s="67" t="s">
-        <v>499</v>
+        <v>502</v>
       </c>
       <c r="AC27" s="67"/>
       <c r="AD27" s="67"/>
@@ -14553,14 +14606,14 @@
       <c r="AH27" s="67"/>
       <c r="AI27" s="67"/>
       <c r="AJ27" s="67" t="s">
-        <v>500</v>
+        <v>503</v>
       </c>
       <c r="AK27" s="67" t="s">
-        <v>501</v>
+        <v>504</v>
       </c>
       <c r="AL27" s="67"/>
       <c r="AM27" s="67" t="s">
-        <v>502</v>
+        <v>505</v>
       </c>
       <c r="AN27" s="67"/>
       <c r="AO27" s="67"/>
@@ -14580,21 +14633,21 @@
       <c r="I28" s="67"/>
       <c r="J28" s="67"/>
       <c r="K28" s="67" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="L28" s="67" t="s">
-        <v>503</v>
+        <v>506</v>
       </c>
       <c r="M28" s="67"/>
       <c r="N28" s="67"/>
       <c r="O28" s="68"/>
       <c r="P28" s="67"/>
       <c r="Q28" s="67" t="s">
-        <v>504</v>
+        <v>507</v>
       </c>
       <c r="R28" s="67"/>
       <c r="S28" s="67" t="s">
-        <v>505</v>
+        <v>508</v>
       </c>
       <c r="T28" s="70"/>
       <c r="U28" s="67"/>
@@ -14605,7 +14658,7 @@
       <c r="Z28" s="67"/>
       <c r="AA28" s="67"/>
       <c r="AB28" s="67" t="s">
-        <v>506</v>
+        <v>509</v>
       </c>
       <c r="AC28" s="67"/>
       <c r="AD28" s="67"/>
@@ -14615,14 +14668,14 @@
       <c r="AH28" s="67"/>
       <c r="AI28" s="67"/>
       <c r="AJ28" s="67" t="s">
-        <v>507</v>
+        <v>510</v>
       </c>
       <c r="AK28" s="67" t="s">
-        <v>508</v>
+        <v>511</v>
       </c>
       <c r="AL28" s="67"/>
       <c r="AM28" s="67" t="s">
-        <v>509</v>
+        <v>512</v>
       </c>
       <c r="AN28" s="67"/>
       <c r="AO28" s="67"/>
@@ -14642,21 +14695,21 @@
       <c r="I29" s="67"/>
       <c r="J29" s="67"/>
       <c r="K29" s="67" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="L29" s="67" t="s">
-        <v>510</v>
+        <v>513</v>
       </c>
       <c r="M29" s="67"/>
       <c r="N29" s="67"/>
       <c r="O29" s="68"/>
       <c r="P29" s="67"/>
       <c r="Q29" s="67" t="s">
-        <v>511</v>
+        <v>514</v>
       </c>
       <c r="R29" s="67"/>
       <c r="S29" s="67" t="s">
-        <v>512</v>
+        <v>515</v>
       </c>
       <c r="T29" s="70"/>
       <c r="U29" s="67"/>
@@ -14677,14 +14730,14 @@
       <c r="AH29" s="67"/>
       <c r="AI29" s="67"/>
       <c r="AJ29" s="67" t="s">
-        <v>513</v>
+        <v>516</v>
       </c>
       <c r="AK29" s="67" t="s">
-        <v>514</v>
+        <v>517</v>
       </c>
       <c r="AL29" s="67"/>
       <c r="AM29" s="67" t="s">
-        <v>515</v>
+        <v>518</v>
       </c>
       <c r="AN29" s="67"/>
       <c r="AO29" s="67"/>
@@ -14704,21 +14757,21 @@
       <c r="I30" s="67"/>
       <c r="J30" s="67"/>
       <c r="K30" s="67" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="L30" s="67" t="s">
-        <v>516</v>
+        <v>519</v>
       </c>
       <c r="M30" s="67"/>
       <c r="N30" s="67"/>
       <c r="O30" s="68"/>
       <c r="P30" s="67"/>
       <c r="Q30" s="67" t="s">
-        <v>517</v>
+        <v>520</v>
       </c>
       <c r="R30" s="67"/>
       <c r="S30" s="67" t="s">
-        <v>518</v>
+        <v>521</v>
       </c>
       <c r="T30" s="67"/>
       <c r="U30" s="67"/>
@@ -14737,14 +14790,14 @@
       <c r="AH30" s="67"/>
       <c r="AI30" s="67"/>
       <c r="AJ30" s="67" t="s">
-        <v>519</v>
+        <v>522</v>
       </c>
       <c r="AK30" s="67" t="s">
-        <v>520</v>
+        <v>523</v>
       </c>
       <c r="AL30" s="67"/>
       <c r="AM30" s="67" t="s">
-        <v>521</v>
+        <v>524</v>
       </c>
       <c r="AN30" s="67"/>
       <c r="AO30" s="67"/>
@@ -14764,21 +14817,21 @@
       <c r="I31" s="67"/>
       <c r="J31" s="67"/>
       <c r="K31" s="67" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="L31" s="67" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="M31" s="67"/>
       <c r="N31" s="67"/>
       <c r="O31" s="68"/>
       <c r="P31" s="67"/>
       <c r="Q31" s="67" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
       <c r="R31" s="67"/>
       <c r="S31" s="67" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="T31" s="67"/>
       <c r="U31" s="67"/>
@@ -14797,10 +14850,10 @@
       <c r="AH31" s="67"/>
       <c r="AI31" s="67"/>
       <c r="AJ31" s="67" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="AK31" s="67" t="s">
-        <v>526</v>
+        <v>529</v>
       </c>
       <c r="AL31" s="67"/>
       <c r="AM31" s="67" t="s">
@@ -14824,21 +14877,21 @@
       <c r="I32" s="67"/>
       <c r="J32" s="67"/>
       <c r="K32" s="67" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="L32" s="67" t="s">
-        <v>527</v>
+        <v>530</v>
       </c>
       <c r="M32" s="67"/>
       <c r="N32" s="67"/>
       <c r="O32" s="68"/>
       <c r="P32" s="67"/>
       <c r="Q32" s="67" t="s">
-        <v>528</v>
+        <v>531</v>
       </c>
       <c r="R32" s="67"/>
       <c r="S32" s="67" t="s">
-        <v>529</v>
+        <v>532</v>
       </c>
       <c r="T32" s="67"/>
       <c r="U32" s="67"/>
@@ -14857,10 +14910,10 @@
       <c r="AH32" s="67"/>
       <c r="AI32" s="67"/>
       <c r="AJ32" s="67" t="s">
-        <v>530</v>
+        <v>533</v>
       </c>
       <c r="AK32" s="67" t="s">
-        <v>531</v>
+        <v>534</v>
       </c>
       <c r="AL32" s="67"/>
       <c r="AM32" s="67"/>
@@ -14882,21 +14935,21 @@
       <c r="I33" s="67"/>
       <c r="J33" s="67"/>
       <c r="K33" s="67" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="L33" s="67" t="s">
-        <v>532</v>
+        <v>535</v>
       </c>
       <c r="M33" s="67"/>
       <c r="N33" s="67"/>
       <c r="O33" s="68"/>
       <c r="P33" s="67"/>
       <c r="Q33" s="67" t="s">
-        <v>533</v>
+        <v>536</v>
       </c>
       <c r="R33" s="67"/>
       <c r="S33" s="67" t="s">
-        <v>534</v>
+        <v>537</v>
       </c>
       <c r="T33" s="67"/>
       <c r="U33" s="67"/>
@@ -14915,10 +14968,10 @@
       <c r="AH33" s="67"/>
       <c r="AI33" s="67"/>
       <c r="AJ33" s="67" t="s">
-        <v>535</v>
+        <v>538</v>
       </c>
       <c r="AK33" s="67" t="s">
-        <v>536</v>
+        <v>539</v>
       </c>
       <c r="AL33" s="67"/>
       <c r="AM33" s="67"/>
@@ -14940,17 +14993,17 @@
       <c r="I34" s="67"/>
       <c r="J34" s="67"/>
       <c r="K34" s="67" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="L34" s="67" t="s">
-        <v>537</v>
+        <v>540</v>
       </c>
       <c r="M34" s="67"/>
       <c r="N34" s="67"/>
       <c r="O34" s="68"/>
       <c r="P34" s="67"/>
       <c r="Q34" s="67" t="s">
-        <v>538</v>
+        <v>541</v>
       </c>
       <c r="R34" s="67"/>
       <c r="S34" s="67" t="s">
@@ -14976,7 +15029,7 @@
         <v>259</v>
       </c>
       <c r="AK34" s="67" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="AL34" s="67"/>
       <c r="AM34" s="67"/>
@@ -14998,21 +15051,21 @@
       <c r="I35" s="67"/>
       <c r="J35" s="67"/>
       <c r="K35" s="67" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="L35" s="67" t="s">
-        <v>540</v>
+        <v>543</v>
       </c>
       <c r="M35" s="67"/>
       <c r="N35" s="67"/>
       <c r="O35" s="68"/>
       <c r="P35" s="67"/>
       <c r="Q35" s="67" t="s">
-        <v>541</v>
+        <v>544</v>
       </c>
       <c r="R35" s="67"/>
       <c r="S35" s="67" t="s">
-        <v>542</v>
+        <v>545</v>
       </c>
       <c r="T35" s="67"/>
       <c r="U35" s="67"/>
@@ -15031,10 +15084,10 @@
       <c r="AH35" s="67"/>
       <c r="AI35" s="67"/>
       <c r="AJ35" s="67" t="s">
-        <v>543</v>
+        <v>546</v>
       </c>
       <c r="AK35" s="67" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="AL35" s="67"/>
       <c r="AM35" s="67"/>
@@ -15056,21 +15109,21 @@
       <c r="I36" s="67"/>
       <c r="J36" s="67"/>
       <c r="K36" s="67" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="L36" s="67" t="s">
-        <v>545</v>
+        <v>548</v>
       </c>
       <c r="M36" s="67"/>
       <c r="N36" s="67"/>
       <c r="O36" s="68"/>
       <c r="P36" s="67"/>
       <c r="Q36" s="67" t="s">
-        <v>546</v>
+        <v>549</v>
       </c>
       <c r="R36" s="67"/>
       <c r="S36" s="67" t="s">
-        <v>547</v>
+        <v>550</v>
       </c>
       <c r="T36" s="67"/>
       <c r="U36" s="67"/>
@@ -15089,10 +15142,10 @@
       <c r="AH36" s="67"/>
       <c r="AI36" s="67"/>
       <c r="AJ36" s="67" t="s">
-        <v>548</v>
+        <v>551</v>
       </c>
       <c r="AK36" s="67" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="AL36" s="67"/>
       <c r="AM36" s="67"/>
@@ -15114,21 +15167,21 @@
       <c r="I37" s="67"/>
       <c r="J37" s="67"/>
       <c r="K37" s="67" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="L37" s="67" t="s">
-        <v>550</v>
+        <v>553</v>
       </c>
       <c r="M37" s="67"/>
       <c r="N37" s="67"/>
       <c r="O37" s="68"/>
       <c r="P37" s="67"/>
       <c r="Q37" s="67" t="s">
-        <v>551</v>
+        <v>554</v>
       </c>
       <c r="R37" s="67"/>
       <c r="S37" s="67" t="s">
-        <v>552</v>
+        <v>555</v>
       </c>
       <c r="T37" s="67"/>
       <c r="U37" s="67"/>
@@ -15147,10 +15200,10 @@
       <c r="AH37" s="67"/>
       <c r="AI37" s="67"/>
       <c r="AJ37" s="67" t="s">
-        <v>553</v>
+        <v>556</v>
       </c>
       <c r="AK37" s="67" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="AL37" s="67"/>
       <c r="AM37" s="67"/>
@@ -15172,21 +15225,21 @@
       <c r="I38" s="67"/>
       <c r="J38" s="67"/>
       <c r="K38" s="67" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="L38" s="67" t="s">
-        <v>555</v>
+        <v>558</v>
       </c>
       <c r="M38" s="67"/>
       <c r="N38" s="67"/>
       <c r="O38" s="68"/>
       <c r="P38" s="67"/>
       <c r="Q38" s="67" t="s">
-        <v>556</v>
+        <v>559</v>
       </c>
       <c r="R38" s="67"/>
       <c r="S38" s="67" t="s">
-        <v>557</v>
+        <v>560</v>
       </c>
       <c r="T38" s="67"/>
       <c r="U38" s="67"/>
@@ -15205,10 +15258,10 @@
       <c r="AH38" s="67"/>
       <c r="AI38" s="67"/>
       <c r="AJ38" s="67" t="s">
-        <v>558</v>
+        <v>561</v>
       </c>
       <c r="AK38" s="67" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="AL38" s="67"/>
       <c r="AM38" s="67"/>
@@ -15230,21 +15283,21 @@
       <c r="I39" s="67"/>
       <c r="J39" s="67"/>
       <c r="K39" s="67" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="L39" s="67" t="s">
-        <v>559</v>
+        <v>562</v>
       </c>
       <c r="M39" s="67"/>
       <c r="N39" s="67"/>
       <c r="O39" s="68"/>
       <c r="P39" s="67"/>
       <c r="Q39" s="67" t="s">
-        <v>560</v>
+        <v>563</v>
       </c>
       <c r="R39" s="67"/>
       <c r="S39" s="67" t="s">
-        <v>561</v>
+        <v>564</v>
       </c>
       <c r="T39" s="67"/>
       <c r="U39" s="67"/>
@@ -15263,10 +15316,10 @@
       <c r="AH39" s="67"/>
       <c r="AI39" s="67"/>
       <c r="AJ39" s="67" t="s">
-        <v>562</v>
+        <v>565</v>
       </c>
       <c r="AK39" s="67" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="AL39" s="67"/>
       <c r="AM39" s="67"/>
@@ -15288,21 +15341,21 @@
       <c r="I40" s="67"/>
       <c r="J40" s="67"/>
       <c r="K40" s="67" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="L40" s="67" t="s">
-        <v>563</v>
+        <v>566</v>
       </c>
       <c r="M40" s="67"/>
       <c r="N40" s="67"/>
       <c r="O40" s="68"/>
       <c r="P40" s="67"/>
       <c r="Q40" s="67" t="s">
-        <v>564</v>
+        <v>567</v>
       </c>
       <c r="R40" s="67"/>
       <c r="S40" s="67" t="s">
-        <v>565</v>
+        <v>568</v>
       </c>
       <c r="T40" s="67"/>
       <c r="U40" s="67"/>
@@ -15321,10 +15374,10 @@
       <c r="AH40" s="67"/>
       <c r="AI40" s="67"/>
       <c r="AJ40" s="67" t="s">
-        <v>566</v>
+        <v>569</v>
       </c>
       <c r="AK40" s="67" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="AL40" s="67"/>
       <c r="AM40" s="67"/>
@@ -15346,21 +15399,21 @@
       <c r="I41" s="67"/>
       <c r="J41" s="67"/>
       <c r="K41" s="67" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="L41" s="67" t="s">
-        <v>567</v>
+        <v>570</v>
       </c>
       <c r="M41" s="67"/>
       <c r="N41" s="67"/>
       <c r="O41" s="68"/>
       <c r="P41" s="67"/>
       <c r="Q41" s="67" t="s">
-        <v>568</v>
+        <v>571</v>
       </c>
       <c r="R41" s="67"/>
       <c r="S41" s="67" t="s">
-        <v>569</v>
+        <v>572</v>
       </c>
       <c r="T41" s="67"/>
       <c r="U41" s="67"/>
@@ -15379,10 +15432,10 @@
       <c r="AH41" s="67"/>
       <c r="AI41" s="67"/>
       <c r="AJ41" s="67" t="s">
-        <v>570</v>
+        <v>573</v>
       </c>
       <c r="AK41" s="67" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="AL41" s="67"/>
       <c r="AM41" s="67"/>
@@ -15404,21 +15457,21 @@
       <c r="I42" s="67"/>
       <c r="J42" s="67"/>
       <c r="K42" s="67" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="L42" s="67" t="s">
-        <v>571</v>
+        <v>574</v>
       </c>
       <c r="M42" s="67"/>
       <c r="N42" s="67"/>
       <c r="O42" s="68"/>
       <c r="P42" s="67"/>
       <c r="Q42" s="67" t="s">
-        <v>572</v>
+        <v>575</v>
       </c>
       <c r="R42" s="67"/>
       <c r="S42" s="67" t="s">
-        <v>573</v>
+        <v>576</v>
       </c>
       <c r="T42" s="67"/>
       <c r="U42" s="67"/>
@@ -15437,10 +15490,10 @@
       <c r="AH42" s="67"/>
       <c r="AI42" s="67"/>
       <c r="AJ42" s="67" t="s">
-        <v>574</v>
+        <v>577</v>
       </c>
       <c r="AK42" s="67" t="s">
-        <v>539</v>
+        <v>542</v>
       </c>
       <c r="AL42" s="67"/>
       <c r="AM42" s="67"/>
@@ -15462,21 +15515,21 @@
       <c r="I43" s="67"/>
       <c r="J43" s="67"/>
       <c r="K43" s="67" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="L43" s="67" t="s">
-        <v>575</v>
+        <v>578</v>
       </c>
       <c r="M43" s="67"/>
       <c r="N43" s="67"/>
       <c r="O43" s="68"/>
       <c r="P43" s="67"/>
       <c r="Q43" s="67" t="s">
-        <v>576</v>
+        <v>579</v>
       </c>
       <c r="R43" s="67"/>
       <c r="S43" s="67" t="s">
-        <v>577</v>
+        <v>580</v>
       </c>
       <c r="T43" s="67"/>
       <c r="U43" s="67"/>
@@ -15495,10 +15548,10 @@
       <c r="AH43" s="67"/>
       <c r="AI43" s="67"/>
       <c r="AJ43" s="67" t="s">
-        <v>578</v>
+        <v>581</v>
       </c>
       <c r="AK43" s="67" t="s">
-        <v>544</v>
+        <v>547</v>
       </c>
       <c r="AL43" s="67"/>
       <c r="AM43" s="67"/>
@@ -15520,21 +15573,21 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="L44" s="67" t="s">
-        <v>579</v>
+        <v>582</v>
       </c>
       <c r="M44" s="67"/>
       <c r="N44" s="67"/>
       <c r="O44" s="68"/>
       <c r="P44" s="67"/>
       <c r="Q44" s="67" t="s">
-        <v>580</v>
+        <v>583</v>
       </c>
       <c r="R44" s="67"/>
       <c r="S44" s="67" t="s">
-        <v>581</v>
+        <v>584</v>
       </c>
       <c r="T44" s="67"/>
       <c r="U44" s="67"/>
@@ -15553,10 +15606,10 @@
       <c r="AH44" s="67"/>
       <c r="AI44" s="67"/>
       <c r="AJ44" s="67" t="s">
-        <v>582</v>
+        <v>585</v>
       </c>
       <c r="AK44" s="67" t="s">
-        <v>549</v>
+        <v>552</v>
       </c>
       <c r="AL44" s="67"/>
       <c r="AM44" s="67"/>
@@ -15578,21 +15631,21 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="L45" s="67" t="s">
-        <v>583</v>
+        <v>586</v>
       </c>
       <c r="M45" s="67"/>
       <c r="N45" s="67"/>
       <c r="O45" s="68"/>
       <c r="P45" s="67"/>
       <c r="Q45" s="67" t="s">
-        <v>584</v>
+        <v>587</v>
       </c>
       <c r="R45" s="67"/>
       <c r="S45" s="67" t="s">
-        <v>585</v>
+        <v>588</v>
       </c>
       <c r="T45" s="67"/>
       <c r="U45" s="67"/>
@@ -15611,10 +15664,10 @@
       <c r="AH45" s="67"/>
       <c r="AI45" s="67"/>
       <c r="AJ45" s="67" t="s">
-        <v>586</v>
+        <v>589</v>
       </c>
       <c r="AK45" s="67" t="s">
-        <v>554</v>
+        <v>557</v>
       </c>
       <c r="AL45" s="67"/>
       <c r="AM45" s="67"/>
@@ -15636,21 +15689,21 @@
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="L46" s="67" t="s">
-        <v>587</v>
+        <v>590</v>
       </c>
       <c r="M46" s="67"/>
       <c r="N46" s="67"/>
       <c r="O46" s="68"/>
       <c r="P46" s="67"/>
       <c r="Q46" s="67" t="s">
-        <v>588</v>
+        <v>591</v>
       </c>
       <c r="R46" s="67"/>
       <c r="S46" s="67" t="s">
-        <v>589</v>
+        <v>592</v>
       </c>
       <c r="T46" s="67"/>
       <c r="U46" s="67"/>
@@ -15669,10 +15722,10 @@
       <c r="AH46" s="67"/>
       <c r="AI46" s="67"/>
       <c r="AJ46" s="67" t="s">
-        <v>590</v>
+        <v>593</v>
       </c>
       <c r="AK46" s="67" t="s">
-        <v>591</v>
+        <v>594</v>
       </c>
       <c r="AL46" s="67"/>
       <c r="AM46" s="67"/>
@@ -15694,21 +15747,21 @@
       <c r="I47" s="67"/>
       <c r="J47" s="67"/>
       <c r="K47" s="67" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="L47" s="67" t="s">
-        <v>592</v>
+        <v>595</v>
       </c>
       <c r="M47" s="67"/>
       <c r="N47" s="67"/>
       <c r="O47" s="68"/>
       <c r="P47" s="67"/>
       <c r="Q47" s="67" t="s">
-        <v>593</v>
+        <v>596</v>
       </c>
       <c r="R47" s="67"/>
       <c r="S47" s="67" t="s">
-        <v>594</v>
+        <v>597</v>
       </c>
       <c r="T47" s="67"/>
       <c r="U47" s="67"/>
@@ -15727,10 +15780,10 @@
       <c r="AH47" s="67"/>
       <c r="AI47" s="67"/>
       <c r="AJ47" s="67" t="s">
-        <v>595</v>
+        <v>598</v>
       </c>
       <c r="AK47" s="67" t="s">
-        <v>596</v>
+        <v>599</v>
       </c>
       <c r="AL47" s="67"/>
       <c r="AM47" s="67"/>
@@ -15752,21 +15805,21 @@
       <c r="I48" s="67"/>
       <c r="J48" s="67"/>
       <c r="K48" s="67" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="L48" s="67" t="s">
-        <v>597</v>
+        <v>600</v>
       </c>
       <c r="M48" s="67"/>
       <c r="N48" s="67"/>
       <c r="O48" s="68"/>
       <c r="P48" s="67"/>
       <c r="Q48" s="67" t="s">
-        <v>598</v>
+        <v>601</v>
       </c>
       <c r="R48" s="67"/>
       <c r="S48" s="67" t="s">
-        <v>599</v>
+        <v>602</v>
       </c>
       <c r="T48" s="67"/>
       <c r="U48" s="67"/>
@@ -15785,10 +15838,10 @@
       <c r="AH48" s="67"/>
       <c r="AI48" s="67"/>
       <c r="AJ48" s="67" t="s">
-        <v>600</v>
+        <v>603</v>
       </c>
       <c r="AK48" s="67" t="s">
-        <v>601</v>
+        <v>604</v>
       </c>
       <c r="AL48" s="67"/>
       <c r="AM48" s="67"/>
@@ -15810,21 +15863,21 @@
       <c r="I49" s="67"/>
       <c r="J49" s="67"/>
       <c r="K49" s="67" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="L49" s="67" t="s">
-        <v>602</v>
+        <v>605</v>
       </c>
       <c r="M49" s="67"/>
       <c r="N49" s="67"/>
       <c r="O49" s="68"/>
       <c r="P49" s="67"/>
       <c r="Q49" s="67" t="s">
-        <v>603</v>
+        <v>606</v>
       </c>
       <c r="R49" s="67"/>
       <c r="S49" s="67" t="s">
-        <v>604</v>
+        <v>607</v>
       </c>
       <c r="T49" s="67"/>
       <c r="U49" s="67"/>
@@ -15843,10 +15896,10 @@
       <c r="AH49" s="67"/>
       <c r="AI49" s="67"/>
       <c r="AJ49" s="67" t="s">
-        <v>605</v>
+        <v>608</v>
       </c>
       <c r="AK49" s="67" t="s">
-        <v>606</v>
+        <v>609</v>
       </c>
       <c r="AL49" s="67"/>
       <c r="AM49" s="67"/>
@@ -15868,21 +15921,21 @@
       <c r="I50" s="67"/>
       <c r="J50" s="67"/>
       <c r="K50" s="67" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="L50" s="67" t="s">
-        <v>607</v>
+        <v>610</v>
       </c>
       <c r="M50" s="67"/>
       <c r="N50" s="67"/>
       <c r="O50" s="68"/>
       <c r="P50" s="67"/>
       <c r="Q50" s="67" t="s">
-        <v>608</v>
+        <v>611</v>
       </c>
       <c r="R50" s="67"/>
       <c r="S50" s="67" t="s">
-        <v>609</v>
+        <v>612</v>
       </c>
       <c r="T50" s="67"/>
       <c r="U50" s="67"/>
@@ -15901,10 +15954,10 @@
       <c r="AH50" s="67"/>
       <c r="AI50" s="67"/>
       <c r="AJ50" s="67" t="s">
-        <v>610</v>
+        <v>613</v>
       </c>
       <c r="AK50" s="67" t="s">
-        <v>611</v>
+        <v>614</v>
       </c>
       <c r="AL50" s="67"/>
       <c r="AM50" s="67"/>
@@ -15926,17 +15979,17 @@
       <c r="I51" s="67"/>
       <c r="J51" s="67"/>
       <c r="K51" s="67" t="s">
-        <v>612</v>
+        <v>615</v>
       </c>
       <c r="L51" s="67" t="s">
-        <v>613</v>
+        <v>616</v>
       </c>
       <c r="M51" s="67"/>
       <c r="N51" s="67"/>
       <c r="O51" s="68"/>
       <c r="P51" s="67"/>
       <c r="Q51" s="67" t="s">
-        <v>614</v>
+        <v>617</v>
       </c>
       <c r="R51" s="67"/>
       <c r="S51" s="67" t="s">
@@ -15959,10 +16012,10 @@
       <c r="AH51" s="67"/>
       <c r="AI51" s="67"/>
       <c r="AJ51" s="67" t="s">
-        <v>615</v>
+        <v>618</v>
       </c>
       <c r="AK51" s="67" t="s">
-        <v>616</v>
+        <v>619</v>
       </c>
       <c r="AL51" s="67"/>
       <c r="AM51" s="67"/>
@@ -15984,17 +16037,17 @@
       <c r="I52" s="67"/>
       <c r="J52" s="67"/>
       <c r="K52" s="67" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="L52" s="67" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="M52" s="67"/>
       <c r="N52" s="67"/>
       <c r="O52" s="68"/>
       <c r="P52" s="67"/>
       <c r="Q52" s="67" t="s">
-        <v>619</v>
+        <v>622</v>
       </c>
       <c r="R52" s="67"/>
       <c r="S52" s="67"/>
@@ -16015,10 +16068,10 @@
       <c r="AH52" s="67"/>
       <c r="AI52" s="67"/>
       <c r="AJ52" s="67" t="s">
-        <v>620</v>
+        <v>623</v>
       </c>
       <c r="AK52" s="67" t="s">
-        <v>621</v>
+        <v>624</v>
       </c>
       <c r="AL52" s="67"/>
       <c r="AM52" s="67"/>
@@ -16040,10 +16093,10 @@
       <c r="I53" s="67"/>
       <c r="J53" s="67"/>
       <c r="K53" s="67" t="s">
-        <v>622</v>
+        <v>625</v>
       </c>
       <c r="L53" s="67" t="s">
-        <v>617</v>
+        <v>620</v>
       </c>
       <c r="M53" s="67"/>
       <c r="N53" s="67"/>
@@ -16071,10 +16124,10 @@
       <c r="AH53" s="67"/>
       <c r="AI53" s="67"/>
       <c r="AJ53" s="67" t="s">
-        <v>623</v>
+        <v>626</v>
       </c>
       <c r="AK53" s="67" t="s">
-        <v>624</v>
+        <v>627</v>
       </c>
       <c r="AL53" s="67"/>
       <c r="AM53" s="67"/>
@@ -16096,17 +16149,17 @@
       <c r="I54" s="67"/>
       <c r="J54" s="67"/>
       <c r="K54" s="67" t="s">
+        <v>628</v>
+      </c>
+      <c r="L54" s="67" t="s">
         <v>625</v>
-      </c>
-      <c r="L54" s="67" t="s">
-        <v>622</v>
       </c>
       <c r="M54" s="67"/>
       <c r="N54" s="67"/>
       <c r="O54" s="68"/>
       <c r="P54" s="67"/>
       <c r="Q54" s="67" t="s">
-        <v>626</v>
+        <v>629</v>
       </c>
       <c r="R54" s="67"/>
       <c r="S54" s="67"/>
@@ -16127,10 +16180,10 @@
       <c r="AH54" s="67"/>
       <c r="AI54" s="67"/>
       <c r="AJ54" s="67" t="s">
-        <v>627</v>
+        <v>630</v>
       </c>
       <c r="AK54" s="67" t="s">
-        <v>628</v>
+        <v>631</v>
       </c>
       <c r="AL54" s="67"/>
       <c r="AM54" s="67"/>
@@ -16152,17 +16205,17 @@
       <c r="I55" s="67"/>
       <c r="J55" s="67"/>
       <c r="K55" s="67" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="L55" s="67" t="s">
-        <v>625</v>
+        <v>628</v>
       </c>
       <c r="M55" s="67"/>
       <c r="N55" s="67"/>
       <c r="O55" s="68"/>
       <c r="P55" s="67"/>
       <c r="Q55" s="67" t="s">
-        <v>630</v>
+        <v>633</v>
       </c>
       <c r="R55" s="67"/>
       <c r="S55" s="67"/>
@@ -16183,10 +16236,10 @@
       <c r="AH55" s="67"/>
       <c r="AI55" s="67"/>
       <c r="AJ55" s="67" t="s">
-        <v>631</v>
+        <v>634</v>
       </c>
       <c r="AK55" s="67" t="s">
-        <v>632</v>
+        <v>635</v>
       </c>
       <c r="AL55" s="67"/>
       <c r="AM55" s="67"/>
@@ -16208,17 +16261,17 @@
       <c r="I56" s="67"/>
       <c r="J56" s="67"/>
       <c r="K56" s="67" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="L56" s="67" t="s">
-        <v>629</v>
+        <v>632</v>
       </c>
       <c r="M56" s="67"/>
       <c r="N56" s="67"/>
       <c r="O56" s="68"/>
       <c r="P56" s="67"/>
       <c r="Q56" s="67" t="s">
-        <v>634</v>
+        <v>637</v>
       </c>
       <c r="R56" s="67"/>
       <c r="S56" s="67"/>
@@ -16239,10 +16292,10 @@
       <c r="AH56" s="67"/>
       <c r="AI56" s="67"/>
       <c r="AJ56" s="67" t="s">
-        <v>635</v>
+        <v>638</v>
       </c>
       <c r="AK56" s="67" t="s">
-        <v>636</v>
+        <v>639</v>
       </c>
       <c r="AL56" s="67"/>
       <c r="AM56" s="67"/>
@@ -16264,17 +16317,17 @@
       <c r="I57" s="67"/>
       <c r="J57" s="67"/>
       <c r="K57" s="67" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="L57" s="67" t="s">
-        <v>633</v>
+        <v>636</v>
       </c>
       <c r="M57" s="67"/>
       <c r="N57" s="67"/>
       <c r="O57" s="68"/>
       <c r="P57" s="67"/>
       <c r="Q57" s="67" t="s">
-        <v>638</v>
+        <v>641</v>
       </c>
       <c r="R57" s="67"/>
       <c r="S57" s="67"/>
@@ -16295,10 +16348,10 @@
       <c r="AH57" s="67"/>
       <c r="AI57" s="67"/>
       <c r="AJ57" s="67" t="s">
-        <v>639</v>
+        <v>642</v>
       </c>
       <c r="AK57" s="67" t="s">
-        <v>640</v>
+        <v>643</v>
       </c>
       <c r="AL57" s="67"/>
       <c r="AM57" s="67"/>
@@ -16320,17 +16373,17 @@
       <c r="I58" s="67"/>
       <c r="J58" s="67"/>
       <c r="K58" s="67" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="L58" s="67" t="s">
-        <v>637</v>
+        <v>640</v>
       </c>
       <c r="M58" s="67"/>
       <c r="N58" s="67"/>
       <c r="O58" s="68"/>
       <c r="P58" s="67"/>
       <c r="Q58" s="67" t="s">
-        <v>642</v>
+        <v>645</v>
       </c>
       <c r="R58" s="67"/>
       <c r="S58" s="67"/>
@@ -16351,10 +16404,10 @@
       <c r="AH58" s="67"/>
       <c r="AI58" s="67"/>
       <c r="AJ58" s="67" t="s">
-        <v>643</v>
+        <v>646</v>
       </c>
       <c r="AK58" s="67" t="s">
-        <v>644</v>
+        <v>647</v>
       </c>
       <c r="AL58" s="67"/>
       <c r="AM58" s="67"/>
@@ -16376,10 +16429,10 @@
       <c r="I59" s="67"/>
       <c r="J59" s="67"/>
       <c r="K59" s="67" t="s">
-        <v>645</v>
+        <v>648</v>
       </c>
       <c r="L59" s="67" t="s">
-        <v>641</v>
+        <v>644</v>
       </c>
       <c r="M59" s="67"/>
       <c r="N59" s="67"/>
@@ -16407,10 +16460,10 @@
       <c r="AH59" s="67"/>
       <c r="AI59" s="67"/>
       <c r="AJ59" s="67" t="s">
-        <v>646</v>
+        <v>649</v>
       </c>
       <c r="AK59" s="67" t="s">
-        <v>647</v>
+        <v>650</v>
       </c>
       <c r="AL59" s="67"/>
       <c r="AM59" s="67"/>
@@ -16432,10 +16485,10 @@
       <c r="I60" s="67"/>
       <c r="J60" s="67"/>
       <c r="K60" s="67" t="s">
+        <v>651</v>
+      </c>
+      <c r="L60" s="67" t="s">
         <v>648</v>
-      </c>
-      <c r="L60" s="67" t="s">
-        <v>645</v>
       </c>
       <c r="M60" s="67"/>
       <c r="N60" s="67"/>
@@ -16460,10 +16513,10 @@
       <c r="AH60" s="67"/>
       <c r="AI60" s="67"/>
       <c r="AJ60" s="67" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="AK60" s="67" t="s">
-        <v>650</v>
+        <v>653</v>
       </c>
       <c r="AL60" s="67"/>
       <c r="AM60" s="67"/>
@@ -16485,10 +16538,10 @@
       <c r="I61" s="67"/>
       <c r="J61" s="67"/>
       <c r="K61" s="67" t="s">
+        <v>654</v>
+      </c>
+      <c r="L61" s="67" t="s">
         <v>651</v>
-      </c>
-      <c r="L61" s="67" t="s">
-        <v>648</v>
       </c>
       <c r="M61" s="67"/>
       <c r="N61" s="67"/>
@@ -16513,10 +16566,10 @@
       <c r="AH61" s="67"/>
       <c r="AI61" s="67"/>
       <c r="AJ61" s="67" t="s">
-        <v>652</v>
+        <v>655</v>
       </c>
       <c r="AK61" s="67" t="s">
-        <v>653</v>
+        <v>656</v>
       </c>
       <c r="AL61" s="67"/>
       <c r="AM61" s="67"/>
@@ -16538,10 +16591,10 @@
       <c r="I62" s="67"/>
       <c r="J62" s="67"/>
       <c r="K62" s="67" t="s">
+        <v>657</v>
+      </c>
+      <c r="L62" s="67" t="s">
         <v>654</v>
-      </c>
-      <c r="L62" s="67" t="s">
-        <v>651</v>
       </c>
       <c r="M62" s="67"/>
       <c r="N62" s="67"/>
@@ -16567,10 +16620,10 @@
       <c r="AH62" s="67"/>
       <c r="AI62" s="67"/>
       <c r="AJ62" s="67" t="s">
-        <v>655</v>
+        <v>658</v>
       </c>
       <c r="AK62" s="67" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="AL62" s="67"/>
       <c r="AM62" s="67"/>
@@ -16592,10 +16645,10 @@
       <c r="I63" s="67"/>
       <c r="J63" s="67"/>
       <c r="K63" s="67" t="s">
-        <v>618</v>
+        <v>621</v>
       </c>
       <c r="L63" s="67" t="s">
-        <v>654</v>
+        <v>657</v>
       </c>
       <c r="M63" s="67"/>
       <c r="N63" s="67"/>
@@ -16621,7 +16674,7 @@
       <c r="AH63" s="67"/>
       <c r="AI63" s="67"/>
       <c r="AJ63" s="67" t="s">
-        <v>657</v>
+        <v>660</v>
       </c>
       <c r="AK63" s="67" t="s">
         <v>139</v>
@@ -16646,10 +16699,10 @@
       <c r="I64" s="67"/>
       <c r="J64" s="67"/>
       <c r="K64" s="67" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="L64" s="67" t="s">
-        <v>658</v>
+        <v>661</v>
       </c>
       <c r="M64" s="67"/>
       <c r="N64" s="67"/>
@@ -16675,10 +16728,10 @@
       <c r="AH64" s="67"/>
       <c r="AI64" s="67"/>
       <c r="AJ64" s="67" t="s">
-        <v>659</v>
+        <v>662</v>
       </c>
       <c r="AK64" s="67" t="s">
-        <v>660</v>
+        <v>663</v>
       </c>
       <c r="AL64" s="67"/>
       <c r="AM64" s="67"/>
@@ -16700,10 +16753,10 @@
       <c r="I65" s="67"/>
       <c r="J65" s="67"/>
       <c r="K65" s="67" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="L65" s="67" t="s">
-        <v>661</v>
+        <v>664</v>
       </c>
       <c r="M65" s="67"/>
       <c r="N65" s="67"/>
@@ -16729,10 +16782,10 @@
       <c r="AH65" s="67"/>
       <c r="AI65" s="67"/>
       <c r="AJ65" s="67" t="s">
-        <v>662</v>
+        <v>665</v>
       </c>
       <c r="AK65" s="67" t="s">
-        <v>663</v>
+        <v>666</v>
       </c>
       <c r="AL65" s="67"/>
       <c r="AM65" s="67"/>
@@ -16754,10 +16807,10 @@
       <c r="I66" s="67"/>
       <c r="J66" s="67"/>
       <c r="K66" s="67" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="L66" s="67" t="s">
-        <v>664</v>
+        <v>667</v>
       </c>
       <c r="M66" s="67"/>
       <c r="N66" s="67"/>
@@ -16783,10 +16836,10 @@
       <c r="AH66" s="67"/>
       <c r="AI66" s="67"/>
       <c r="AJ66" s="67" t="s">
-        <v>665</v>
+        <v>668</v>
       </c>
       <c r="AK66" s="67" t="s">
-        <v>666</v>
+        <v>669</v>
       </c>
       <c r="AL66" s="67"/>
       <c r="AM66" s="67"/>
@@ -16808,10 +16861,10 @@
       <c r="I67" s="67"/>
       <c r="J67" s="67"/>
       <c r="K67" s="67" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="L67" s="67" t="s">
-        <v>667</v>
+        <v>670</v>
       </c>
       <c r="M67" s="67"/>
       <c r="N67" s="67"/>
@@ -16837,10 +16890,10 @@
       <c r="AH67" s="67"/>
       <c r="AI67" s="67"/>
       <c r="AJ67" s="67" t="s">
-        <v>668</v>
+        <v>671</v>
       </c>
       <c r="AK67" s="67" t="s">
-        <v>669</v>
+        <v>672</v>
       </c>
       <c r="AL67" s="67"/>
       <c r="AM67" s="67"/>
@@ -16862,10 +16915,10 @@
       <c r="I68" s="67"/>
       <c r="J68" s="67"/>
       <c r="K68" s="67" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="L68" s="67" t="s">
-        <v>670</v>
+        <v>673</v>
       </c>
       <c r="M68" s="67"/>
       <c r="N68" s="67"/>
@@ -16891,10 +16944,10 @@
       <c r="AH68" s="67"/>
       <c r="AI68" s="67"/>
       <c r="AJ68" s="67" t="s">
-        <v>671</v>
+        <v>674</v>
       </c>
       <c r="AK68" s="67" t="s">
-        <v>672</v>
+        <v>675</v>
       </c>
       <c r="AL68" s="67"/>
       <c r="AM68" s="67"/>
@@ -16916,10 +16969,10 @@
       <c r="I69" s="67"/>
       <c r="J69" s="67"/>
       <c r="K69" s="67" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="L69" s="67" t="s">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="M69" s="67"/>
       <c r="N69" s="67"/>
@@ -16945,10 +16998,10 @@
       <c r="AH69" s="67"/>
       <c r="AI69" s="67"/>
       <c r="AJ69" s="67" t="s">
-        <v>674</v>
+        <v>677</v>
       </c>
       <c r="AK69" s="67" t="s">
-        <v>675</v>
+        <v>678</v>
       </c>
       <c r="AL69" s="67"/>
       <c r="AM69" s="67"/>
@@ -16970,10 +17023,10 @@
       <c r="I70" s="67"/>
       <c r="J70" s="67"/>
       <c r="K70" s="67" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="L70" s="67" t="s">
-        <v>676</v>
+        <v>679</v>
       </c>
       <c r="M70" s="67"/>
       <c r="N70" s="67"/>
@@ -16999,10 +17052,10 @@
       <c r="AH70" s="67"/>
       <c r="AI70" s="67"/>
       <c r="AJ70" s="67" t="s">
-        <v>677</v>
+        <v>680</v>
       </c>
       <c r="AK70" s="67" t="s">
-        <v>678</v>
+        <v>681</v>
       </c>
       <c r="AL70" s="67"/>
       <c r="AM70" s="67"/>
@@ -17024,10 +17077,10 @@
       <c r="I71" s="67"/>
       <c r="J71" s="67"/>
       <c r="K71" s="67" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="L71" s="67" t="s">
-        <v>679</v>
+        <v>682</v>
       </c>
       <c r="M71" s="67"/>
       <c r="N71" s="67"/>
@@ -17053,10 +17106,10 @@
       <c r="AH71" s="67"/>
       <c r="AI71" s="67"/>
       <c r="AJ71" s="67" t="s">
-        <v>680</v>
+        <v>683</v>
       </c>
       <c r="AK71" s="67" t="s">
-        <v>681</v>
+        <v>684</v>
       </c>
       <c r="AL71" s="67"/>
       <c r="AM71" s="67"/>
@@ -17078,10 +17131,10 @@
       <c r="I72" s="67"/>
       <c r="J72" s="67"/>
       <c r="K72" s="67" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="L72" s="67" t="s">
-        <v>682</v>
+        <v>685</v>
       </c>
       <c r="M72" s="67"/>
       <c r="N72" s="67"/>
@@ -17110,7 +17163,7 @@
         <v>202</v>
       </c>
       <c r="AK72" s="67" t="s">
-        <v>683</v>
+        <v>686</v>
       </c>
       <c r="AL72" s="67"/>
       <c r="AM72" s="67"/>
@@ -17132,10 +17185,10 @@
       <c r="I73" s="67"/>
       <c r="J73" s="67"/>
       <c r="K73" s="67" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="L73" s="67" t="s">
-        <v>684</v>
+        <v>687</v>
       </c>
       <c r="M73" s="67"/>
       <c r="N73" s="67"/>
@@ -17162,7 +17215,7 @@
       <c r="AI73" s="67"/>
       <c r="AJ73" s="67"/>
       <c r="AK73" s="67" t="s">
-        <v>685</v>
+        <v>688</v>
       </c>
       <c r="AL73" s="67"/>
       <c r="AM73" s="67"/>
@@ -17184,10 +17237,10 @@
       <c r="I74" s="67"/>
       <c r="J74" s="67"/>
       <c r="K74" s="67" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="L74" s="67" t="s">
-        <v>686</v>
+        <v>689</v>
       </c>
       <c r="M74" s="67"/>
       <c r="N74" s="67"/>
@@ -17214,7 +17267,7 @@
       <c r="AI74" s="67"/>
       <c r="AJ74" s="67"/>
       <c r="AK74" s="67" t="s">
-        <v>687</v>
+        <v>690</v>
       </c>
       <c r="AL74" s="67"/>
       <c r="AM74" s="67"/>
@@ -17226,98 +17279,98 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K75" s="67" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="L75" s="67" t="s">
-        <v>688</v>
+        <v>691</v>
       </c>
       <c r="O75" s="68"/>
       <c r="AJ75" s="5"/>
       <c r="AK75" s="5" t="s">
-        <v>689</v>
+        <v>692</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K76" s="67" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="L76" s="67" t="s">
-        <v>690</v>
+        <v>693</v>
       </c>
       <c r="O76" s="68"/>
       <c r="AJ76" s="5"/>
       <c r="AK76" s="5" t="s">
-        <v>691</v>
+        <v>694</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K77" s="67" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="L77" s="67" t="s">
-        <v>692</v>
+        <v>695</v>
       </c>
       <c r="O77" s="68"/>
       <c r="AJ77" s="5"/>
       <c r="AK77" s="5" t="s">
-        <v>693</v>
+        <v>696</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K78" s="67" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="L78" s="67" t="s">
-        <v>694</v>
+        <v>697</v>
       </c>
       <c r="O78" s="68"/>
       <c r="AJ78" s="5"/>
       <c r="AK78" s="5" t="s">
-        <v>695</v>
+        <v>698</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K79" s="67" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="L79" s="67" t="s">
-        <v>696</v>
+        <v>699</v>
       </c>
       <c r="O79" s="68"/>
       <c r="AJ79" s="5"/>
       <c r="AK79" s="5" t="s">
-        <v>697</v>
+        <v>700</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K80" s="67" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="L80" s="67" t="s">
-        <v>698</v>
+        <v>701</v>
       </c>
       <c r="O80" s="68"/>
       <c r="AJ80" s="5"/>
       <c r="AK80" s="5" t="s">
-        <v>699</v>
+        <v>702</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K81" s="67" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="L81" s="67" t="s">
-        <v>700</v>
+        <v>703</v>
       </c>
       <c r="O81" s="68"/>
       <c r="AJ81" s="5"/>
       <c r="AK81" s="5" t="s">
-        <v>701</v>
+        <v>704</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K82" s="67" t="s">
-        <v>702</v>
+        <v>705</v>
       </c>
       <c r="L82" s="67" t="s">
         <v>202</v>
@@ -17325,229 +17378,229 @@
       <c r="O82" s="68"/>
       <c r="AJ82" s="5"/>
       <c r="AK82" s="5" t="s">
-        <v>703</v>
+        <v>706</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K83" s="0" t="s">
-        <v>704</v>
+        <v>707</v>
       </c>
       <c r="O83" s="68"/>
       <c r="AJ83" s="5"/>
       <c r="AK83" s="5" t="s">
-        <v>705</v>
+        <v>708</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K84" s="67" t="s">
-        <v>706</v>
+        <v>709</v>
       </c>
       <c r="O84" s="68"/>
       <c r="AJ84" s="5"/>
       <c r="AK84" s="5" t="s">
-        <v>707</v>
+        <v>710</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K85" s="0" t="s">
-        <v>708</v>
+        <v>711</v>
       </c>
       <c r="O85" s="68"/>
       <c r="Q85" s="67"/>
       <c r="AJ85" s="5"/>
       <c r="AK85" s="5" t="s">
-        <v>709</v>
+        <v>712</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K86" s="67" t="s">
-        <v>710</v>
+        <v>713</v>
       </c>
       <c r="O86" s="68"/>
       <c r="Q86" s="67"/>
       <c r="AJ86" s="5"/>
       <c r="AK86" s="5" t="s">
-        <v>711</v>
+        <v>714</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K87" s="0" t="s">
-        <v>712</v>
+        <v>715</v>
       </c>
       <c r="O87" s="68"/>
       <c r="AJ87" s="5"/>
       <c r="AK87" s="5" t="s">
-        <v>713</v>
+        <v>716</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K88" s="67" t="s">
-        <v>714</v>
+        <v>717</v>
       </c>
       <c r="O88" s="68"/>
       <c r="AJ88" s="5"/>
       <c r="AK88" s="5" t="s">
-        <v>715</v>
+        <v>718</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K89" s="67" t="s">
-        <v>716</v>
+        <v>719</v>
       </c>
       <c r="O89" s="68"/>
       <c r="AJ89" s="5"/>
       <c r="AK89" s="5" t="s">
-        <v>717</v>
+        <v>720</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K90" s="67" t="s">
-        <v>718</v>
+        <v>721</v>
       </c>
       <c r="O90" s="68"/>
       <c r="AJ90" s="5"/>
       <c r="AK90" s="5" t="s">
-        <v>719</v>
+        <v>722</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K91" s="67" t="s">
-        <v>720</v>
+        <v>723</v>
       </c>
       <c r="O91" s="68"/>
       <c r="AJ91" s="5"/>
       <c r="AK91" s="5" t="s">
-        <v>721</v>
+        <v>724</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K92" s="67" t="s">
-        <v>722</v>
+        <v>725</v>
       </c>
       <c r="O92" s="68"/>
       <c r="AJ92" s="5"/>
       <c r="AK92" s="5" t="s">
-        <v>723</v>
+        <v>726</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K93" s="67" t="s">
-        <v>724</v>
+        <v>727</v>
       </c>
       <c r="O93" s="68"/>
       <c r="AJ93" s="5"/>
       <c r="AK93" s="5" t="s">
-        <v>725</v>
+        <v>728</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K94" s="67" t="s">
-        <v>726</v>
+        <v>729</v>
       </c>
       <c r="O94" s="68"/>
       <c r="AJ94" s="5"/>
       <c r="AK94" s="5" t="s">
-        <v>727</v>
+        <v>730</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K95" s="67" t="s">
-        <v>728</v>
+        <v>731</v>
       </c>
       <c r="O95" s="68"/>
       <c r="AJ95" s="5"/>
       <c r="AK95" s="5" t="s">
-        <v>729</v>
+        <v>732</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K96" s="67" t="s">
-        <v>730</v>
+        <v>733</v>
       </c>
       <c r="O96" s="68"/>
       <c r="AJ96" s="5"/>
       <c r="AK96" s="5" t="s">
-        <v>731</v>
+        <v>734</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K97" s="67" t="s">
-        <v>732</v>
+        <v>735</v>
       </c>
       <c r="O97" s="68"/>
       <c r="AJ97" s="5"/>
       <c r="AK97" s="5" t="s">
-        <v>733</v>
+        <v>736</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K98" s="67" t="s">
-        <v>734</v>
+        <v>737</v>
       </c>
       <c r="O98" s="68"/>
       <c r="AJ98" s="5"/>
       <c r="AK98" s="5" t="s">
-        <v>735</v>
+        <v>738</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K99" s="67" t="s">
-        <v>736</v>
+        <v>739</v>
       </c>
       <c r="O99" s="68"/>
       <c r="AJ99" s="5"/>
       <c r="AK99" s="5" t="s">
-        <v>737</v>
+        <v>740</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K100" s="67" t="s">
-        <v>738</v>
+        <v>741</v>
       </c>
       <c r="O100" s="68"/>
       <c r="AJ100" s="5"/>
       <c r="AK100" s="5" t="s">
-        <v>739</v>
+        <v>742</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K101" s="67" t="s">
-        <v>740</v>
+        <v>743</v>
       </c>
       <c r="O101" s="68"/>
       <c r="AJ101" s="5"/>
       <c r="AK101" s="5" t="s">
-        <v>741</v>
+        <v>744</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K102" s="67" t="s">
-        <v>742</v>
+        <v>745</v>
       </c>
       <c r="O102" s="68"/>
       <c r="AJ102" s="5"/>
       <c r="AK102" s="5" t="s">
-        <v>743</v>
+        <v>746</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K103" s="67" t="s">
-        <v>744</v>
+        <v>747</v>
       </c>
       <c r="O103" s="68"/>
       <c r="AJ103" s="5"/>
       <c r="AK103" s="5" t="s">
-        <v>745</v>
+        <v>748</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K104" s="67" t="s">
-        <v>746</v>
+        <v>749</v>
       </c>
       <c r="O104" s="68"/>
       <c r="AJ104" s="5"/>
       <c r="AK104" s="5" t="s">
-        <v>747</v>
+        <v>750</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17557,182 +17610,182 @@
       <c r="O105" s="68"/>
       <c r="AJ105" s="5"/>
       <c r="AK105" s="5" t="s">
-        <v>748</v>
+        <v>751</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O106" s="68"/>
       <c r="AJ106" s="5"/>
       <c r="AK106" s="5" t="s">
-        <v>749</v>
+        <v>752</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O107" s="68"/>
       <c r="AJ107" s="5"/>
       <c r="AK107" s="5" t="s">
-        <v>750</v>
+        <v>753</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O108" s="68"/>
       <c r="AJ108" s="5"/>
       <c r="AK108" s="5" t="s">
-        <v>751</v>
+        <v>754</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O109" s="68"/>
       <c r="AJ109" s="5"/>
       <c r="AK109" s="5" t="s">
-        <v>752</v>
+        <v>755</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O110" s="68"/>
       <c r="AJ110" s="5"/>
       <c r="AK110" s="5" t="s">
-        <v>753</v>
+        <v>756</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O111" s="68"/>
       <c r="AJ111" s="5"/>
       <c r="AK111" s="5" t="s">
-        <v>754</v>
+        <v>757</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O112" s="68"/>
       <c r="AJ112" s="5"/>
       <c r="AK112" s="5" t="s">
-        <v>755</v>
+        <v>758</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O113" s="68"/>
       <c r="AJ113" s="5"/>
       <c r="AK113" s="5" t="s">
-        <v>756</v>
+        <v>759</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O114" s="68"/>
       <c r="AJ114" s="5"/>
       <c r="AK114" s="5" t="s">
-        <v>757</v>
+        <v>760</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O115" s="68"/>
       <c r="AJ115" s="5"/>
       <c r="AK115" s="5" t="s">
-        <v>758</v>
+        <v>761</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O116" s="68"/>
       <c r="AJ116" s="5"/>
       <c r="AK116" s="5" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O117" s="68"/>
       <c r="AJ117" s="5"/>
       <c r="AK117" s="5" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O118" s="68"/>
       <c r="AJ118" s="5"/>
       <c r="AK118" s="5" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O119" s="68"/>
       <c r="AJ119" s="5"/>
       <c r="AK119" s="5" t="s">
-        <v>434</v>
+        <v>438</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O120" s="68"/>
       <c r="AJ120" s="5"/>
       <c r="AK120" s="5" t="s">
-        <v>442</v>
+        <v>446</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O121" s="68"/>
       <c r="AJ121" s="5"/>
       <c r="AK121" s="5" t="s">
-        <v>449</v>
+        <v>452</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O122" s="68"/>
       <c r="AJ122" s="5"/>
       <c r="AK122" s="5" t="s">
-        <v>759</v>
+        <v>762</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O123" s="68"/>
       <c r="AJ123" s="5"/>
       <c r="AK123" s="5" t="s">
-        <v>760</v>
+        <v>763</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O124" s="68"/>
       <c r="AJ124" s="5"/>
       <c r="AK124" s="5" t="s">
-        <v>761</v>
+        <v>764</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O125" s="68"/>
       <c r="AJ125" s="5"/>
       <c r="AK125" s="5" t="s">
-        <v>762</v>
+        <v>765</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O126" s="68"/>
       <c r="AJ126" s="5"/>
       <c r="AK126" s="5" t="s">
-        <v>763</v>
+        <v>766</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O127" s="68"/>
       <c r="AJ127" s="5"/>
       <c r="AK127" s="5" t="s">
-        <v>764</v>
+        <v>767</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O128" s="68"/>
       <c r="AJ128" s="5"/>
       <c r="AK128" s="5" t="s">
-        <v>765</v>
+        <v>768</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O129" s="68"/>
       <c r="AJ129" s="5"/>
       <c r="AK129" s="5" t="s">
-        <v>766</v>
+        <v>769</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O130" s="68"/>
       <c r="AJ130" s="5"/>
       <c r="AK130" s="5" t="s">
-        <v>767</v>
+        <v>770</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18633,7 +18686,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="AV12 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18646,27 +18699,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="72" t="s">
-        <v>768</v>
+        <v>771</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>769</v>
+        <v>772</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>770</v>
+        <v>773</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>771</v>
+        <v>774</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="73" t="s">
-        <v>772</v>
+        <v>775</v>
       </c>
       <c r="B2" s="73" t="s">
-        <v>773</v>
+        <v>776</v>
       </c>
       <c r="C2" s="73" t="s">
-        <v>774</v>
+        <v>777</v>
       </c>
       <c r="D2" s="74" t="n">
         <v>45253</v>
@@ -18674,13 +18727,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="75" t="s">
-        <v>775</v>
+        <v>778</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>776</v>
+        <v>779</v>
       </c>
       <c r="C3" s="76" t="s">
-        <v>777</v>
+        <v>780</v>
       </c>
       <c r="D3" s="77" t="n">
         <v>45265</v>
@@ -18688,13 +18741,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="73" t="s">
-        <v>778</v>
+        <v>781</v>
       </c>
       <c r="B4" s="78" t="s">
-        <v>779</v>
+        <v>782</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="D4" s="80" t="n">
         <v>45310</v>
@@ -18702,13 +18755,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="81" t="s">
-        <v>781</v>
+        <v>784</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>782</v>
+        <v>785</v>
       </c>
       <c r="C5" s="83" t="s">
-        <v>780</v>
+        <v>783</v>
       </c>
       <c r="D5" s="84" t="n">
         <v>45313</v>
@@ -18716,13 +18769,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="73" t="s">
+        <v>786</v>
+      </c>
+      <c r="B6" s="73" t="s">
+        <v>787</v>
+      </c>
+      <c r="C6" s="79" t="s">
         <v>783</v>
-      </c>
-      <c r="B6" s="73" t="s">
-        <v>784</v>
-      </c>
-      <c r="C6" s="79" t="s">
-        <v>780</v>
       </c>
       <c r="D6" s="85" t="n">
         <v>45314</v>
@@ -18730,13 +18783,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="81" t="s">
-        <v>785</v>
+        <v>788</v>
       </c>
       <c r="B7" s="82" t="s">
-        <v>786</v>
+        <v>789</v>
       </c>
       <c r="C7" s="83" t="s">
-        <v>787</v>
+        <v>790</v>
       </c>
       <c r="D7" s="84" t="n">
         <v>45316</v>
@@ -18744,13 +18797,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="86" t="s">
-        <v>788</v>
+        <v>791</v>
       </c>
       <c r="B8" s="86" t="s">
-        <v>789</v>
+        <v>792</v>
       </c>
       <c r="C8" s="87" t="s">
-        <v>790</v>
+        <v>793</v>
       </c>
       <c r="D8" s="88" t="n">
         <v>45316</v>
@@ -18776,10 +18829,10 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.14"/>
@@ -18787,7 +18840,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="55.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="70.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="70.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="46.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.28"/>
@@ -20297,20 +20350,20 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="34.13"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="28.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="31.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="19.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="37.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="60.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="60.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="40.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="49.15"/>
@@ -20425,7 +20478,7 @@
         <v>66</v>
       </c>
       <c r="J3" s="102" t="s">
-        <v>291</v>
+        <v>295</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>70</v>
@@ -20448,13 +20501,13 @@
       <c r="H4" s="103"/>
       <c r="I4" s="103"/>
       <c r="J4" s="103" t="s">
-        <v>791</v>
+        <v>794</v>
       </c>
       <c r="K4" s="103" t="s">
-        <v>792</v>
+        <v>795</v>
       </c>
       <c r="L4" s="103" t="s">
-        <v>793</v>
+        <v>796</v>
       </c>
       <c r="M4" s="103"/>
     </row>
@@ -20469,7 +20522,7 @@
       <c r="H5" s="103"/>
       <c r="I5" s="103"/>
       <c r="J5" s="104" t="s">
-        <v>794</v>
+        <v>797</v>
       </c>
       <c r="K5" s="103"/>
       <c r="L5" s="103"/>
@@ -21970,10 +22023,10 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
@@ -22030,7 +22083,7 @@
         <v>84</v>
       </c>
       <c r="D2" s="55" t="s">
-        <v>286</v>
+        <v>290</v>
       </c>
       <c r="E2" s="55" t="s">
         <v>91</v>
@@ -22061,7 +22114,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>83</v>
@@ -24019,20 +24072,20 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="32.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="91.86"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="41.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="91.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="41.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="28.14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="26.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="26.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="31.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="32.15"/>
@@ -24160,13 +24213,13 @@
         <v>194</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="C3" s="110" t="s">
         <v>95</v>
       </c>
       <c r="D3" s="110" t="s">
-        <v>796</v>
+        <v>799</v>
       </c>
       <c r="E3" s="114" t="s">
         <v>101</v>
@@ -24181,13 +24234,13 @@
         <v>113</v>
       </c>
       <c r="I3" s="115" t="s">
-        <v>292</v>
+        <v>296</v>
       </c>
       <c r="J3" s="110" t="s">
-        <v>293</v>
+        <v>297</v>
       </c>
       <c r="K3" s="110" t="s">
-        <v>294</v>
+        <v>298</v>
       </c>
       <c r="L3" s="110" t="s">
         <v>126</v>
@@ -25940,10 +25993,10 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.72265625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
@@ -26037,7 +26090,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="119" t="s">
-        <v>795</v>
+        <v>798</v>
       </c>
       <c r="C3" s="127" t="s">
         <v>158</v>

</xml_diff>

<commit_message>
Added duplicated samples to tests data
</commit_message>
<xml_diff>
--- a/tests/data/sftp_handle/datatest1/metadata_validation_test.xlsx
+++ b/tests/data/sftp_handle/datatest1/metadata_validation_test.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1547" uniqueCount="800">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1619" uniqueCount="818">
   <si>
     <t xml:space="preserve">Label name</t>
   </si>
@@ -894,6 +894,60 @@
   </si>
   <si>
     <t xml:space="preserve">SAMPLE7.R2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">888</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeated88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeated8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id008repeated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runid1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMPLE8_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMPLE8_R2.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">888bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeated88bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeated8bis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id008repeatedbis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Runid2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">999</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeated99</t>
+  </si>
+  <si>
+    <t xml:space="preserve">repeated9</t>
+  </si>
+  <si>
+    <t xml:space="preserve">id009repeated</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMPLE9_R1.fastq.gz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SAMPLE9_R2.fastq.gz</t>
   </si>
   <si>
     <t xml:space="preserve">ARTIC v.4</t>
@@ -3494,10 +3548,10 @@
   <dimension ref="A1:Z1001"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B3" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C20" activeCellId="1" sqref="AV12 C20"/>
+      <selection pane="topLeft" activeCell="C20" activeCellId="0" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="72.7"/>
@@ -3505,7 +3559,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="29.86"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="14.69"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="41.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="25.4"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6397,10 +6451,10 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
@@ -6448,10 +6502,10 @@
         <v>27</v>
       </c>
       <c r="C2" s="59" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="D2" s="59" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="E2" s="59" t="s">
         <v>193</v>
@@ -6482,13 +6536,13 @@
         <v>194</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>798</v>
+        <v>816</v>
       </c>
       <c r="C3" s="117" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="D3" s="117" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="E3" s="117" t="s">
         <v>171</v>
@@ -7530,10 +7584,10 @@
   <dimension ref="A1:D1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="30.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
@@ -7574,7 +7628,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="89" t="s">
-        <v>798</v>
+        <v>816</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>176</v>
@@ -8600,11 +8654,11 @@
   </sheetPr>
   <dimension ref="A1:AV1000"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AM1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AV12" activeCellId="0" sqref="AV12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L14" activeCellId="0" sqref="L14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="22.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="28.86"/>
@@ -9911,152 +9965,296 @@
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="44"/>
       <c r="B13" s="34"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
+      <c r="C13" s="41" t="s">
+        <v>287</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>288</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>289</v>
+      </c>
       <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
+      <c r="G13" s="41" t="s">
+        <v>290</v>
+      </c>
       <c r="H13" s="41"/>
       <c r="I13" s="41"/>
       <c r="J13" s="41"/>
-      <c r="K13" s="41"/>
-      <c r="L13" s="41"/>
-      <c r="M13" s="41"/>
-      <c r="N13" s="41"/>
-      <c r="O13" s="41"/>
-      <c r="P13" s="41"/>
+      <c r="K13" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="L13" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="M13" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="N13" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="O13" s="41" t="s">
+        <v>265</v>
+      </c>
+      <c r="P13" s="41" t="s">
+        <v>60</v>
+      </c>
       <c r="Q13" s="41"/>
       <c r="R13" s="41"/>
       <c r="S13" s="41"/>
       <c r="T13" s="41"/>
       <c r="U13" s="41"/>
-      <c r="V13" s="41"/>
+      <c r="V13" s="41" t="s">
+        <v>85</v>
+      </c>
       <c r="W13" s="41"/>
       <c r="X13" s="41"/>
-      <c r="Y13" s="41"/>
+      <c r="Y13" s="41" t="s">
+        <v>203</v>
+      </c>
       <c r="Z13" s="41"/>
-      <c r="AA13" s="41"/>
+      <c r="AA13" s="41" t="s">
+        <v>206</v>
+      </c>
       <c r="AB13" s="41"/>
-      <c r="AC13" s="41"/>
+      <c r="AC13" s="41" t="s">
+        <v>111</v>
+      </c>
       <c r="AD13" s="41"/>
-      <c r="AE13" s="41"/>
+      <c r="AE13" s="41" t="s">
+        <v>207</v>
+      </c>
       <c r="AF13" s="41"/>
-      <c r="AG13" s="41"/>
+      <c r="AG13" s="41" t="s">
+        <v>269</v>
+      </c>
       <c r="AH13" s="41"/>
-      <c r="AI13" s="41"/>
-      <c r="AJ13" s="41"/>
+      <c r="AI13" s="41" t="s">
+        <v>291</v>
+      </c>
+      <c r="AJ13" s="41" t="s">
+        <v>187</v>
+      </c>
       <c r="AK13" s="41"/>
-      <c r="AL13" s="41"/>
-      <c r="AM13" s="41"/>
-      <c r="AN13" s="41"/>
-      <c r="AO13" s="41"/>
+      <c r="AL13" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM13" s="41" t="s">
+        <v>270</v>
+      </c>
+      <c r="AN13" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO13" s="41" t="s">
+        <v>210</v>
+      </c>
       <c r="AP13" s="41"/>
       <c r="AQ13" s="41"/>
       <c r="AR13" s="41"/>
       <c r="AS13" s="41"/>
       <c r="AT13" s="41"/>
-      <c r="AU13" s="41"/>
-      <c r="AV13" s="41"/>
+      <c r="AU13" s="41" t="s">
+        <v>292</v>
+      </c>
+      <c r="AV13" s="41" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="44"/>
       <c r="B14" s="34"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
+      <c r="C14" s="41" t="s">
+        <v>294</v>
+      </c>
+      <c r="D14" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="E14" s="41" t="s">
+        <v>296</v>
+      </c>
       <c r="F14" s="41"/>
-      <c r="G14" s="41"/>
+      <c r="G14" s="41" t="s">
+        <v>297</v>
+      </c>
       <c r="H14" s="41"/>
       <c r="I14" s="41"/>
       <c r="J14" s="41"/>
-      <c r="K14" s="41"/>
-      <c r="L14" s="41"/>
-      <c r="M14" s="41"/>
-      <c r="N14" s="41"/>
-      <c r="O14" s="41"/>
-      <c r="P14" s="41"/>
+      <c r="K14" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="L14" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="M14" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="N14" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="O14" s="41" t="s">
+        <v>265</v>
+      </c>
+      <c r="P14" s="41" t="s">
+        <v>60</v>
+      </c>
       <c r="Q14" s="41"/>
       <c r="R14" s="41"/>
       <c r="S14" s="41"/>
       <c r="T14" s="41"/>
       <c r="U14" s="41"/>
-      <c r="V14" s="41"/>
+      <c r="V14" s="41" t="s">
+        <v>85</v>
+      </c>
       <c r="W14" s="41"/>
       <c r="X14" s="41"/>
-      <c r="Y14" s="41"/>
+      <c r="Y14" s="41" t="s">
+        <v>268</v>
+      </c>
       <c r="Z14" s="41"/>
-      <c r="AA14" s="41"/>
+      <c r="AA14" s="41" t="s">
+        <v>206</v>
+      </c>
       <c r="AB14" s="41"/>
-      <c r="AC14" s="41"/>
+      <c r="AC14" s="41" t="s">
+        <v>111</v>
+      </c>
       <c r="AD14" s="41"/>
-      <c r="AE14" s="41"/>
+      <c r="AE14" s="41" t="s">
+        <v>207</v>
+      </c>
       <c r="AF14" s="41"/>
-      <c r="AG14" s="41"/>
+      <c r="AG14" s="41" t="s">
+        <v>269</v>
+      </c>
       <c r="AH14" s="41"/>
-      <c r="AI14" s="41"/>
-      <c r="AJ14" s="41"/>
+      <c r="AI14" s="41" t="s">
+        <v>298</v>
+      </c>
+      <c r="AJ14" s="41" t="s">
+        <v>187</v>
+      </c>
       <c r="AK14" s="41"/>
-      <c r="AL14" s="41"/>
-      <c r="AM14" s="41"/>
-      <c r="AN14" s="41"/>
-      <c r="AO14" s="41"/>
+      <c r="AL14" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM14" s="41" t="s">
+        <v>270</v>
+      </c>
+      <c r="AN14" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO14" s="41" t="s">
+        <v>210</v>
+      </c>
       <c r="AP14" s="41"/>
       <c r="AQ14" s="41"/>
       <c r="AR14" s="41"/>
       <c r="AS14" s="41"/>
       <c r="AT14" s="41"/>
-      <c r="AU14" s="41"/>
-      <c r="AV14" s="41"/>
+      <c r="AU14" s="41" t="s">
+        <v>292</v>
+      </c>
+      <c r="AV14" s="41" t="s">
+        <v>293</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="44"/>
       <c r="B15" s="34"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
+      <c r="C15" s="41" t="s">
+        <v>299</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>300</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>301</v>
+      </c>
       <c r="F15" s="41"/>
-      <c r="G15" s="41"/>
+      <c r="G15" s="41" t="s">
+        <v>302</v>
+      </c>
       <c r="H15" s="41"/>
       <c r="I15" s="41"/>
       <c r="J15" s="41"/>
-      <c r="K15" s="41"/>
-      <c r="L15" s="41"/>
-      <c r="M15" s="41"/>
-      <c r="N15" s="41"/>
-      <c r="O15" s="41"/>
-      <c r="P15" s="41"/>
+      <c r="K15" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="L15" s="41" t="s">
+        <v>48</v>
+      </c>
+      <c r="M15" s="41" t="s">
+        <v>202</v>
+      </c>
+      <c r="N15" s="41" t="s">
+        <v>203</v>
+      </c>
+      <c r="O15" s="41" t="s">
+        <v>265</v>
+      </c>
+      <c r="P15" s="41" t="s">
+        <v>60</v>
+      </c>
       <c r="Q15" s="41"/>
       <c r="R15" s="41"/>
       <c r="S15" s="41"/>
       <c r="T15" s="41"/>
       <c r="U15" s="41"/>
-      <c r="V15" s="41"/>
+      <c r="V15" s="41" t="s">
+        <v>85</v>
+      </c>
       <c r="W15" s="41"/>
       <c r="X15" s="41"/>
-      <c r="Y15" s="41"/>
+      <c r="Y15" s="41" t="s">
+        <v>268</v>
+      </c>
       <c r="Z15" s="41"/>
-      <c r="AA15" s="41"/>
+      <c r="AA15" s="41" t="s">
+        <v>206</v>
+      </c>
       <c r="AB15" s="41"/>
-      <c r="AC15" s="41"/>
+      <c r="AC15" s="41" t="s">
+        <v>111</v>
+      </c>
       <c r="AD15" s="41"/>
-      <c r="AE15" s="41"/>
+      <c r="AE15" s="41" t="s">
+        <v>207</v>
+      </c>
       <c r="AF15" s="41"/>
-      <c r="AG15" s="41"/>
+      <c r="AG15" s="41" t="s">
+        <v>269</v>
+      </c>
       <c r="AH15" s="41"/>
-      <c r="AI15" s="41"/>
-      <c r="AJ15" s="41"/>
+      <c r="AI15" s="41" t="s">
+        <v>298</v>
+      </c>
+      <c r="AJ15" s="41" t="s">
+        <v>187</v>
+      </c>
       <c r="AK15" s="41"/>
-      <c r="AL15" s="41"/>
-      <c r="AM15" s="41"/>
-      <c r="AN15" s="41"/>
-      <c r="AO15" s="41"/>
+      <c r="AL15" s="41" t="s">
+        <v>209</v>
+      </c>
+      <c r="AM15" s="41" t="s">
+        <v>270</v>
+      </c>
+      <c r="AN15" s="41" t="s">
+        <v>151</v>
+      </c>
+      <c r="AO15" s="41" t="s">
+        <v>210</v>
+      </c>
       <c r="AP15" s="41"/>
       <c r="AQ15" s="41"/>
       <c r="AR15" s="41"/>
       <c r="AS15" s="41"/>
       <c r="AT15" s="41"/>
-      <c r="AU15" s="41"/>
-      <c r="AV15" s="41"/>
+      <c r="AU15" s="41" t="s">
+        <v>303</v>
+      </c>
+      <c r="AV15" s="41" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="44"/>
@@ -12474,15 +12672,15 @@
   <dimension ref="A1:AV1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="AC1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="AG15" activeCellId="1" sqref="AV12 AG15"/>
+      <selection pane="topLeft" activeCell="AG15" activeCellId="0" sqref="AG15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="13.86"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="10" min="2" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="60"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="61.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="61.31"/>
     <col collapsed="false" customWidth="true" hidden="true" outlineLevel="0" max="14" min="13" style="0" width="0.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="60.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="38.43"/>
@@ -12508,7 +12706,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="36" min="36" style="0" width="32.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="37" min="37" style="0" width="49.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="38" min="38" style="0" width="71.42"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="44.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="39" min="39" style="0" width="44.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="40" min="40" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="41" min="41" style="0" width="15.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="42" min="42" style="0" width="15.71"/>
@@ -12661,7 +12859,7 @@
       </c>
       <c r="AF2" s="50"/>
       <c r="AG2" s="50" t="s">
-        <v>287</v>
+        <v>305</v>
       </c>
       <c r="AH2" s="50" t="n">
         <v>96</v>
@@ -12670,7 +12868,7 @@
         <v>131</v>
       </c>
       <c r="AJ2" s="50" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="AK2" s="50" t="s">
         <v>139</v>
@@ -12760,7 +12958,7 @@
         <v>71</v>
       </c>
       <c r="T3" s="56" t="s">
-        <v>289</v>
+        <v>307</v>
       </c>
       <c r="U3" s="56" t="s">
         <v>79</v>
@@ -12769,7 +12967,7 @@
         <v>84</v>
       </c>
       <c r="W3" s="56" t="s">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="X3" s="56" t="s">
         <v>91</v>
@@ -12836,10 +13034,10 @@
         <v>168</v>
       </c>
       <c r="AT3" s="59" t="s">
-        <v>291</v>
+        <v>309</v>
       </c>
       <c r="AU3" s="59" t="s">
-        <v>292</v>
+        <v>310</v>
       </c>
       <c r="AV3" s="59" t="s">
         <v>193</v>
@@ -12880,7 +13078,7 @@
         <v>42</v>
       </c>
       <c r="L4" s="28" t="s">
-        <v>293</v>
+        <v>311</v>
       </c>
       <c r="M4" s="28" t="s">
         <v>53</v>
@@ -12892,13 +13090,13 @@
         <v>58</v>
       </c>
       <c r="P4" s="28" t="s">
-        <v>294</v>
+        <v>312</v>
       </c>
       <c r="Q4" s="28" t="s">
         <v>66</v>
       </c>
       <c r="R4" s="28" t="s">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="S4" s="28" t="s">
         <v>70</v>
@@ -12937,13 +13135,13 @@
         <v>113</v>
       </c>
       <c r="AE4" s="28" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="AF4" s="28" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="AG4" s="28" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="AH4" s="28" t="s">
         <v>126</v>
@@ -12982,10 +13180,10 @@
         <v>167</v>
       </c>
       <c r="AT4" s="63" t="s">
-        <v>299</v>
+        <v>317</v>
       </c>
       <c r="AU4" s="63" t="s">
-        <v>300</v>
+        <v>318</v>
       </c>
       <c r="AV4" s="63" t="s">
         <v>171</v>
@@ -13065,11 +13263,11 @@
       </c>
       <c r="P6" s="67"/>
       <c r="Q6" s="67" t="s">
-        <v>301</v>
+        <v>319</v>
       </c>
       <c r="R6" s="67"/>
       <c r="S6" s="67" t="s">
-        <v>302</v>
+        <v>320</v>
       </c>
       <c r="T6" s="67" t="s">
         <v>76</v>
@@ -13082,15 +13280,15 @@
       </c>
       <c r="W6" s="67"/>
       <c r="X6" s="67" t="s">
-        <v>303</v>
+        <v>321</v>
       </c>
       <c r="Y6" s="67"/>
       <c r="Z6" s="67"/>
       <c r="AA6" s="67" t="s">
-        <v>304</v>
+        <v>322</v>
       </c>
       <c r="AB6" s="67" t="s">
-        <v>305</v>
+        <v>323</v>
       </c>
       <c r="AC6" s="67" t="s">
         <v>111</v>
@@ -13101,21 +13299,21 @@
       </c>
       <c r="AF6" s="67"/>
       <c r="AG6" s="67" t="s">
-        <v>306</v>
+        <v>324</v>
       </c>
       <c r="AH6" s="67"/>
       <c r="AI6" s="67"/>
       <c r="AJ6" s="67" t="s">
-        <v>307</v>
+        <v>325</v>
       </c>
       <c r="AK6" s="67" t="s">
-        <v>308</v>
+        <v>326</v>
       </c>
       <c r="AL6" s="67" t="s">
         <v>235</v>
       </c>
       <c r="AM6" s="67" t="s">
-        <v>309</v>
+        <v>327</v>
       </c>
       <c r="AN6" s="67" t="s">
         <v>151</v>
@@ -13124,11 +13322,11 @@
         <v>237</v>
       </c>
       <c r="AP6" s="67" t="s">
-        <v>310</v>
+        <v>328</v>
       </c>
       <c r="AQ6" s="67"/>
       <c r="AR6" s="67" t="s">
-        <v>310</v>
+        <v>328</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13143,10 +13341,10 @@
       <c r="I7" s="67"/>
       <c r="J7" s="67"/>
       <c r="K7" s="67" t="s">
-        <v>311</v>
+        <v>329</v>
       </c>
       <c r="L7" s="67" t="s">
-        <v>312</v>
+        <v>330</v>
       </c>
       <c r="M7" s="67"/>
       <c r="N7" s="67"/>
@@ -13155,54 +13353,54 @@
       </c>
       <c r="P7" s="67"/>
       <c r="Q7" s="67" t="s">
-        <v>313</v>
+        <v>331</v>
       </c>
       <c r="R7" s="67"/>
       <c r="S7" s="67" t="s">
-        <v>314</v>
+        <v>332</v>
       </c>
       <c r="T7" s="67" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="U7" s="67" t="s">
         <v>202</v>
       </c>
       <c r="V7" s="67" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
       <c r="W7" s="67"/>
       <c r="X7" s="67" t="s">
-        <v>317</v>
+        <v>335</v>
       </c>
       <c r="Y7" s="67"/>
       <c r="Z7" s="67"/>
       <c r="AA7" s="67" t="s">
-        <v>318</v>
+        <v>336</v>
       </c>
       <c r="AB7" s="67" t="s">
         <v>233</v>
       </c>
       <c r="AC7" s="67" t="s">
-        <v>319</v>
+        <v>337</v>
       </c>
       <c r="AD7" s="67"/>
       <c r="AE7" s="67" t="s">
-        <v>320</v>
+        <v>338</v>
       </c>
       <c r="AF7" s="67"/>
       <c r="AG7" s="67" t="s">
-        <v>321</v>
+        <v>339</v>
       </c>
       <c r="AH7" s="67"/>
       <c r="AI7" s="67"/>
       <c r="AJ7" s="67" t="s">
-        <v>322</v>
+        <v>340</v>
       </c>
       <c r="AK7" s="67" t="s">
-        <v>323</v>
+        <v>341</v>
       </c>
       <c r="AL7" s="67" t="s">
-        <v>324</v>
+        <v>342</v>
       </c>
       <c r="AM7" s="67" t="s">
         <v>270</v>
@@ -13214,11 +13412,11 @@
         <v>210</v>
       </c>
       <c r="AP7" s="67" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
       <c r="AQ7" s="67"/>
       <c r="AR7" s="67" t="s">
-        <v>325</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13233,47 +13431,47 @@
       <c r="I8" s="67"/>
       <c r="J8" s="67"/>
       <c r="K8" s="67" t="s">
-        <v>326</v>
+        <v>344</v>
       </c>
       <c r="L8" s="67" t="s">
-        <v>326</v>
+        <v>344</v>
       </c>
       <c r="M8" s="67"/>
       <c r="N8" s="67"/>
       <c r="O8" s="68"/>
       <c r="P8" s="67"/>
       <c r="Q8" s="67" t="s">
-        <v>327</v>
+        <v>345</v>
       </c>
       <c r="R8" s="67"/>
       <c r="S8" s="67" t="s">
-        <v>328</v>
+        <v>346</v>
       </c>
       <c r="T8" s="67" t="s">
-        <v>329</v>
+        <v>347</v>
       </c>
       <c r="U8" s="67"/>
       <c r="V8" s="67" t="s">
-        <v>330</v>
+        <v>348</v>
       </c>
       <c r="W8" s="67"/>
       <c r="X8" s="67" t="s">
-        <v>331</v>
+        <v>349</v>
       </c>
       <c r="Y8" s="67"/>
       <c r="Z8" s="67"/>
       <c r="AA8" s="67" t="s">
-        <v>332</v>
+        <v>350</v>
       </c>
       <c r="AB8" s="67" t="s">
-        <v>333</v>
+        <v>351</v>
       </c>
       <c r="AC8" s="67" t="s">
-        <v>334</v>
+        <v>352</v>
       </c>
       <c r="AD8" s="67"/>
       <c r="AE8" s="67" t="s">
-        <v>335</v>
+        <v>353</v>
       </c>
       <c r="AF8" s="67"/>
       <c r="AG8" s="67" t="s">
@@ -13282,27 +13480,27 @@
       <c r="AH8" s="67"/>
       <c r="AI8" s="67"/>
       <c r="AJ8" s="67" t="s">
-        <v>336</v>
+        <v>354</v>
       </c>
       <c r="AK8" s="67" t="s">
-        <v>337</v>
+        <v>355</v>
       </c>
       <c r="AL8" s="67" t="s">
-        <v>338</v>
+        <v>356</v>
       </c>
       <c r="AM8" s="67" t="s">
-        <v>339</v>
+        <v>357</v>
       </c>
       <c r="AN8" s="67" t="s">
-        <v>340</v>
+        <v>358</v>
       </c>
       <c r="AO8" s="67"/>
       <c r="AP8" s="67" t="s">
-        <v>341</v>
+        <v>359</v>
       </c>
       <c r="AQ8" s="67"/>
       <c r="AR8" s="67" t="s">
-        <v>341</v>
+        <v>359</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13317,28 +13515,28 @@
       <c r="I9" s="67"/>
       <c r="J9" s="67"/>
       <c r="K9" s="67" t="s">
-        <v>342</v>
+        <v>360</v>
       </c>
       <c r="L9" s="67" t="s">
-        <v>342</v>
+        <v>360</v>
       </c>
       <c r="M9" s="67"/>
       <c r="N9" s="67"/>
       <c r="O9" s="68"/>
       <c r="P9" s="67"/>
       <c r="Q9" s="67" t="s">
-        <v>343</v>
+        <v>361</v>
       </c>
       <c r="R9" s="67"/>
       <c r="S9" s="67" t="s">
-        <v>344</v>
+        <v>362</v>
       </c>
       <c r="T9" s="67" t="s">
-        <v>345</v>
+        <v>363</v>
       </c>
       <c r="U9" s="67"/>
       <c r="V9" s="67" t="s">
-        <v>346</v>
+        <v>364</v>
       </c>
       <c r="W9" s="67"/>
       <c r="X9" s="67" t="s">
@@ -13347,13 +13545,13 @@
       <c r="Y9" s="67"/>
       <c r="Z9" s="67"/>
       <c r="AA9" s="67" t="s">
-        <v>347</v>
+        <v>365</v>
       </c>
       <c r="AB9" s="67" t="s">
-        <v>348</v>
+        <v>366</v>
       </c>
       <c r="AC9" s="67" t="s">
-        <v>349</v>
+        <v>367</v>
       </c>
       <c r="AD9" s="67"/>
       <c r="AE9" s="67" t="s">
@@ -13366,13 +13564,13 @@
       <c r="AH9" s="67"/>
       <c r="AI9" s="67"/>
       <c r="AJ9" s="67" t="s">
-        <v>350</v>
+        <v>368</v>
       </c>
       <c r="AK9" s="67" t="s">
-        <v>351</v>
+        <v>369</v>
       </c>
       <c r="AL9" s="67" t="s">
-        <v>352</v>
+        <v>370</v>
       </c>
       <c r="AM9" s="67" t="s">
         <v>99</v>
@@ -13382,11 +13580,11 @@
       </c>
       <c r="AO9" s="67"/>
       <c r="AP9" s="67" t="s">
-        <v>353</v>
+        <v>371</v>
       </c>
       <c r="AQ9" s="67"/>
       <c r="AR9" s="67" t="s">
-        <v>353</v>
+        <v>371</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13401,21 +13599,21 @@
       <c r="I10" s="67"/>
       <c r="J10" s="67"/>
       <c r="K10" s="67" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="L10" s="67" t="s">
-        <v>354</v>
+        <v>372</v>
       </c>
       <c r="M10" s="67"/>
       <c r="N10" s="67"/>
       <c r="O10" s="68"/>
       <c r="P10" s="67"/>
       <c r="Q10" s="67" t="s">
-        <v>355</v>
+        <v>373</v>
       </c>
       <c r="R10" s="67"/>
       <c r="S10" s="67" t="s">
-        <v>356</v>
+        <v>374</v>
       </c>
       <c r="T10" s="67" t="s">
         <v>202</v>
@@ -13429,13 +13627,13 @@
       <c r="Y10" s="67"/>
       <c r="Z10" s="67"/>
       <c r="AA10" s="67" t="s">
-        <v>357</v>
+        <v>375</v>
       </c>
       <c r="AB10" s="67" t="s">
-        <v>358</v>
+        <v>376</v>
       </c>
       <c r="AC10" s="67" t="s">
-        <v>359</v>
+        <v>377</v>
       </c>
       <c r="AD10" s="67"/>
       <c r="AE10" s="67" t="s">
@@ -13448,27 +13646,27 @@
       <c r="AH10" s="67"/>
       <c r="AI10" s="67"/>
       <c r="AJ10" s="67" t="s">
-        <v>360</v>
+        <v>378</v>
       </c>
       <c r="AK10" s="67" t="s">
-        <v>361</v>
+        <v>379</v>
       </c>
       <c r="AL10" s="67" t="s">
-        <v>362</v>
+        <v>380</v>
       </c>
       <c r="AM10" s="67" t="s">
-        <v>363</v>
+        <v>381</v>
       </c>
       <c r="AN10" s="67" t="s">
-        <v>364</v>
+        <v>382</v>
       </c>
       <c r="AO10" s="67"/>
       <c r="AP10" s="67" t="s">
-        <v>365</v>
+        <v>383</v>
       </c>
       <c r="AQ10" s="67"/>
       <c r="AR10" s="67" t="s">
-        <v>365</v>
+        <v>383</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13483,21 +13681,21 @@
       <c r="I11" s="67"/>
       <c r="J11" s="67"/>
       <c r="K11" s="67" t="s">
-        <v>366</v>
+        <v>384</v>
       </c>
       <c r="L11" s="67" t="s">
-        <v>366</v>
+        <v>384</v>
       </c>
       <c r="M11" s="67"/>
       <c r="N11" s="67"/>
       <c r="O11" s="68"/>
       <c r="P11" s="67"/>
       <c r="Q11" s="67" t="s">
-        <v>367</v>
+        <v>385</v>
       </c>
       <c r="R11" s="67"/>
       <c r="S11" s="67" t="s">
-        <v>368</v>
+        <v>386</v>
       </c>
       <c r="T11" s="67"/>
       <c r="U11" s="67"/>
@@ -13507,46 +13705,46 @@
       <c r="Y11" s="67"/>
       <c r="Z11" s="67"/>
       <c r="AA11" s="67" t="s">
-        <v>369</v>
+        <v>387</v>
       </c>
       <c r="AB11" s="67" t="s">
-        <v>370</v>
+        <v>388</v>
       </c>
       <c r="AC11" s="67" t="s">
         <v>202</v>
       </c>
       <c r="AD11" s="67"/>
       <c r="AE11" s="67" t="s">
-        <v>371</v>
+        <v>389</v>
       </c>
       <c r="AF11" s="67"/>
       <c r="AG11" s="67" t="s">
-        <v>335</v>
+        <v>353</v>
       </c>
       <c r="AH11" s="67"/>
       <c r="AI11" s="67"/>
       <c r="AJ11" s="67" t="s">
-        <v>372</v>
+        <v>390</v>
       </c>
       <c r="AK11" s="67" t="s">
-        <v>373</v>
+        <v>391</v>
       </c>
       <c r="AL11" s="67" t="s">
         <v>209</v>
       </c>
       <c r="AM11" s="67" t="s">
-        <v>374</v>
+        <v>392</v>
       </c>
       <c r="AN11" s="67" t="s">
-        <v>375</v>
+        <v>393</v>
       </c>
       <c r="AO11" s="67"/>
       <c r="AP11" s="67" t="s">
-        <v>376</v>
+        <v>394</v>
       </c>
       <c r="AQ11" s="67"/>
       <c r="AR11" s="67" t="s">
-        <v>376</v>
+        <v>394</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13561,21 +13759,21 @@
       <c r="I12" s="67"/>
       <c r="J12" s="67"/>
       <c r="K12" s="67" t="s">
-        <v>377</v>
+        <v>395</v>
       </c>
       <c r="L12" s="67" t="s">
-        <v>377</v>
+        <v>395</v>
       </c>
       <c r="M12" s="67"/>
       <c r="N12" s="67"/>
       <c r="O12" s="68"/>
       <c r="P12" s="67"/>
       <c r="Q12" s="67" t="s">
-        <v>378</v>
+        <v>396</v>
       </c>
       <c r="R12" s="67"/>
       <c r="S12" s="67" t="s">
-        <v>379</v>
+        <v>397</v>
       </c>
       <c r="T12" s="67"/>
       <c r="U12" s="67"/>
@@ -13588,12 +13786,12 @@
         <v>206</v>
       </c>
       <c r="AB12" s="67" t="s">
-        <v>380</v>
+        <v>398</v>
       </c>
       <c r="AC12" s="67"/>
       <c r="AD12" s="67"/>
       <c r="AE12" s="67" t="s">
-        <v>381</v>
+        <v>399</v>
       </c>
       <c r="AF12" s="67"/>
       <c r="AG12" s="67" t="s">
@@ -13602,27 +13800,27 @@
       <c r="AH12" s="67"/>
       <c r="AI12" s="67"/>
       <c r="AJ12" s="67" t="s">
-        <v>382</v>
+        <v>400</v>
       </c>
       <c r="AK12" s="67" t="s">
-        <v>383</v>
+        <v>401</v>
       </c>
       <c r="AL12" s="67" t="s">
-        <v>384</v>
+        <v>402</v>
       </c>
       <c r="AM12" s="67" t="s">
-        <v>385</v>
+        <v>403</v>
       </c>
       <c r="AN12" s="67" t="s">
-        <v>386</v>
+        <v>404</v>
       </c>
       <c r="AO12" s="67"/>
       <c r="AP12" s="67" t="s">
-        <v>387</v>
+        <v>405</v>
       </c>
       <c r="AQ12" s="67"/>
       <c r="AR12" s="67" t="s">
-        <v>387</v>
+        <v>405</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13637,21 +13835,21 @@
       <c r="I13" s="67"/>
       <c r="J13" s="67"/>
       <c r="K13" s="67" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
       <c r="L13" s="67" t="s">
-        <v>388</v>
+        <v>406</v>
       </c>
       <c r="M13" s="67"/>
       <c r="N13" s="67"/>
       <c r="O13" s="68"/>
       <c r="P13" s="67"/>
       <c r="Q13" s="67" t="s">
-        <v>389</v>
+        <v>407</v>
       </c>
       <c r="R13" s="67"/>
       <c r="S13" s="67" t="s">
-        <v>390</v>
+        <v>408</v>
       </c>
       <c r="T13" s="67"/>
       <c r="U13" s="67"/>
@@ -13661,44 +13859,44 @@
       <c r="Y13" s="67"/>
       <c r="Z13" s="67"/>
       <c r="AA13" s="67" t="s">
-        <v>391</v>
+        <v>409</v>
       </c>
       <c r="AB13" s="67" t="s">
-        <v>392</v>
+        <v>410</v>
       </c>
       <c r="AC13" s="67"/>
       <c r="AD13" s="67"/>
       <c r="AE13" s="67" t="s">
-        <v>393</v>
+        <v>411</v>
       </c>
       <c r="AF13" s="67"/>
       <c r="AG13" s="67" t="s">
-        <v>394</v>
+        <v>412</v>
       </c>
       <c r="AH13" s="67"/>
       <c r="AI13" s="67"/>
       <c r="AJ13" s="67" t="s">
-        <v>395</v>
+        <v>413</v>
       </c>
       <c r="AK13" s="67" t="s">
-        <v>396</v>
+        <v>414</v>
       </c>
       <c r="AL13" s="67" t="s">
-        <v>397</v>
+        <v>415</v>
       </c>
       <c r="AM13" s="67" t="s">
-        <v>398</v>
+        <v>416</v>
       </c>
       <c r="AN13" s="67" t="s">
-        <v>399</v>
+        <v>417</v>
       </c>
       <c r="AO13" s="67"/>
       <c r="AP13" s="67" t="s">
-        <v>400</v>
+        <v>418</v>
       </c>
       <c r="AQ13" s="67"/>
       <c r="AR13" s="67" t="s">
-        <v>400</v>
+        <v>418</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13713,21 +13911,21 @@
       <c r="I14" s="67"/>
       <c r="J14" s="67"/>
       <c r="K14" s="67" t="s">
-        <v>401</v>
+        <v>419</v>
       </c>
       <c r="L14" s="67" t="s">
-        <v>401</v>
+        <v>419</v>
       </c>
       <c r="M14" s="67"/>
       <c r="N14" s="67"/>
       <c r="O14" s="68"/>
       <c r="P14" s="67"/>
       <c r="Q14" s="67" t="s">
-        <v>402</v>
+        <v>420</v>
       </c>
       <c r="R14" s="67"/>
       <c r="S14" s="67" t="s">
-        <v>403</v>
+        <v>421</v>
       </c>
       <c r="T14" s="67"/>
       <c r="U14" s="67"/>
@@ -13740,7 +13938,7 @@
         <v>202</v>
       </c>
       <c r="AB14" s="67" t="s">
-        <v>404</v>
+        <v>422</v>
       </c>
       <c r="AC14" s="67"/>
       <c r="AD14" s="67"/>
@@ -13749,32 +13947,32 @@
       </c>
       <c r="AF14" s="67"/>
       <c r="AG14" s="67" t="s">
-        <v>405</v>
+        <v>423</v>
       </c>
       <c r="AH14" s="67"/>
       <c r="AI14" s="67"/>
       <c r="AJ14" s="67" t="s">
-        <v>406</v>
+        <v>424</v>
       </c>
       <c r="AK14" s="67" t="s">
-        <v>407</v>
+        <v>425</v>
       </c>
       <c r="AL14" s="67" t="s">
-        <v>408</v>
+        <v>426</v>
       </c>
       <c r="AM14" s="67" t="s">
-        <v>409</v>
+        <v>427</v>
       </c>
       <c r="AN14" s="67" t="s">
-        <v>410</v>
+        <v>428</v>
       </c>
       <c r="AO14" s="67"/>
       <c r="AP14" s="67" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
       <c r="AQ14" s="67"/>
       <c r="AR14" s="67" t="s">
-        <v>411</v>
+        <v>429</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13789,21 +13987,21 @@
       <c r="I15" s="67"/>
       <c r="J15" s="67"/>
       <c r="K15" s="67" t="s">
-        <v>412</v>
+        <v>430</v>
       </c>
       <c r="L15" s="67" t="s">
-        <v>412</v>
+        <v>430</v>
       </c>
       <c r="M15" s="67"/>
       <c r="N15" s="67"/>
       <c r="O15" s="68"/>
       <c r="P15" s="67"/>
       <c r="Q15" s="67" t="s">
-        <v>413</v>
+        <v>431</v>
       </c>
       <c r="R15" s="67"/>
       <c r="S15" s="67" t="s">
-        <v>414</v>
+        <v>432</v>
       </c>
       <c r="T15" s="67"/>
       <c r="U15" s="67"/>
@@ -13814,7 +14012,7 @@
       <c r="Z15" s="67"/>
       <c r="AA15" s="67"/>
       <c r="AB15" s="67" t="s">
-        <v>415</v>
+        <v>433</v>
       </c>
       <c r="AC15" s="67"/>
       <c r="AD15" s="67"/>
@@ -13826,25 +14024,25 @@
       <c r="AH15" s="67"/>
       <c r="AI15" s="67"/>
       <c r="AJ15" s="67" t="s">
-        <v>416</v>
+        <v>434</v>
       </c>
       <c r="AK15" s="67" t="s">
-        <v>417</v>
+        <v>435</v>
       </c>
       <c r="AL15" s="67"/>
       <c r="AM15" s="67" t="s">
-        <v>418</v>
+        <v>436</v>
       </c>
       <c r="AN15" s="67" t="s">
-        <v>419</v>
+        <v>437</v>
       </c>
       <c r="AO15" s="67"/>
       <c r="AP15" s="67" t="s">
-        <v>420</v>
+        <v>438</v>
       </c>
       <c r="AQ15" s="67"/>
       <c r="AR15" s="67" t="s">
-        <v>420</v>
+        <v>438</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -13859,17 +14057,17 @@
       <c r="I16" s="67"/>
       <c r="J16" s="67"/>
       <c r="K16" s="67" t="s">
-        <v>421</v>
+        <v>439</v>
       </c>
       <c r="L16" s="67" t="s">
-        <v>421</v>
+        <v>439</v>
       </c>
       <c r="M16" s="67"/>
       <c r="N16" s="67"/>
       <c r="O16" s="68"/>
       <c r="P16" s="67"/>
       <c r="Q16" s="67" t="s">
-        <v>422</v>
+        <v>440</v>
       </c>
       <c r="R16" s="67"/>
       <c r="S16" s="67" t="s">
@@ -13884,29 +14082,29 @@
       <c r="Z16" s="67"/>
       <c r="AA16" s="67"/>
       <c r="AB16" s="67" t="s">
-        <v>423</v>
+        <v>441</v>
       </c>
       <c r="AC16" s="67"/>
       <c r="AD16" s="67"/>
       <c r="AE16" s="67"/>
       <c r="AF16" s="67"/>
       <c r="AG16" s="67" t="s">
-        <v>371</v>
+        <v>389</v>
       </c>
       <c r="AH16" s="67"/>
       <c r="AI16" s="67"/>
       <c r="AJ16" s="67" t="s">
-        <v>424</v>
+        <v>442</v>
       </c>
       <c r="AK16" s="67" t="s">
-        <v>425</v>
+        <v>443</v>
       </c>
       <c r="AL16" s="67"/>
       <c r="AM16" s="67" t="s">
-        <v>426</v>
+        <v>444</v>
       </c>
       <c r="AN16" s="67" t="s">
-        <v>427</v>
+        <v>445</v>
       </c>
       <c r="AO16" s="67"/>
       <c r="AP16" s="67" t="s">
@@ -13929,21 +14127,21 @@
       <c r="I17" s="67"/>
       <c r="J17" s="67"/>
       <c r="K17" s="67" t="s">
-        <v>428</v>
+        <v>446</v>
       </c>
       <c r="L17" s="67" t="s">
-        <v>428</v>
+        <v>446</v>
       </c>
       <c r="M17" s="67"/>
       <c r="N17" s="67"/>
       <c r="O17" s="68"/>
       <c r="P17" s="67"/>
       <c r="Q17" s="67" t="s">
-        <v>429</v>
+        <v>447</v>
       </c>
       <c r="R17" s="67"/>
       <c r="S17" s="67" t="s">
-        <v>430</v>
+        <v>448</v>
       </c>
       <c r="T17" s="67"/>
       <c r="U17" s="67"/>
@@ -13954,29 +14152,29 @@
       <c r="Z17" s="67"/>
       <c r="AA17" s="67"/>
       <c r="AB17" s="67" t="s">
-        <v>431</v>
+        <v>449</v>
       </c>
       <c r="AC17" s="67"/>
       <c r="AD17" s="67"/>
       <c r="AE17" s="67"/>
       <c r="AF17" s="67"/>
       <c r="AG17" s="67" t="s">
-        <v>381</v>
+        <v>399</v>
       </c>
       <c r="AH17" s="67"/>
       <c r="AI17" s="67"/>
       <c r="AJ17" s="67" t="s">
-        <v>288</v>
+        <v>306</v>
       </c>
       <c r="AK17" s="67" t="s">
-        <v>432</v>
+        <v>450</v>
       </c>
       <c r="AL17" s="67"/>
       <c r="AM17" s="67" t="s">
-        <v>433</v>
+        <v>451</v>
       </c>
       <c r="AN17" s="67" t="s">
-        <v>434</v>
+        <v>452</v>
       </c>
       <c r="AO17" s="67"/>
       <c r="AP17" s="67"/>
@@ -13995,21 +14193,21 @@
       <c r="I18" s="67"/>
       <c r="J18" s="67"/>
       <c r="K18" s="67" t="s">
-        <v>435</v>
+        <v>453</v>
       </c>
       <c r="L18" s="67" t="s">
-        <v>435</v>
+        <v>453</v>
       </c>
       <c r="M18" s="67"/>
       <c r="N18" s="67"/>
       <c r="O18" s="68"/>
       <c r="P18" s="67"/>
       <c r="Q18" s="67" t="s">
-        <v>436</v>
+        <v>454</v>
       </c>
       <c r="R18" s="67"/>
       <c r="S18" s="67" t="s">
-        <v>437</v>
+        <v>455</v>
       </c>
       <c r="T18" s="67"/>
       <c r="U18" s="67"/>
@@ -14027,7 +14225,7 @@
       <c r="AE18" s="67"/>
       <c r="AF18" s="67"/>
       <c r="AG18" s="67" t="s">
-        <v>393</v>
+        <v>411</v>
       </c>
       <c r="AH18" s="67"/>
       <c r="AI18" s="67"/>
@@ -14035,14 +14233,14 @@
         <v>187</v>
       </c>
       <c r="AK18" s="67" t="s">
-        <v>438</v>
+        <v>456</v>
       </c>
       <c r="AL18" s="67"/>
       <c r="AM18" s="67" t="s">
-        <v>439</v>
+        <v>457</v>
       </c>
       <c r="AN18" s="67" t="s">
-        <v>440</v>
+        <v>458</v>
       </c>
       <c r="AO18" s="67"/>
       <c r="AP18" s="67"/>
@@ -14061,21 +14259,21 @@
       <c r="I19" s="67"/>
       <c r="J19" s="67"/>
       <c r="K19" s="67" t="s">
-        <v>441</v>
+        <v>459</v>
       </c>
       <c r="L19" s="67" t="s">
-        <v>441</v>
+        <v>459</v>
       </c>
       <c r="M19" s="67"/>
       <c r="N19" s="67"/>
       <c r="O19" s="68"/>
       <c r="P19" s="67"/>
       <c r="Q19" s="67" t="s">
-        <v>442</v>
+        <v>460</v>
       </c>
       <c r="R19" s="67"/>
       <c r="S19" s="67" t="s">
-        <v>443</v>
+        <v>461</v>
       </c>
       <c r="T19" s="67"/>
       <c r="U19" s="67"/>
@@ -14086,7 +14284,7 @@
       <c r="Z19" s="67"/>
       <c r="AA19" s="67"/>
       <c r="AB19" s="67" t="s">
-        <v>444</v>
+        <v>462</v>
       </c>
       <c r="AC19" s="67"/>
       <c r="AD19" s="67"/>
@@ -14098,17 +14296,17 @@
       <c r="AH19" s="67"/>
       <c r="AI19" s="67"/>
       <c r="AJ19" s="67" t="s">
-        <v>445</v>
+        <v>463</v>
       </c>
       <c r="AK19" s="67" t="s">
-        <v>446</v>
+        <v>464</v>
       </c>
       <c r="AL19" s="67"/>
       <c r="AM19" s="67" t="s">
-        <v>447</v>
+        <v>465</v>
       </c>
       <c r="AN19" s="67" t="s">
-        <v>448</v>
+        <v>466</v>
       </c>
       <c r="AO19" s="67"/>
       <c r="AP19" s="67"/>
@@ -14127,21 +14325,21 @@
       <c r="I20" s="67"/>
       <c r="J20" s="67"/>
       <c r="K20" s="67" t="s">
-        <v>449</v>
+        <v>467</v>
       </c>
       <c r="L20" s="67" t="s">
-        <v>449</v>
+        <v>467</v>
       </c>
       <c r="M20" s="67"/>
       <c r="N20" s="67"/>
       <c r="O20" s="68"/>
       <c r="P20" s="67"/>
       <c r="Q20" s="67" t="s">
-        <v>450</v>
+        <v>468</v>
       </c>
       <c r="R20" s="67"/>
       <c r="S20" s="67" t="s">
-        <v>451</v>
+        <v>469</v>
       </c>
       <c r="T20" s="67"/>
       <c r="U20" s="67"/>
@@ -14152,7 +14350,7 @@
       <c r="Z20" s="67"/>
       <c r="AA20" s="67"/>
       <c r="AB20" s="67" t="s">
-        <v>444</v>
+        <v>462</v>
       </c>
       <c r="AC20" s="67"/>
       <c r="AD20" s="67"/>
@@ -14165,14 +14363,14 @@
         <v>284</v>
       </c>
       <c r="AK20" s="67" t="s">
-        <v>452</v>
+        <v>470</v>
       </c>
       <c r="AL20" s="67"/>
       <c r="AM20" s="67" t="s">
-        <v>453</v>
+        <v>471</v>
       </c>
       <c r="AN20" s="67" t="s">
-        <v>454</v>
+        <v>472</v>
       </c>
       <c r="AO20" s="67"/>
       <c r="AP20" s="67"/>
@@ -14191,21 +14389,21 @@
       <c r="I21" s="67"/>
       <c r="J21" s="67"/>
       <c r="K21" s="69" t="s">
-        <v>455</v>
+        <v>473</v>
       </c>
       <c r="L21" s="69" t="s">
-        <v>455</v>
+        <v>473</v>
       </c>
       <c r="M21" s="67"/>
       <c r="N21" s="67"/>
       <c r="O21" s="68"/>
       <c r="P21" s="67"/>
       <c r="Q21" s="67" t="s">
-        <v>456</v>
+        <v>474</v>
       </c>
       <c r="R21" s="67"/>
       <c r="S21" s="67" t="s">
-        <v>457</v>
+        <v>475</v>
       </c>
       <c r="T21" s="67"/>
       <c r="U21" s="67"/>
@@ -14216,7 +14414,7 @@
       <c r="Z21" s="67"/>
       <c r="AA21" s="67"/>
       <c r="AB21" s="67" t="s">
-        <v>458</v>
+        <v>476</v>
       </c>
       <c r="AC21" s="67"/>
       <c r="AD21" s="67"/>
@@ -14226,14 +14424,14 @@
       <c r="AH21" s="67"/>
       <c r="AI21" s="67"/>
       <c r="AJ21" s="67" t="s">
-        <v>459</v>
+        <v>477</v>
       </c>
       <c r="AK21" s="67" t="s">
-        <v>460</v>
+        <v>478</v>
       </c>
       <c r="AL21" s="67"/>
       <c r="AM21" s="67" t="s">
-        <v>461</v>
+        <v>479</v>
       </c>
       <c r="AN21" s="67" t="s">
         <v>222</v>
@@ -14255,21 +14453,21 @@
       <c r="I22" s="67"/>
       <c r="J22" s="67"/>
       <c r="K22" s="67" t="s">
-        <v>462</v>
+        <v>480</v>
       </c>
       <c r="L22" s="67" t="s">
-        <v>462</v>
+        <v>480</v>
       </c>
       <c r="M22" s="67"/>
       <c r="N22" s="67"/>
       <c r="O22" s="68"/>
       <c r="P22" s="67"/>
       <c r="Q22" s="67" t="s">
-        <v>463</v>
+        <v>481</v>
       </c>
       <c r="R22" s="67"/>
       <c r="S22" s="67" t="s">
-        <v>464</v>
+        <v>482</v>
       </c>
       <c r="T22" s="67"/>
       <c r="U22" s="67"/>
@@ -14290,17 +14488,17 @@
       <c r="AH22" s="67"/>
       <c r="AI22" s="67"/>
       <c r="AJ22" s="67" t="s">
-        <v>465</v>
+        <v>483</v>
       </c>
       <c r="AK22" s="67" t="s">
-        <v>466</v>
+        <v>484</v>
       </c>
       <c r="AL22" s="67"/>
       <c r="AM22" s="67" t="s">
-        <v>467</v>
+        <v>485</v>
       </c>
       <c r="AN22" s="67" t="s">
-        <v>468</v>
+        <v>486</v>
       </c>
       <c r="AO22" s="67"/>
       <c r="AP22" s="67"/>
@@ -14319,21 +14517,21 @@
       <c r="I23" s="67"/>
       <c r="J23" s="67"/>
       <c r="K23" s="67" t="s">
-        <v>469</v>
+        <v>487</v>
       </c>
       <c r="L23" s="67" t="s">
-        <v>469</v>
+        <v>487</v>
       </c>
       <c r="M23" s="67"/>
       <c r="N23" s="67"/>
       <c r="O23" s="68"/>
       <c r="P23" s="67"/>
       <c r="Q23" s="67" t="s">
-        <v>470</v>
+        <v>488</v>
       </c>
       <c r="R23" s="67"/>
       <c r="S23" s="67" t="s">
-        <v>471</v>
+        <v>489</v>
       </c>
       <c r="T23" s="70"/>
       <c r="U23" s="67"/>
@@ -14344,7 +14542,7 @@
       <c r="Z23" s="67"/>
       <c r="AA23" s="67"/>
       <c r="AB23" s="67" t="s">
-        <v>472</v>
+        <v>490</v>
       </c>
       <c r="AC23" s="67"/>
       <c r="AD23" s="67"/>
@@ -14354,17 +14552,17 @@
       <c r="AH23" s="67"/>
       <c r="AI23" s="67"/>
       <c r="AJ23" s="67" t="s">
-        <v>473</v>
+        <v>491</v>
       </c>
       <c r="AK23" s="67" t="s">
-        <v>474</v>
+        <v>492</v>
       </c>
       <c r="AL23" s="67"/>
       <c r="AM23" s="67" t="s">
-        <v>475</v>
+        <v>493</v>
       </c>
       <c r="AN23" s="67" t="s">
-        <v>476</v>
+        <v>494</v>
       </c>
       <c r="AO23" s="67"/>
       <c r="AP23" s="67"/>
@@ -14383,21 +14581,21 @@
       <c r="I24" s="67"/>
       <c r="J24" s="67"/>
       <c r="K24" s="67" t="s">
-        <v>477</v>
+        <v>495</v>
       </c>
       <c r="L24" s="67" t="s">
-        <v>477</v>
+        <v>495</v>
       </c>
       <c r="M24" s="67"/>
       <c r="N24" s="67"/>
       <c r="O24" s="68"/>
       <c r="P24" s="67"/>
       <c r="Q24" s="67" t="s">
-        <v>478</v>
+        <v>496</v>
       </c>
       <c r="R24" s="67"/>
       <c r="S24" s="67" t="s">
-        <v>479</v>
+        <v>497</v>
       </c>
       <c r="T24" s="70"/>
       <c r="U24" s="67"/>
@@ -14408,7 +14606,7 @@
       <c r="Z24" s="67"/>
       <c r="AA24" s="67"/>
       <c r="AB24" s="67" t="s">
-        <v>480</v>
+        <v>498</v>
       </c>
       <c r="AC24" s="67"/>
       <c r="AD24" s="67"/>
@@ -14418,17 +14616,17 @@
       <c r="AH24" s="67"/>
       <c r="AI24" s="67"/>
       <c r="AJ24" s="67" t="s">
-        <v>481</v>
+        <v>499</v>
       </c>
       <c r="AK24" s="67" t="s">
-        <v>482</v>
+        <v>500</v>
       </c>
       <c r="AL24" s="67"/>
       <c r="AM24" s="67" t="s">
-        <v>483</v>
+        <v>501</v>
       </c>
       <c r="AN24" s="67" t="s">
-        <v>484</v>
+        <v>502</v>
       </c>
       <c r="AO24" s="67"/>
       <c r="AP24" s="67"/>
@@ -14447,21 +14645,21 @@
       <c r="I25" s="67"/>
       <c r="J25" s="67"/>
       <c r="K25" s="67" t="s">
-        <v>485</v>
+        <v>503</v>
       </c>
       <c r="L25" s="67" t="s">
-        <v>485</v>
+        <v>503</v>
       </c>
       <c r="M25" s="67"/>
       <c r="N25" s="67"/>
       <c r="O25" s="68"/>
       <c r="P25" s="67"/>
       <c r="Q25" s="67" t="s">
-        <v>486</v>
+        <v>504</v>
       </c>
       <c r="R25" s="67"/>
       <c r="S25" s="67" t="s">
-        <v>487</v>
+        <v>505</v>
       </c>
       <c r="T25" s="70"/>
       <c r="U25" s="67"/>
@@ -14472,7 +14670,7 @@
       <c r="Z25" s="67"/>
       <c r="AA25" s="67"/>
       <c r="AB25" s="67" t="s">
-        <v>488</v>
+        <v>506</v>
       </c>
       <c r="AC25" s="67"/>
       <c r="AD25" s="67"/>
@@ -14482,14 +14680,14 @@
       <c r="AH25" s="67"/>
       <c r="AI25" s="67"/>
       <c r="AJ25" s="67" t="s">
-        <v>489</v>
+        <v>507</v>
       </c>
       <c r="AK25" s="67" t="s">
-        <v>490</v>
+        <v>508</v>
       </c>
       <c r="AL25" s="67"/>
       <c r="AM25" s="67" t="s">
-        <v>491</v>
+        <v>509</v>
       </c>
       <c r="AN25" s="67"/>
       <c r="AO25" s="67"/>
@@ -14509,21 +14707,21 @@
       <c r="I26" s="67"/>
       <c r="J26" s="67"/>
       <c r="K26" s="67" t="s">
-        <v>492</v>
+        <v>510</v>
       </c>
       <c r="L26" s="67" t="s">
-        <v>492</v>
+        <v>510</v>
       </c>
       <c r="M26" s="67"/>
       <c r="N26" s="67"/>
       <c r="O26" s="68"/>
       <c r="P26" s="67"/>
       <c r="Q26" s="67" t="s">
-        <v>493</v>
+        <v>511</v>
       </c>
       <c r="R26" s="67"/>
       <c r="S26" s="67" t="s">
-        <v>494</v>
+        <v>512</v>
       </c>
       <c r="T26" s="70"/>
       <c r="U26" s="67"/>
@@ -14534,7 +14732,7 @@
       <c r="Z26" s="67"/>
       <c r="AA26" s="67"/>
       <c r="AB26" s="67" t="s">
-        <v>495</v>
+        <v>513</v>
       </c>
       <c r="AC26" s="67"/>
       <c r="AD26" s="67"/>
@@ -14544,14 +14742,14 @@
       <c r="AH26" s="67"/>
       <c r="AI26" s="67"/>
       <c r="AJ26" s="67" t="s">
-        <v>496</v>
+        <v>514</v>
       </c>
       <c r="AK26" s="67" t="s">
-        <v>497</v>
+        <v>515</v>
       </c>
       <c r="AL26" s="67"/>
       <c r="AM26" s="67" t="s">
-        <v>498</v>
+        <v>516</v>
       </c>
       <c r="AN26" s="67"/>
       <c r="AO26" s="67"/>
@@ -14571,21 +14769,21 @@
       <c r="I27" s="67"/>
       <c r="J27" s="67"/>
       <c r="K27" s="67" t="s">
-        <v>499</v>
+        <v>517</v>
       </c>
       <c r="L27" s="67" t="s">
-        <v>499</v>
+        <v>517</v>
       </c>
       <c r="M27" s="67"/>
       <c r="N27" s="67"/>
       <c r="O27" s="68"/>
       <c r="P27" s="67"/>
       <c r="Q27" s="67" t="s">
-        <v>500</v>
+        <v>518</v>
       </c>
       <c r="R27" s="67"/>
       <c r="S27" s="67" t="s">
-        <v>501</v>
+        <v>519</v>
       </c>
       <c r="T27" s="67"/>
       <c r="U27" s="67"/>
@@ -14596,7 +14794,7 @@
       <c r="Z27" s="67"/>
       <c r="AA27" s="67"/>
       <c r="AB27" s="67" t="s">
-        <v>502</v>
+        <v>520</v>
       </c>
       <c r="AC27" s="67"/>
       <c r="AD27" s="67"/>
@@ -14606,14 +14804,14 @@
       <c r="AH27" s="67"/>
       <c r="AI27" s="67"/>
       <c r="AJ27" s="67" t="s">
-        <v>503</v>
+        <v>521</v>
       </c>
       <c r="AK27" s="67" t="s">
-        <v>504</v>
+        <v>522</v>
       </c>
       <c r="AL27" s="67"/>
       <c r="AM27" s="67" t="s">
-        <v>505</v>
+        <v>523</v>
       </c>
       <c r="AN27" s="67"/>
       <c r="AO27" s="67"/>
@@ -14633,21 +14831,21 @@
       <c r="I28" s="67"/>
       <c r="J28" s="67"/>
       <c r="K28" s="67" t="s">
-        <v>506</v>
+        <v>524</v>
       </c>
       <c r="L28" s="67" t="s">
-        <v>506</v>
+        <v>524</v>
       </c>
       <c r="M28" s="67"/>
       <c r="N28" s="67"/>
       <c r="O28" s="68"/>
       <c r="P28" s="67"/>
       <c r="Q28" s="67" t="s">
-        <v>507</v>
+        <v>525</v>
       </c>
       <c r="R28" s="67"/>
       <c r="S28" s="67" t="s">
-        <v>508</v>
+        <v>526</v>
       </c>
       <c r="T28" s="70"/>
       <c r="U28" s="67"/>
@@ -14658,7 +14856,7 @@
       <c r="Z28" s="67"/>
       <c r="AA28" s="67"/>
       <c r="AB28" s="67" t="s">
-        <v>509</v>
+        <v>527</v>
       </c>
       <c r="AC28" s="67"/>
       <c r="AD28" s="67"/>
@@ -14668,14 +14866,14 @@
       <c r="AH28" s="67"/>
       <c r="AI28" s="67"/>
       <c r="AJ28" s="67" t="s">
-        <v>510</v>
+        <v>528</v>
       </c>
       <c r="AK28" s="67" t="s">
-        <v>511</v>
+        <v>529</v>
       </c>
       <c r="AL28" s="67"/>
       <c r="AM28" s="67" t="s">
-        <v>512</v>
+        <v>530</v>
       </c>
       <c r="AN28" s="67"/>
       <c r="AO28" s="67"/>
@@ -14695,21 +14893,21 @@
       <c r="I29" s="67"/>
       <c r="J29" s="67"/>
       <c r="K29" s="67" t="s">
-        <v>513</v>
+        <v>531</v>
       </c>
       <c r="L29" s="67" t="s">
-        <v>513</v>
+        <v>531</v>
       </c>
       <c r="M29" s="67"/>
       <c r="N29" s="67"/>
       <c r="O29" s="68"/>
       <c r="P29" s="67"/>
       <c r="Q29" s="67" t="s">
-        <v>514</v>
+        <v>532</v>
       </c>
       <c r="R29" s="67"/>
       <c r="S29" s="67" t="s">
-        <v>515</v>
+        <v>533</v>
       </c>
       <c r="T29" s="70"/>
       <c r="U29" s="67"/>
@@ -14730,14 +14928,14 @@
       <c r="AH29" s="67"/>
       <c r="AI29" s="67"/>
       <c r="AJ29" s="67" t="s">
-        <v>516</v>
+        <v>534</v>
       </c>
       <c r="AK29" s="67" t="s">
-        <v>517</v>
+        <v>535</v>
       </c>
       <c r="AL29" s="67"/>
       <c r="AM29" s="67" t="s">
-        <v>518</v>
+        <v>536</v>
       </c>
       <c r="AN29" s="67"/>
       <c r="AO29" s="67"/>
@@ -14757,21 +14955,21 @@
       <c r="I30" s="67"/>
       <c r="J30" s="67"/>
       <c r="K30" s="67" t="s">
-        <v>519</v>
+        <v>537</v>
       </c>
       <c r="L30" s="67" t="s">
-        <v>519</v>
+        <v>537</v>
       </c>
       <c r="M30" s="67"/>
       <c r="N30" s="67"/>
       <c r="O30" s="68"/>
       <c r="P30" s="67"/>
       <c r="Q30" s="67" t="s">
-        <v>520</v>
+        <v>538</v>
       </c>
       <c r="R30" s="67"/>
       <c r="S30" s="67" t="s">
-        <v>521</v>
+        <v>539</v>
       </c>
       <c r="T30" s="67"/>
       <c r="U30" s="67"/>
@@ -14790,14 +14988,14 @@
       <c r="AH30" s="67"/>
       <c r="AI30" s="67"/>
       <c r="AJ30" s="67" t="s">
-        <v>522</v>
+        <v>540</v>
       </c>
       <c r="AK30" s="67" t="s">
-        <v>523</v>
+        <v>541</v>
       </c>
       <c r="AL30" s="67"/>
       <c r="AM30" s="67" t="s">
-        <v>524</v>
+        <v>542</v>
       </c>
       <c r="AN30" s="67"/>
       <c r="AO30" s="67"/>
@@ -14817,21 +15015,21 @@
       <c r="I31" s="67"/>
       <c r="J31" s="67"/>
       <c r="K31" s="67" t="s">
-        <v>525</v>
+        <v>543</v>
       </c>
       <c r="L31" s="67" t="s">
-        <v>525</v>
+        <v>543</v>
       </c>
       <c r="M31" s="67"/>
       <c r="N31" s="67"/>
       <c r="O31" s="68"/>
       <c r="P31" s="67"/>
       <c r="Q31" s="67" t="s">
-        <v>526</v>
+        <v>544</v>
       </c>
       <c r="R31" s="67"/>
       <c r="S31" s="67" t="s">
-        <v>527</v>
+        <v>545</v>
       </c>
       <c r="T31" s="67"/>
       <c r="U31" s="67"/>
@@ -14850,10 +15048,10 @@
       <c r="AH31" s="67"/>
       <c r="AI31" s="67"/>
       <c r="AJ31" s="67" t="s">
-        <v>528</v>
+        <v>546</v>
       </c>
       <c r="AK31" s="67" t="s">
-        <v>529</v>
+        <v>547</v>
       </c>
       <c r="AL31" s="67"/>
       <c r="AM31" s="67" t="s">
@@ -14877,21 +15075,21 @@
       <c r="I32" s="67"/>
       <c r="J32" s="67"/>
       <c r="K32" s="67" t="s">
-        <v>530</v>
+        <v>548</v>
       </c>
       <c r="L32" s="67" t="s">
-        <v>530</v>
+        <v>548</v>
       </c>
       <c r="M32" s="67"/>
       <c r="N32" s="67"/>
       <c r="O32" s="68"/>
       <c r="P32" s="67"/>
       <c r="Q32" s="67" t="s">
-        <v>531</v>
+        <v>549</v>
       </c>
       <c r="R32" s="67"/>
       <c r="S32" s="67" t="s">
-        <v>532</v>
+        <v>550</v>
       </c>
       <c r="T32" s="67"/>
       <c r="U32" s="67"/>
@@ -14910,10 +15108,10 @@
       <c r="AH32" s="67"/>
       <c r="AI32" s="67"/>
       <c r="AJ32" s="67" t="s">
-        <v>533</v>
+        <v>551</v>
       </c>
       <c r="AK32" s="67" t="s">
-        <v>534</v>
+        <v>552</v>
       </c>
       <c r="AL32" s="67"/>
       <c r="AM32" s="67"/>
@@ -14935,21 +15133,21 @@
       <c r="I33" s="67"/>
       <c r="J33" s="67"/>
       <c r="K33" s="67" t="s">
-        <v>535</v>
+        <v>553</v>
       </c>
       <c r="L33" s="67" t="s">
-        <v>535</v>
+        <v>553</v>
       </c>
       <c r="M33" s="67"/>
       <c r="N33" s="67"/>
       <c r="O33" s="68"/>
       <c r="P33" s="67"/>
       <c r="Q33" s="67" t="s">
-        <v>536</v>
+        <v>554</v>
       </c>
       <c r="R33" s="67"/>
       <c r="S33" s="67" t="s">
-        <v>537</v>
+        <v>555</v>
       </c>
       <c r="T33" s="67"/>
       <c r="U33" s="67"/>
@@ -14968,10 +15166,10 @@
       <c r="AH33" s="67"/>
       <c r="AI33" s="67"/>
       <c r="AJ33" s="67" t="s">
-        <v>538</v>
+        <v>556</v>
       </c>
       <c r="AK33" s="67" t="s">
-        <v>539</v>
+        <v>557</v>
       </c>
       <c r="AL33" s="67"/>
       <c r="AM33" s="67"/>
@@ -14993,17 +15191,17 @@
       <c r="I34" s="67"/>
       <c r="J34" s="67"/>
       <c r="K34" s="67" t="s">
-        <v>540</v>
+        <v>558</v>
       </c>
       <c r="L34" s="67" t="s">
-        <v>540</v>
+        <v>558</v>
       </c>
       <c r="M34" s="67"/>
       <c r="N34" s="67"/>
       <c r="O34" s="68"/>
       <c r="P34" s="67"/>
       <c r="Q34" s="67" t="s">
-        <v>541</v>
+        <v>559</v>
       </c>
       <c r="R34" s="67"/>
       <c r="S34" s="67" t="s">
@@ -15029,7 +15227,7 @@
         <v>259</v>
       </c>
       <c r="AK34" s="67" t="s">
-        <v>542</v>
+        <v>560</v>
       </c>
       <c r="AL34" s="67"/>
       <c r="AM34" s="67"/>
@@ -15051,21 +15249,21 @@
       <c r="I35" s="67"/>
       <c r="J35" s="67"/>
       <c r="K35" s="67" t="s">
-        <v>543</v>
+        <v>561</v>
       </c>
       <c r="L35" s="67" t="s">
-        <v>543</v>
+        <v>561</v>
       </c>
       <c r="M35" s="67"/>
       <c r="N35" s="67"/>
       <c r="O35" s="68"/>
       <c r="P35" s="67"/>
       <c r="Q35" s="67" t="s">
-        <v>544</v>
+        <v>562</v>
       </c>
       <c r="R35" s="67"/>
       <c r="S35" s="67" t="s">
-        <v>545</v>
+        <v>563</v>
       </c>
       <c r="T35" s="67"/>
       <c r="U35" s="67"/>
@@ -15084,10 +15282,10 @@
       <c r="AH35" s="67"/>
       <c r="AI35" s="67"/>
       <c r="AJ35" s="67" t="s">
-        <v>546</v>
+        <v>564</v>
       </c>
       <c r="AK35" s="67" t="s">
-        <v>547</v>
+        <v>565</v>
       </c>
       <c r="AL35" s="67"/>
       <c r="AM35" s="67"/>
@@ -15109,21 +15307,21 @@
       <c r="I36" s="67"/>
       <c r="J36" s="67"/>
       <c r="K36" s="67" t="s">
-        <v>548</v>
+        <v>566</v>
       </c>
       <c r="L36" s="67" t="s">
-        <v>548</v>
+        <v>566</v>
       </c>
       <c r="M36" s="67"/>
       <c r="N36" s="67"/>
       <c r="O36" s="68"/>
       <c r="P36" s="67"/>
       <c r="Q36" s="67" t="s">
-        <v>549</v>
+        <v>567</v>
       </c>
       <c r="R36" s="67"/>
       <c r="S36" s="67" t="s">
-        <v>550</v>
+        <v>568</v>
       </c>
       <c r="T36" s="67"/>
       <c r="U36" s="67"/>
@@ -15142,10 +15340,10 @@
       <c r="AH36" s="67"/>
       <c r="AI36" s="67"/>
       <c r="AJ36" s="67" t="s">
-        <v>551</v>
+        <v>569</v>
       </c>
       <c r="AK36" s="67" t="s">
-        <v>552</v>
+        <v>570</v>
       </c>
       <c r="AL36" s="67"/>
       <c r="AM36" s="67"/>
@@ -15167,21 +15365,21 @@
       <c r="I37" s="67"/>
       <c r="J37" s="67"/>
       <c r="K37" s="67" t="s">
-        <v>553</v>
+        <v>571</v>
       </c>
       <c r="L37" s="67" t="s">
-        <v>553</v>
+        <v>571</v>
       </c>
       <c r="M37" s="67"/>
       <c r="N37" s="67"/>
       <c r="O37" s="68"/>
       <c r="P37" s="67"/>
       <c r="Q37" s="67" t="s">
-        <v>554</v>
+        <v>572</v>
       </c>
       <c r="R37" s="67"/>
       <c r="S37" s="67" t="s">
-        <v>555</v>
+        <v>573</v>
       </c>
       <c r="T37" s="67"/>
       <c r="U37" s="67"/>
@@ -15200,10 +15398,10 @@
       <c r="AH37" s="67"/>
       <c r="AI37" s="67"/>
       <c r="AJ37" s="67" t="s">
-        <v>556</v>
+        <v>574</v>
       </c>
       <c r="AK37" s="67" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="AL37" s="67"/>
       <c r="AM37" s="67"/>
@@ -15225,21 +15423,21 @@
       <c r="I38" s="67"/>
       <c r="J38" s="67"/>
       <c r="K38" s="67" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
       <c r="L38" s="67" t="s">
-        <v>558</v>
+        <v>576</v>
       </c>
       <c r="M38" s="67"/>
       <c r="N38" s="67"/>
       <c r="O38" s="68"/>
       <c r="P38" s="67"/>
       <c r="Q38" s="67" t="s">
-        <v>559</v>
+        <v>577</v>
       </c>
       <c r="R38" s="67"/>
       <c r="S38" s="67" t="s">
-        <v>560</v>
+        <v>578</v>
       </c>
       <c r="T38" s="67"/>
       <c r="U38" s="67"/>
@@ -15258,10 +15456,10 @@
       <c r="AH38" s="67"/>
       <c r="AI38" s="67"/>
       <c r="AJ38" s="67" t="s">
-        <v>561</v>
+        <v>579</v>
       </c>
       <c r="AK38" s="67" t="s">
-        <v>542</v>
+        <v>560</v>
       </c>
       <c r="AL38" s="67"/>
       <c r="AM38" s="67"/>
@@ -15283,21 +15481,21 @@
       <c r="I39" s="67"/>
       <c r="J39" s="67"/>
       <c r="K39" s="67" t="s">
-        <v>562</v>
+        <v>580</v>
       </c>
       <c r="L39" s="67" t="s">
-        <v>562</v>
+        <v>580</v>
       </c>
       <c r="M39" s="67"/>
       <c r="N39" s="67"/>
       <c r="O39" s="68"/>
       <c r="P39" s="67"/>
       <c r="Q39" s="67" t="s">
-        <v>563</v>
+        <v>581</v>
       </c>
       <c r="R39" s="67"/>
       <c r="S39" s="67" t="s">
-        <v>564</v>
+        <v>582</v>
       </c>
       <c r="T39" s="67"/>
       <c r="U39" s="67"/>
@@ -15316,10 +15514,10 @@
       <c r="AH39" s="67"/>
       <c r="AI39" s="67"/>
       <c r="AJ39" s="67" t="s">
+        <v>583</v>
+      </c>
+      <c r="AK39" s="67" t="s">
         <v>565</v>
-      </c>
-      <c r="AK39" s="67" t="s">
-        <v>547</v>
       </c>
       <c r="AL39" s="67"/>
       <c r="AM39" s="67"/>
@@ -15341,21 +15539,21 @@
       <c r="I40" s="67"/>
       <c r="J40" s="67"/>
       <c r="K40" s="67" t="s">
-        <v>566</v>
+        <v>584</v>
       </c>
       <c r="L40" s="67" t="s">
-        <v>566</v>
+        <v>584</v>
       </c>
       <c r="M40" s="67"/>
       <c r="N40" s="67"/>
       <c r="O40" s="68"/>
       <c r="P40" s="67"/>
       <c r="Q40" s="67" t="s">
-        <v>567</v>
+        <v>585</v>
       </c>
       <c r="R40" s="67"/>
       <c r="S40" s="67" t="s">
-        <v>568</v>
+        <v>586</v>
       </c>
       <c r="T40" s="67"/>
       <c r="U40" s="67"/>
@@ -15374,10 +15572,10 @@
       <c r="AH40" s="67"/>
       <c r="AI40" s="67"/>
       <c r="AJ40" s="67" t="s">
-        <v>569</v>
+        <v>587</v>
       </c>
       <c r="AK40" s="67" t="s">
-        <v>552</v>
+        <v>570</v>
       </c>
       <c r="AL40" s="67"/>
       <c r="AM40" s="67"/>
@@ -15399,21 +15597,21 @@
       <c r="I41" s="67"/>
       <c r="J41" s="67"/>
       <c r="K41" s="67" t="s">
-        <v>570</v>
+        <v>588</v>
       </c>
       <c r="L41" s="67" t="s">
-        <v>570</v>
+        <v>588</v>
       </c>
       <c r="M41" s="67"/>
       <c r="N41" s="67"/>
       <c r="O41" s="68"/>
       <c r="P41" s="67"/>
       <c r="Q41" s="67" t="s">
-        <v>571</v>
+        <v>589</v>
       </c>
       <c r="R41" s="67"/>
       <c r="S41" s="67" t="s">
-        <v>572</v>
+        <v>590</v>
       </c>
       <c r="T41" s="67"/>
       <c r="U41" s="67"/>
@@ -15432,10 +15630,10 @@
       <c r="AH41" s="67"/>
       <c r="AI41" s="67"/>
       <c r="AJ41" s="67" t="s">
-        <v>573</v>
+        <v>591</v>
       </c>
       <c r="AK41" s="67" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="AL41" s="67"/>
       <c r="AM41" s="67"/>
@@ -15457,21 +15655,21 @@
       <c r="I42" s="67"/>
       <c r="J42" s="67"/>
       <c r="K42" s="67" t="s">
-        <v>574</v>
+        <v>592</v>
       </c>
       <c r="L42" s="67" t="s">
-        <v>574</v>
+        <v>592</v>
       </c>
       <c r="M42" s="67"/>
       <c r="N42" s="67"/>
       <c r="O42" s="68"/>
       <c r="P42" s="67"/>
       <c r="Q42" s="67" t="s">
-        <v>575</v>
+        <v>593</v>
       </c>
       <c r="R42" s="67"/>
       <c r="S42" s="67" t="s">
-        <v>576</v>
+        <v>594</v>
       </c>
       <c r="T42" s="67"/>
       <c r="U42" s="67"/>
@@ -15490,10 +15688,10 @@
       <c r="AH42" s="67"/>
       <c r="AI42" s="67"/>
       <c r="AJ42" s="67" t="s">
-        <v>577</v>
+        <v>595</v>
       </c>
       <c r="AK42" s="67" t="s">
-        <v>542</v>
+        <v>560</v>
       </c>
       <c r="AL42" s="67"/>
       <c r="AM42" s="67"/>
@@ -15515,21 +15713,21 @@
       <c r="I43" s="67"/>
       <c r="J43" s="67"/>
       <c r="K43" s="67" t="s">
-        <v>578</v>
+        <v>596</v>
       </c>
       <c r="L43" s="67" t="s">
-        <v>578</v>
+        <v>596</v>
       </c>
       <c r="M43" s="67"/>
       <c r="N43" s="67"/>
       <c r="O43" s="68"/>
       <c r="P43" s="67"/>
       <c r="Q43" s="67" t="s">
-        <v>579</v>
+        <v>597</v>
       </c>
       <c r="R43" s="67"/>
       <c r="S43" s="67" t="s">
-        <v>580</v>
+        <v>598</v>
       </c>
       <c r="T43" s="67"/>
       <c r="U43" s="67"/>
@@ -15548,10 +15746,10 @@
       <c r="AH43" s="67"/>
       <c r="AI43" s="67"/>
       <c r="AJ43" s="67" t="s">
-        <v>581</v>
+        <v>599</v>
       </c>
       <c r="AK43" s="67" t="s">
-        <v>547</v>
+        <v>565</v>
       </c>
       <c r="AL43" s="67"/>
       <c r="AM43" s="67"/>
@@ -15573,21 +15771,21 @@
       <c r="I44" s="67"/>
       <c r="J44" s="67"/>
       <c r="K44" s="67" t="s">
-        <v>582</v>
+        <v>600</v>
       </c>
       <c r="L44" s="67" t="s">
-        <v>582</v>
+        <v>600</v>
       </c>
       <c r="M44" s="67"/>
       <c r="N44" s="67"/>
       <c r="O44" s="68"/>
       <c r="P44" s="67"/>
       <c r="Q44" s="67" t="s">
-        <v>583</v>
+        <v>601</v>
       </c>
       <c r="R44" s="67"/>
       <c r="S44" s="67" t="s">
-        <v>584</v>
+        <v>602</v>
       </c>
       <c r="T44" s="67"/>
       <c r="U44" s="67"/>
@@ -15606,10 +15804,10 @@
       <c r="AH44" s="67"/>
       <c r="AI44" s="67"/>
       <c r="AJ44" s="67" t="s">
-        <v>585</v>
+        <v>603</v>
       </c>
       <c r="AK44" s="67" t="s">
-        <v>552</v>
+        <v>570</v>
       </c>
       <c r="AL44" s="67"/>
       <c r="AM44" s="67"/>
@@ -15631,21 +15829,21 @@
       <c r="I45" s="67"/>
       <c r="J45" s="67"/>
       <c r="K45" s="67" t="s">
-        <v>586</v>
+        <v>604</v>
       </c>
       <c r="L45" s="67" t="s">
-        <v>586</v>
+        <v>604</v>
       </c>
       <c r="M45" s="67"/>
       <c r="N45" s="67"/>
       <c r="O45" s="68"/>
       <c r="P45" s="67"/>
       <c r="Q45" s="67" t="s">
-        <v>587</v>
+        <v>605</v>
       </c>
       <c r="R45" s="67"/>
       <c r="S45" s="67" t="s">
-        <v>588</v>
+        <v>606</v>
       </c>
       <c r="T45" s="67"/>
       <c r="U45" s="67"/>
@@ -15664,10 +15862,10 @@
       <c r="AH45" s="67"/>
       <c r="AI45" s="67"/>
       <c r="AJ45" s="67" t="s">
-        <v>589</v>
+        <v>607</v>
       </c>
       <c r="AK45" s="67" t="s">
-        <v>557</v>
+        <v>575</v>
       </c>
       <c r="AL45" s="67"/>
       <c r="AM45" s="67"/>
@@ -15689,21 +15887,21 @@
       <c r="I46" s="67"/>
       <c r="J46" s="67"/>
       <c r="K46" s="67" t="s">
-        <v>590</v>
+        <v>608</v>
       </c>
       <c r="L46" s="67" t="s">
-        <v>590</v>
+        <v>608</v>
       </c>
       <c r="M46" s="67"/>
       <c r="N46" s="67"/>
       <c r="O46" s="68"/>
       <c r="P46" s="67"/>
       <c r="Q46" s="67" t="s">
-        <v>591</v>
+        <v>609</v>
       </c>
       <c r="R46" s="67"/>
       <c r="S46" s="67" t="s">
-        <v>592</v>
+        <v>610</v>
       </c>
       <c r="T46" s="67"/>
       <c r="U46" s="67"/>
@@ -15722,10 +15920,10 @@
       <c r="AH46" s="67"/>
       <c r="AI46" s="67"/>
       <c r="AJ46" s="67" t="s">
-        <v>593</v>
+        <v>611</v>
       </c>
       <c r="AK46" s="67" t="s">
-        <v>594</v>
+        <v>612</v>
       </c>
       <c r="AL46" s="67"/>
       <c r="AM46" s="67"/>
@@ -15747,21 +15945,21 @@
       <c r="I47" s="67"/>
       <c r="J47" s="67"/>
       <c r="K47" s="67" t="s">
-        <v>595</v>
+        <v>613</v>
       </c>
       <c r="L47" s="67" t="s">
-        <v>595</v>
+        <v>613</v>
       </c>
       <c r="M47" s="67"/>
       <c r="N47" s="67"/>
       <c r="O47" s="68"/>
       <c r="P47" s="67"/>
       <c r="Q47" s="67" t="s">
-        <v>596</v>
+        <v>614</v>
       </c>
       <c r="R47" s="67"/>
       <c r="S47" s="67" t="s">
-        <v>597</v>
+        <v>615</v>
       </c>
       <c r="T47" s="67"/>
       <c r="U47" s="67"/>
@@ -15780,10 +15978,10 @@
       <c r="AH47" s="67"/>
       <c r="AI47" s="67"/>
       <c r="AJ47" s="67" t="s">
-        <v>598</v>
+        <v>616</v>
       </c>
       <c r="AK47" s="67" t="s">
-        <v>599</v>
+        <v>617</v>
       </c>
       <c r="AL47" s="67"/>
       <c r="AM47" s="67"/>
@@ -15805,21 +16003,21 @@
       <c r="I48" s="67"/>
       <c r="J48" s="67"/>
       <c r="K48" s="67" t="s">
-        <v>600</v>
+        <v>618</v>
       </c>
       <c r="L48" s="67" t="s">
-        <v>600</v>
+        <v>618</v>
       </c>
       <c r="M48" s="67"/>
       <c r="N48" s="67"/>
       <c r="O48" s="68"/>
       <c r="P48" s="67"/>
       <c r="Q48" s="67" t="s">
-        <v>601</v>
+        <v>619</v>
       </c>
       <c r="R48" s="67"/>
       <c r="S48" s="67" t="s">
-        <v>602</v>
+        <v>620</v>
       </c>
       <c r="T48" s="67"/>
       <c r="U48" s="67"/>
@@ -15838,10 +16036,10 @@
       <c r="AH48" s="67"/>
       <c r="AI48" s="67"/>
       <c r="AJ48" s="67" t="s">
-        <v>603</v>
+        <v>621</v>
       </c>
       <c r="AK48" s="67" t="s">
-        <v>604</v>
+        <v>622</v>
       </c>
       <c r="AL48" s="67"/>
       <c r="AM48" s="67"/>
@@ -15863,21 +16061,21 @@
       <c r="I49" s="67"/>
       <c r="J49" s="67"/>
       <c r="K49" s="67" t="s">
-        <v>605</v>
+        <v>623</v>
       </c>
       <c r="L49" s="67" t="s">
-        <v>605</v>
+        <v>623</v>
       </c>
       <c r="M49" s="67"/>
       <c r="N49" s="67"/>
       <c r="O49" s="68"/>
       <c r="P49" s="67"/>
       <c r="Q49" s="67" t="s">
-        <v>606</v>
+        <v>624</v>
       </c>
       <c r="R49" s="67"/>
       <c r="S49" s="67" t="s">
-        <v>607</v>
+        <v>625</v>
       </c>
       <c r="T49" s="67"/>
       <c r="U49" s="67"/>
@@ -15896,10 +16094,10 @@
       <c r="AH49" s="67"/>
       <c r="AI49" s="67"/>
       <c r="AJ49" s="67" t="s">
-        <v>608</v>
+        <v>626</v>
       </c>
       <c r="AK49" s="67" t="s">
-        <v>609</v>
+        <v>627</v>
       </c>
       <c r="AL49" s="67"/>
       <c r="AM49" s="67"/>
@@ -15921,21 +16119,21 @@
       <c r="I50" s="67"/>
       <c r="J50" s="67"/>
       <c r="K50" s="67" t="s">
-        <v>610</v>
+        <v>628</v>
       </c>
       <c r="L50" s="67" t="s">
-        <v>610</v>
+        <v>628</v>
       </c>
       <c r="M50" s="67"/>
       <c r="N50" s="67"/>
       <c r="O50" s="68"/>
       <c r="P50" s="67"/>
       <c r="Q50" s="67" t="s">
-        <v>611</v>
+        <v>629</v>
       </c>
       <c r="R50" s="67"/>
       <c r="S50" s="67" t="s">
-        <v>612</v>
+        <v>630</v>
       </c>
       <c r="T50" s="67"/>
       <c r="U50" s="67"/>
@@ -15954,10 +16152,10 @@
       <c r="AH50" s="67"/>
       <c r="AI50" s="67"/>
       <c r="AJ50" s="67" t="s">
-        <v>613</v>
+        <v>631</v>
       </c>
       <c r="AK50" s="67" t="s">
-        <v>614</v>
+        <v>632</v>
       </c>
       <c r="AL50" s="67"/>
       <c r="AM50" s="67"/>
@@ -15979,17 +16177,17 @@
       <c r="I51" s="67"/>
       <c r="J51" s="67"/>
       <c r="K51" s="67" t="s">
-        <v>615</v>
+        <v>633</v>
       </c>
       <c r="L51" s="67" t="s">
-        <v>616</v>
+        <v>634</v>
       </c>
       <c r="M51" s="67"/>
       <c r="N51" s="67"/>
       <c r="O51" s="68"/>
       <c r="P51" s="67"/>
       <c r="Q51" s="67" t="s">
-        <v>617</v>
+        <v>635</v>
       </c>
       <c r="R51" s="67"/>
       <c r="S51" s="67" t="s">
@@ -16012,10 +16210,10 @@
       <c r="AH51" s="67"/>
       <c r="AI51" s="67"/>
       <c r="AJ51" s="67" t="s">
-        <v>618</v>
+        <v>636</v>
       </c>
       <c r="AK51" s="67" t="s">
-        <v>619</v>
+        <v>637</v>
       </c>
       <c r="AL51" s="67"/>
       <c r="AM51" s="67"/>
@@ -16037,17 +16235,17 @@
       <c r="I52" s="67"/>
       <c r="J52" s="67"/>
       <c r="K52" s="67" t="s">
-        <v>620</v>
+        <v>638</v>
       </c>
       <c r="L52" s="67" t="s">
-        <v>621</v>
+        <v>639</v>
       </c>
       <c r="M52" s="67"/>
       <c r="N52" s="67"/>
       <c r="O52" s="68"/>
       <c r="P52" s="67"/>
       <c r="Q52" s="67" t="s">
-        <v>622</v>
+        <v>640</v>
       </c>
       <c r="R52" s="67"/>
       <c r="S52" s="67"/>
@@ -16068,10 +16266,10 @@
       <c r="AH52" s="67"/>
       <c r="AI52" s="67"/>
       <c r="AJ52" s="67" t="s">
-        <v>623</v>
+        <v>641</v>
       </c>
       <c r="AK52" s="67" t="s">
-        <v>624</v>
+        <v>642</v>
       </c>
       <c r="AL52" s="67"/>
       <c r="AM52" s="67"/>
@@ -16093,10 +16291,10 @@
       <c r="I53" s="67"/>
       <c r="J53" s="67"/>
       <c r="K53" s="67" t="s">
-        <v>625</v>
+        <v>643</v>
       </c>
       <c r="L53" s="67" t="s">
-        <v>620</v>
+        <v>638</v>
       </c>
       <c r="M53" s="67"/>
       <c r="N53" s="67"/>
@@ -16124,10 +16322,10 @@
       <c r="AH53" s="67"/>
       <c r="AI53" s="67"/>
       <c r="AJ53" s="67" t="s">
-        <v>626</v>
+        <v>644</v>
       </c>
       <c r="AK53" s="67" t="s">
-        <v>627</v>
+        <v>645</v>
       </c>
       <c r="AL53" s="67"/>
       <c r="AM53" s="67"/>
@@ -16149,17 +16347,17 @@
       <c r="I54" s="67"/>
       <c r="J54" s="67"/>
       <c r="K54" s="67" t="s">
-        <v>628</v>
+        <v>646</v>
       </c>
       <c r="L54" s="67" t="s">
-        <v>625</v>
+        <v>643</v>
       </c>
       <c r="M54" s="67"/>
       <c r="N54" s="67"/>
       <c r="O54" s="68"/>
       <c r="P54" s="67"/>
       <c r="Q54" s="67" t="s">
-        <v>629</v>
+        <v>647</v>
       </c>
       <c r="R54" s="67"/>
       <c r="S54" s="67"/>
@@ -16180,10 +16378,10 @@
       <c r="AH54" s="67"/>
       <c r="AI54" s="67"/>
       <c r="AJ54" s="67" t="s">
-        <v>630</v>
+        <v>648</v>
       </c>
       <c r="AK54" s="67" t="s">
-        <v>631</v>
+        <v>649</v>
       </c>
       <c r="AL54" s="67"/>
       <c r="AM54" s="67"/>
@@ -16205,17 +16403,17 @@
       <c r="I55" s="67"/>
       <c r="J55" s="67"/>
       <c r="K55" s="67" t="s">
-        <v>632</v>
+        <v>650</v>
       </c>
       <c r="L55" s="67" t="s">
-        <v>628</v>
+        <v>646</v>
       </c>
       <c r="M55" s="67"/>
       <c r="N55" s="67"/>
       <c r="O55" s="68"/>
       <c r="P55" s="67"/>
       <c r="Q55" s="67" t="s">
-        <v>633</v>
+        <v>651</v>
       </c>
       <c r="R55" s="67"/>
       <c r="S55" s="67"/>
@@ -16236,10 +16434,10 @@
       <c r="AH55" s="67"/>
       <c r="AI55" s="67"/>
       <c r="AJ55" s="67" t="s">
-        <v>634</v>
+        <v>652</v>
       </c>
       <c r="AK55" s="67" t="s">
-        <v>635</v>
+        <v>653</v>
       </c>
       <c r="AL55" s="67"/>
       <c r="AM55" s="67"/>
@@ -16261,17 +16459,17 @@
       <c r="I56" s="67"/>
       <c r="J56" s="67"/>
       <c r="K56" s="67" t="s">
-        <v>636</v>
+        <v>654</v>
       </c>
       <c r="L56" s="67" t="s">
-        <v>632</v>
+        <v>650</v>
       </c>
       <c r="M56" s="67"/>
       <c r="N56" s="67"/>
       <c r="O56" s="68"/>
       <c r="P56" s="67"/>
       <c r="Q56" s="67" t="s">
-        <v>637</v>
+        <v>655</v>
       </c>
       <c r="R56" s="67"/>
       <c r="S56" s="67"/>
@@ -16292,10 +16490,10 @@
       <c r="AH56" s="67"/>
       <c r="AI56" s="67"/>
       <c r="AJ56" s="67" t="s">
-        <v>638</v>
+        <v>656</v>
       </c>
       <c r="AK56" s="67" t="s">
-        <v>639</v>
+        <v>657</v>
       </c>
       <c r="AL56" s="67"/>
       <c r="AM56" s="67"/>
@@ -16317,17 +16515,17 @@
       <c r="I57" s="67"/>
       <c r="J57" s="67"/>
       <c r="K57" s="67" t="s">
-        <v>640</v>
+        <v>658</v>
       </c>
       <c r="L57" s="67" t="s">
-        <v>636</v>
+        <v>654</v>
       </c>
       <c r="M57" s="67"/>
       <c r="N57" s="67"/>
       <c r="O57" s="68"/>
       <c r="P57" s="67"/>
       <c r="Q57" s="67" t="s">
-        <v>641</v>
+        <v>659</v>
       </c>
       <c r="R57" s="67"/>
       <c r="S57" s="67"/>
@@ -16348,10 +16546,10 @@
       <c r="AH57" s="67"/>
       <c r="AI57" s="67"/>
       <c r="AJ57" s="67" t="s">
-        <v>642</v>
+        <v>660</v>
       </c>
       <c r="AK57" s="67" t="s">
-        <v>643</v>
+        <v>661</v>
       </c>
       <c r="AL57" s="67"/>
       <c r="AM57" s="67"/>
@@ -16373,17 +16571,17 @@
       <c r="I58" s="67"/>
       <c r="J58" s="67"/>
       <c r="K58" s="67" t="s">
-        <v>644</v>
+        <v>662</v>
       </c>
       <c r="L58" s="67" t="s">
-        <v>640</v>
+        <v>658</v>
       </c>
       <c r="M58" s="67"/>
       <c r="N58" s="67"/>
       <c r="O58" s="68"/>
       <c r="P58" s="67"/>
       <c r="Q58" s="67" t="s">
-        <v>645</v>
+        <v>663</v>
       </c>
       <c r="R58" s="67"/>
       <c r="S58" s="67"/>
@@ -16404,10 +16602,10 @@
       <c r="AH58" s="67"/>
       <c r="AI58" s="67"/>
       <c r="AJ58" s="67" t="s">
-        <v>646</v>
+        <v>664</v>
       </c>
       <c r="AK58" s="67" t="s">
-        <v>647</v>
+        <v>665</v>
       </c>
       <c r="AL58" s="67"/>
       <c r="AM58" s="67"/>
@@ -16429,10 +16627,10 @@
       <c r="I59" s="67"/>
       <c r="J59" s="67"/>
       <c r="K59" s="67" t="s">
-        <v>648</v>
+        <v>666</v>
       </c>
       <c r="L59" s="67" t="s">
-        <v>644</v>
+        <v>662</v>
       </c>
       <c r="M59" s="67"/>
       <c r="N59" s="67"/>
@@ -16460,10 +16658,10 @@
       <c r="AH59" s="67"/>
       <c r="AI59" s="67"/>
       <c r="AJ59" s="67" t="s">
-        <v>649</v>
+        <v>667</v>
       </c>
       <c r="AK59" s="67" t="s">
-        <v>650</v>
+        <v>668</v>
       </c>
       <c r="AL59" s="67"/>
       <c r="AM59" s="67"/>
@@ -16485,10 +16683,10 @@
       <c r="I60" s="67"/>
       <c r="J60" s="67"/>
       <c r="K60" s="67" t="s">
-        <v>651</v>
+        <v>669</v>
       </c>
       <c r="L60" s="67" t="s">
-        <v>648</v>
+        <v>666</v>
       </c>
       <c r="M60" s="67"/>
       <c r="N60" s="67"/>
@@ -16513,10 +16711,10 @@
       <c r="AH60" s="67"/>
       <c r="AI60" s="67"/>
       <c r="AJ60" s="67" t="s">
-        <v>652</v>
+        <v>670</v>
       </c>
       <c r="AK60" s="67" t="s">
-        <v>653</v>
+        <v>671</v>
       </c>
       <c r="AL60" s="67"/>
       <c r="AM60" s="67"/>
@@ -16538,10 +16736,10 @@
       <c r="I61" s="67"/>
       <c r="J61" s="67"/>
       <c r="K61" s="67" t="s">
-        <v>654</v>
+        <v>672</v>
       </c>
       <c r="L61" s="67" t="s">
-        <v>651</v>
+        <v>669</v>
       </c>
       <c r="M61" s="67"/>
       <c r="N61" s="67"/>
@@ -16566,10 +16764,10 @@
       <c r="AH61" s="67"/>
       <c r="AI61" s="67"/>
       <c r="AJ61" s="67" t="s">
-        <v>655</v>
+        <v>673</v>
       </c>
       <c r="AK61" s="67" t="s">
-        <v>656</v>
+        <v>674</v>
       </c>
       <c r="AL61" s="67"/>
       <c r="AM61" s="67"/>
@@ -16591,10 +16789,10 @@
       <c r="I62" s="67"/>
       <c r="J62" s="67"/>
       <c r="K62" s="67" t="s">
-        <v>657</v>
+        <v>675</v>
       </c>
       <c r="L62" s="67" t="s">
-        <v>654</v>
+        <v>672</v>
       </c>
       <c r="M62" s="67"/>
       <c r="N62" s="67"/>
@@ -16620,10 +16818,10 @@
       <c r="AH62" s="67"/>
       <c r="AI62" s="67"/>
       <c r="AJ62" s="67" t="s">
-        <v>658</v>
+        <v>676</v>
       </c>
       <c r="AK62" s="67" t="s">
-        <v>659</v>
+        <v>677</v>
       </c>
       <c r="AL62" s="67"/>
       <c r="AM62" s="67"/>
@@ -16645,10 +16843,10 @@
       <c r="I63" s="67"/>
       <c r="J63" s="67"/>
       <c r="K63" s="67" t="s">
-        <v>621</v>
+        <v>639</v>
       </c>
       <c r="L63" s="67" t="s">
-        <v>657</v>
+        <v>675</v>
       </c>
       <c r="M63" s="67"/>
       <c r="N63" s="67"/>
@@ -16674,7 +16872,7 @@
       <c r="AH63" s="67"/>
       <c r="AI63" s="67"/>
       <c r="AJ63" s="67" t="s">
-        <v>660</v>
+        <v>678</v>
       </c>
       <c r="AK63" s="67" t="s">
         <v>139</v>
@@ -16699,10 +16897,10 @@
       <c r="I64" s="67"/>
       <c r="J64" s="67"/>
       <c r="K64" s="67" t="s">
-        <v>661</v>
+        <v>679</v>
       </c>
       <c r="L64" s="67" t="s">
-        <v>661</v>
+        <v>679</v>
       </c>
       <c r="M64" s="67"/>
       <c r="N64" s="67"/>
@@ -16728,10 +16926,10 @@
       <c r="AH64" s="67"/>
       <c r="AI64" s="67"/>
       <c r="AJ64" s="67" t="s">
-        <v>662</v>
+        <v>680</v>
       </c>
       <c r="AK64" s="67" t="s">
-        <v>663</v>
+        <v>681</v>
       </c>
       <c r="AL64" s="67"/>
       <c r="AM64" s="67"/>
@@ -16753,10 +16951,10 @@
       <c r="I65" s="67"/>
       <c r="J65" s="67"/>
       <c r="K65" s="67" t="s">
-        <v>664</v>
+        <v>682</v>
       </c>
       <c r="L65" s="67" t="s">
-        <v>664</v>
+        <v>682</v>
       </c>
       <c r="M65" s="67"/>
       <c r="N65" s="67"/>
@@ -16782,10 +16980,10 @@
       <c r="AH65" s="67"/>
       <c r="AI65" s="67"/>
       <c r="AJ65" s="67" t="s">
-        <v>665</v>
+        <v>683</v>
       </c>
       <c r="AK65" s="67" t="s">
-        <v>666</v>
+        <v>684</v>
       </c>
       <c r="AL65" s="67"/>
       <c r="AM65" s="67"/>
@@ -16807,10 +17005,10 @@
       <c r="I66" s="67"/>
       <c r="J66" s="67"/>
       <c r="K66" s="67" t="s">
-        <v>667</v>
+        <v>685</v>
       </c>
       <c r="L66" s="67" t="s">
-        <v>667</v>
+        <v>685</v>
       </c>
       <c r="M66" s="67"/>
       <c r="N66" s="67"/>
@@ -16836,10 +17034,10 @@
       <c r="AH66" s="67"/>
       <c r="AI66" s="67"/>
       <c r="AJ66" s="67" t="s">
-        <v>668</v>
+        <v>686</v>
       </c>
       <c r="AK66" s="67" t="s">
-        <v>669</v>
+        <v>687</v>
       </c>
       <c r="AL66" s="67"/>
       <c r="AM66" s="67"/>
@@ -16861,10 +17059,10 @@
       <c r="I67" s="67"/>
       <c r="J67" s="67"/>
       <c r="K67" s="67" t="s">
-        <v>670</v>
+        <v>688</v>
       </c>
       <c r="L67" s="67" t="s">
-        <v>670</v>
+        <v>688</v>
       </c>
       <c r="M67" s="67"/>
       <c r="N67" s="67"/>
@@ -16890,10 +17088,10 @@
       <c r="AH67" s="67"/>
       <c r="AI67" s="67"/>
       <c r="AJ67" s="67" t="s">
-        <v>671</v>
+        <v>689</v>
       </c>
       <c r="AK67" s="67" t="s">
-        <v>672</v>
+        <v>690</v>
       </c>
       <c r="AL67" s="67"/>
       <c r="AM67" s="67"/>
@@ -16915,10 +17113,10 @@
       <c r="I68" s="67"/>
       <c r="J68" s="67"/>
       <c r="K68" s="67" t="s">
-        <v>673</v>
+        <v>691</v>
       </c>
       <c r="L68" s="67" t="s">
-        <v>673</v>
+        <v>691</v>
       </c>
       <c r="M68" s="67"/>
       <c r="N68" s="67"/>
@@ -16944,10 +17142,10 @@
       <c r="AH68" s="67"/>
       <c r="AI68" s="67"/>
       <c r="AJ68" s="67" t="s">
-        <v>674</v>
+        <v>692</v>
       </c>
       <c r="AK68" s="67" t="s">
-        <v>675</v>
+        <v>693</v>
       </c>
       <c r="AL68" s="67"/>
       <c r="AM68" s="67"/>
@@ -16969,10 +17167,10 @@
       <c r="I69" s="67"/>
       <c r="J69" s="67"/>
       <c r="K69" s="67" t="s">
-        <v>676</v>
+        <v>694</v>
       </c>
       <c r="L69" s="67" t="s">
-        <v>676</v>
+        <v>694</v>
       </c>
       <c r="M69" s="67"/>
       <c r="N69" s="67"/>
@@ -16998,10 +17196,10 @@
       <c r="AH69" s="67"/>
       <c r="AI69" s="67"/>
       <c r="AJ69" s="67" t="s">
-        <v>677</v>
+        <v>695</v>
       </c>
       <c r="AK69" s="67" t="s">
-        <v>678</v>
+        <v>696</v>
       </c>
       <c r="AL69" s="67"/>
       <c r="AM69" s="67"/>
@@ -17023,10 +17221,10 @@
       <c r="I70" s="67"/>
       <c r="J70" s="67"/>
       <c r="K70" s="67" t="s">
-        <v>679</v>
+        <v>697</v>
       </c>
       <c r="L70" s="67" t="s">
-        <v>679</v>
+        <v>697</v>
       </c>
       <c r="M70" s="67"/>
       <c r="N70" s="67"/>
@@ -17052,10 +17250,10 @@
       <c r="AH70" s="67"/>
       <c r="AI70" s="67"/>
       <c r="AJ70" s="67" t="s">
-        <v>680</v>
+        <v>698</v>
       </c>
       <c r="AK70" s="67" t="s">
-        <v>681</v>
+        <v>699</v>
       </c>
       <c r="AL70" s="67"/>
       <c r="AM70" s="67"/>
@@ -17077,10 +17275,10 @@
       <c r="I71" s="67"/>
       <c r="J71" s="67"/>
       <c r="K71" s="67" t="s">
-        <v>682</v>
+        <v>700</v>
       </c>
       <c r="L71" s="67" t="s">
-        <v>682</v>
+        <v>700</v>
       </c>
       <c r="M71" s="67"/>
       <c r="N71" s="67"/>
@@ -17106,10 +17304,10 @@
       <c r="AH71" s="67"/>
       <c r="AI71" s="67"/>
       <c r="AJ71" s="67" t="s">
-        <v>683</v>
+        <v>701</v>
       </c>
       <c r="AK71" s="67" t="s">
-        <v>684</v>
+        <v>702</v>
       </c>
       <c r="AL71" s="67"/>
       <c r="AM71" s="67"/>
@@ -17131,10 +17329,10 @@
       <c r="I72" s="67"/>
       <c r="J72" s="67"/>
       <c r="K72" s="67" t="s">
-        <v>685</v>
+        <v>703</v>
       </c>
       <c r="L72" s="67" t="s">
-        <v>685</v>
+        <v>703</v>
       </c>
       <c r="M72" s="67"/>
       <c r="N72" s="67"/>
@@ -17163,7 +17361,7 @@
         <v>202</v>
       </c>
       <c r="AK72" s="67" t="s">
-        <v>686</v>
+        <v>704</v>
       </c>
       <c r="AL72" s="67"/>
       <c r="AM72" s="67"/>
@@ -17185,10 +17383,10 @@
       <c r="I73" s="67"/>
       <c r="J73" s="67"/>
       <c r="K73" s="67" t="s">
-        <v>687</v>
+        <v>705</v>
       </c>
       <c r="L73" s="67" t="s">
-        <v>687</v>
+        <v>705</v>
       </c>
       <c r="M73" s="67"/>
       <c r="N73" s="67"/>
@@ -17215,7 +17413,7 @@
       <c r="AI73" s="67"/>
       <c r="AJ73" s="67"/>
       <c r="AK73" s="67" t="s">
-        <v>688</v>
+        <v>706</v>
       </c>
       <c r="AL73" s="67"/>
       <c r="AM73" s="67"/>
@@ -17237,10 +17435,10 @@
       <c r="I74" s="67"/>
       <c r="J74" s="67"/>
       <c r="K74" s="67" t="s">
-        <v>689</v>
+        <v>707</v>
       </c>
       <c r="L74" s="67" t="s">
-        <v>689</v>
+        <v>707</v>
       </c>
       <c r="M74" s="67"/>
       <c r="N74" s="67"/>
@@ -17267,7 +17465,7 @@
       <c r="AI74" s="67"/>
       <c r="AJ74" s="67"/>
       <c r="AK74" s="67" t="s">
-        <v>690</v>
+        <v>708</v>
       </c>
       <c r="AL74" s="67"/>
       <c r="AM74" s="67"/>
@@ -17279,98 +17477,98 @@
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K75" s="67" t="s">
-        <v>691</v>
+        <v>709</v>
       </c>
       <c r="L75" s="67" t="s">
-        <v>691</v>
+        <v>709</v>
       </c>
       <c r="O75" s="68"/>
       <c r="AJ75" s="5"/>
       <c r="AK75" s="5" t="s">
-        <v>692</v>
+        <v>710</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K76" s="67" t="s">
-        <v>693</v>
+        <v>711</v>
       </c>
       <c r="L76" s="67" t="s">
-        <v>693</v>
+        <v>711</v>
       </c>
       <c r="O76" s="68"/>
       <c r="AJ76" s="5"/>
       <c r="AK76" s="5" t="s">
-        <v>694</v>
+        <v>712</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K77" s="67" t="s">
-        <v>695</v>
+        <v>713</v>
       </c>
       <c r="L77" s="67" t="s">
-        <v>695</v>
+        <v>713</v>
       </c>
       <c r="O77" s="68"/>
       <c r="AJ77" s="5"/>
       <c r="AK77" s="5" t="s">
-        <v>696</v>
+        <v>714</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K78" s="67" t="s">
-        <v>697</v>
+        <v>715</v>
       </c>
       <c r="L78" s="67" t="s">
-        <v>697</v>
+        <v>715</v>
       </c>
       <c r="O78" s="68"/>
       <c r="AJ78" s="5"/>
       <c r="AK78" s="5" t="s">
-        <v>698</v>
+        <v>716</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K79" s="67" t="s">
-        <v>699</v>
+        <v>717</v>
       </c>
       <c r="L79" s="67" t="s">
-        <v>699</v>
+        <v>717</v>
       </c>
       <c r="O79" s="68"/>
       <c r="AJ79" s="5"/>
       <c r="AK79" s="5" t="s">
-        <v>700</v>
+        <v>718</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K80" s="67" t="s">
-        <v>701</v>
+        <v>719</v>
       </c>
       <c r="L80" s="67" t="s">
-        <v>701</v>
+        <v>719</v>
       </c>
       <c r="O80" s="68"/>
       <c r="AJ80" s="5"/>
       <c r="AK80" s="5" t="s">
-        <v>702</v>
+        <v>720</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K81" s="67" t="s">
-        <v>703</v>
+        <v>721</v>
       </c>
       <c r="L81" s="67" t="s">
-        <v>703</v>
+        <v>721</v>
       </c>
       <c r="O81" s="68"/>
       <c r="AJ81" s="5"/>
       <c r="AK81" s="5" t="s">
-        <v>704</v>
+        <v>722</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K82" s="67" t="s">
-        <v>705</v>
+        <v>723</v>
       </c>
       <c r="L82" s="67" t="s">
         <v>202</v>
@@ -17378,229 +17576,229 @@
       <c r="O82" s="68"/>
       <c r="AJ82" s="5"/>
       <c r="AK82" s="5" t="s">
-        <v>706</v>
+        <v>724</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K83" s="0" t="s">
-        <v>707</v>
+        <v>725</v>
       </c>
       <c r="O83" s="68"/>
       <c r="AJ83" s="5"/>
       <c r="AK83" s="5" t="s">
-        <v>708</v>
+        <v>726</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K84" s="67" t="s">
-        <v>709</v>
+        <v>727</v>
       </c>
       <c r="O84" s="68"/>
       <c r="AJ84" s="5"/>
       <c r="AK84" s="5" t="s">
-        <v>710</v>
+        <v>728</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K85" s="0" t="s">
-        <v>711</v>
+        <v>729</v>
       </c>
       <c r="O85" s="68"/>
       <c r="Q85" s="67"/>
       <c r="AJ85" s="5"/>
       <c r="AK85" s="5" t="s">
-        <v>712</v>
+        <v>730</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K86" s="67" t="s">
-        <v>713</v>
+        <v>731</v>
       </c>
       <c r="O86" s="68"/>
       <c r="Q86" s="67"/>
       <c r="AJ86" s="5"/>
       <c r="AK86" s="5" t="s">
-        <v>714</v>
+        <v>732</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K87" s="0" t="s">
-        <v>715</v>
+        <v>733</v>
       </c>
       <c r="O87" s="68"/>
       <c r="AJ87" s="5"/>
       <c r="AK87" s="5" t="s">
-        <v>716</v>
+        <v>734</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K88" s="67" t="s">
-        <v>717</v>
+        <v>735</v>
       </c>
       <c r="O88" s="68"/>
       <c r="AJ88" s="5"/>
       <c r="AK88" s="5" t="s">
-        <v>718</v>
+        <v>736</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K89" s="67" t="s">
-        <v>719</v>
+        <v>737</v>
       </c>
       <c r="O89" s="68"/>
       <c r="AJ89" s="5"/>
       <c r="AK89" s="5" t="s">
-        <v>720</v>
+        <v>738</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K90" s="67" t="s">
-        <v>721</v>
+        <v>739</v>
       </c>
       <c r="O90" s="68"/>
       <c r="AJ90" s="5"/>
       <c r="AK90" s="5" t="s">
-        <v>722</v>
+        <v>740</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K91" s="67" t="s">
-        <v>723</v>
+        <v>741</v>
       </c>
       <c r="O91" s="68"/>
       <c r="AJ91" s="5"/>
       <c r="AK91" s="5" t="s">
-        <v>724</v>
+        <v>742</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K92" s="67" t="s">
-        <v>725</v>
+        <v>743</v>
       </c>
       <c r="O92" s="68"/>
       <c r="AJ92" s="5"/>
       <c r="AK92" s="5" t="s">
-        <v>726</v>
+        <v>744</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K93" s="67" t="s">
-        <v>727</v>
+        <v>745</v>
       </c>
       <c r="O93" s="68"/>
       <c r="AJ93" s="5"/>
       <c r="AK93" s="5" t="s">
-        <v>728</v>
+        <v>746</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K94" s="67" t="s">
-        <v>729</v>
+        <v>747</v>
       </c>
       <c r="O94" s="68"/>
       <c r="AJ94" s="5"/>
       <c r="AK94" s="5" t="s">
-        <v>730</v>
+        <v>748</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K95" s="67" t="s">
-        <v>731</v>
+        <v>749</v>
       </c>
       <c r="O95" s="68"/>
       <c r="AJ95" s="5"/>
       <c r="AK95" s="5" t="s">
-        <v>732</v>
+        <v>750</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K96" s="67" t="s">
-        <v>733</v>
+        <v>751</v>
       </c>
       <c r="O96" s="68"/>
       <c r="AJ96" s="5"/>
       <c r="AK96" s="5" t="s">
-        <v>734</v>
+        <v>752</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K97" s="67" t="s">
-        <v>735</v>
+        <v>753</v>
       </c>
       <c r="O97" s="68"/>
       <c r="AJ97" s="5"/>
       <c r="AK97" s="5" t="s">
-        <v>736</v>
+        <v>754</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K98" s="67" t="s">
-        <v>737</v>
+        <v>755</v>
       </c>
       <c r="O98" s="68"/>
       <c r="AJ98" s="5"/>
       <c r="AK98" s="5" t="s">
-        <v>738</v>
+        <v>756</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K99" s="67" t="s">
-        <v>739</v>
+        <v>757</v>
       </c>
       <c r="O99" s="68"/>
       <c r="AJ99" s="5"/>
       <c r="AK99" s="5" t="s">
-        <v>740</v>
+        <v>758</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K100" s="67" t="s">
-        <v>741</v>
+        <v>759</v>
       </c>
       <c r="O100" s="68"/>
       <c r="AJ100" s="5"/>
       <c r="AK100" s="5" t="s">
-        <v>742</v>
+        <v>760</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K101" s="67" t="s">
-        <v>743</v>
+        <v>761</v>
       </c>
       <c r="O101" s="68"/>
       <c r="AJ101" s="5"/>
       <c r="AK101" s="5" t="s">
-        <v>744</v>
+        <v>762</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K102" s="67" t="s">
-        <v>745</v>
+        <v>763</v>
       </c>
       <c r="O102" s="68"/>
       <c r="AJ102" s="5"/>
       <c r="AK102" s="5" t="s">
-        <v>746</v>
+        <v>764</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K103" s="67" t="s">
-        <v>747</v>
+        <v>765</v>
       </c>
       <c r="O103" s="68"/>
       <c r="AJ103" s="5"/>
       <c r="AK103" s="5" t="s">
-        <v>748</v>
+        <v>766</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="K104" s="67" t="s">
-        <v>749</v>
+        <v>767</v>
       </c>
       <c r="O104" s="68"/>
       <c r="AJ104" s="5"/>
       <c r="AK104" s="5" t="s">
-        <v>750</v>
+        <v>768</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17610,182 +17808,182 @@
       <c r="O105" s="68"/>
       <c r="AJ105" s="5"/>
       <c r="AK105" s="5" t="s">
-        <v>751</v>
+        <v>769</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O106" s="68"/>
       <c r="AJ106" s="5"/>
       <c r="AK106" s="5" t="s">
-        <v>752</v>
+        <v>770</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O107" s="68"/>
       <c r="AJ107" s="5"/>
       <c r="AK107" s="5" t="s">
-        <v>753</v>
+        <v>771</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O108" s="68"/>
       <c r="AJ108" s="5"/>
       <c r="AK108" s="5" t="s">
-        <v>754</v>
+        <v>772</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O109" s="68"/>
       <c r="AJ109" s="5"/>
       <c r="AK109" s="5" t="s">
-        <v>755</v>
+        <v>773</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O110" s="68"/>
       <c r="AJ110" s="5"/>
       <c r="AK110" s="5" t="s">
-        <v>756</v>
+        <v>774</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O111" s="68"/>
       <c r="AJ111" s="5"/>
       <c r="AK111" s="5" t="s">
-        <v>757</v>
+        <v>775</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O112" s="68"/>
       <c r="AJ112" s="5"/>
       <c r="AK112" s="5" t="s">
-        <v>758</v>
+        <v>776</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O113" s="68"/>
       <c r="AJ113" s="5"/>
       <c r="AK113" s="5" t="s">
-        <v>759</v>
+        <v>777</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O114" s="68"/>
       <c r="AJ114" s="5"/>
       <c r="AK114" s="5" t="s">
-        <v>760</v>
+        <v>778</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O115" s="68"/>
       <c r="AJ115" s="5"/>
       <c r="AK115" s="5" t="s">
-        <v>761</v>
+        <v>779</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O116" s="68"/>
       <c r="AJ116" s="5"/>
       <c r="AK116" s="5" t="s">
-        <v>438</v>
+        <v>456</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O117" s="68"/>
       <c r="AJ117" s="5"/>
       <c r="AK117" s="5" t="s">
-        <v>446</v>
+        <v>464</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O118" s="68"/>
       <c r="AJ118" s="5"/>
       <c r="AK118" s="5" t="s">
-        <v>452</v>
+        <v>470</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O119" s="68"/>
       <c r="AJ119" s="5"/>
       <c r="AK119" s="5" t="s">
-        <v>438</v>
+        <v>456</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O120" s="68"/>
       <c r="AJ120" s="5"/>
       <c r="AK120" s="5" t="s">
-        <v>446</v>
+        <v>464</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O121" s="68"/>
       <c r="AJ121" s="5"/>
       <c r="AK121" s="5" t="s">
-        <v>452</v>
+        <v>470</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O122" s="68"/>
       <c r="AJ122" s="5"/>
       <c r="AK122" s="5" t="s">
-        <v>762</v>
+        <v>780</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O123" s="68"/>
       <c r="AJ123" s="5"/>
       <c r="AK123" s="5" t="s">
-        <v>763</v>
+        <v>781</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O124" s="68"/>
       <c r="AJ124" s="5"/>
       <c r="AK124" s="5" t="s">
-        <v>764</v>
+        <v>782</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O125" s="68"/>
       <c r="AJ125" s="5"/>
       <c r="AK125" s="5" t="s">
-        <v>765</v>
+        <v>783</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O126" s="68"/>
       <c r="AJ126" s="5"/>
       <c r="AK126" s="5" t="s">
-        <v>766</v>
+        <v>784</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O127" s="68"/>
       <c r="AJ127" s="5"/>
       <c r="AK127" s="5" t="s">
-        <v>767</v>
+        <v>785</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O128" s="68"/>
       <c r="AJ128" s="5"/>
       <c r="AK128" s="5" t="s">
-        <v>768</v>
+        <v>786</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O129" s="68"/>
       <c r="AJ129" s="5"/>
       <c r="AK129" s="5" t="s">
-        <v>769</v>
+        <v>787</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="O130" s="68"/>
       <c r="AJ130" s="5"/>
       <c r="AK130" s="5" t="s">
-        <v>770</v>
+        <v>788</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -18686,7 +18884,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="AV12 A2"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -18699,27 +18897,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="72" t="s">
-        <v>771</v>
+        <v>789</v>
       </c>
       <c r="B1" s="72" t="s">
-        <v>772</v>
+        <v>790</v>
       </c>
       <c r="C1" s="72" t="s">
-        <v>773</v>
+        <v>791</v>
       </c>
       <c r="D1" s="72" t="s">
-        <v>774</v>
+        <v>792</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="73" t="s">
-        <v>775</v>
+        <v>793</v>
       </c>
       <c r="B2" s="73" t="s">
-        <v>776</v>
+        <v>794</v>
       </c>
       <c r="C2" s="73" t="s">
-        <v>777</v>
+        <v>795</v>
       </c>
       <c r="D2" s="74" t="n">
         <v>45253</v>
@@ -18727,13 +18925,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="75" t="s">
-        <v>778</v>
+        <v>796</v>
       </c>
       <c r="B3" s="75" t="s">
-        <v>779</v>
+        <v>797</v>
       </c>
       <c r="C3" s="76" t="s">
-        <v>780</v>
+        <v>798</v>
       </c>
       <c r="D3" s="77" t="n">
         <v>45265</v>
@@ -18741,13 +18939,13 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="73" t="s">
-        <v>781</v>
+        <v>799</v>
       </c>
       <c r="B4" s="78" t="s">
-        <v>782</v>
+        <v>800</v>
       </c>
       <c r="C4" s="79" t="s">
-        <v>783</v>
+        <v>801</v>
       </c>
       <c r="D4" s="80" t="n">
         <v>45310</v>
@@ -18755,13 +18953,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="81" t="s">
-        <v>784</v>
+        <v>802</v>
       </c>
       <c r="B5" s="82" t="s">
-        <v>785</v>
+        <v>803</v>
       </c>
       <c r="C5" s="83" t="s">
-        <v>783</v>
+        <v>801</v>
       </c>
       <c r="D5" s="84" t="n">
         <v>45313</v>
@@ -18769,13 +18967,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="73" t="s">
-        <v>786</v>
+        <v>804</v>
       </c>
       <c r="B6" s="73" t="s">
-        <v>787</v>
+        <v>805</v>
       </c>
       <c r="C6" s="79" t="s">
-        <v>783</v>
+        <v>801</v>
       </c>
       <c r="D6" s="85" t="n">
         <v>45314</v>
@@ -18783,13 +18981,13 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="81" t="s">
-        <v>788</v>
+        <v>806</v>
       </c>
       <c r="B7" s="82" t="s">
-        <v>789</v>
+        <v>807</v>
       </c>
       <c r="C7" s="83" t="s">
-        <v>790</v>
+        <v>808</v>
       </c>
       <c r="D7" s="84" t="n">
         <v>45316</v>
@@ -18797,13 +18995,13 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="86" t="s">
-        <v>791</v>
+        <v>809</v>
       </c>
       <c r="B8" s="86" t="s">
-        <v>792</v>
+        <v>810</v>
       </c>
       <c r="C8" s="87" t="s">
-        <v>793</v>
+        <v>811</v>
       </c>
       <c r="D8" s="88" t="n">
         <v>45316</v>
@@ -18829,10 +19027,10 @@
   <dimension ref="A1:AA1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="24"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="37.14"/>
@@ -18840,7 +19038,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="37.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="41.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="55.7"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="70.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="70.31"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="32.15"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="46.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="30.28"/>
@@ -20350,10 +20548,10 @@
   <dimension ref="A1:M1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
@@ -20478,7 +20676,7 @@
         <v>66</v>
       </c>
       <c r="J3" s="102" t="s">
-        <v>295</v>
+        <v>313</v>
       </c>
       <c r="K3" s="7" t="s">
         <v>70</v>
@@ -20501,13 +20699,13 @@
       <c r="H4" s="103"/>
       <c r="I4" s="103"/>
       <c r="J4" s="103" t="s">
-        <v>794</v>
+        <v>812</v>
       </c>
       <c r="K4" s="103" t="s">
-        <v>795</v>
+        <v>813</v>
       </c>
       <c r="L4" s="103" t="s">
-        <v>796</v>
+        <v>814</v>
       </c>
       <c r="M4" s="103"/>
     </row>
@@ -20522,7 +20720,7 @@
       <c r="H5" s="103"/>
       <c r="I5" s="103"/>
       <c r="J5" s="104" t="s">
-        <v>797</v>
+        <v>815</v>
       </c>
       <c r="K5" s="103"/>
       <c r="L5" s="103"/>
@@ -22023,10 +22221,10 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
@@ -22083,7 +22281,7 @@
         <v>84</v>
       </c>
       <c r="D2" s="55" t="s">
-        <v>290</v>
+        <v>308</v>
       </c>
       <c r="E2" s="55" t="s">
         <v>91</v>
@@ -22114,7 +22312,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>798</v>
+        <v>816</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>83</v>
@@ -24072,15 +24270,15 @@
   <dimension ref="A1:S1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="33.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="32.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="91.87"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="91.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="6" style="0" width="41.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="45.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="31.15"/>
@@ -24213,13 +24411,13 @@
         <v>194</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>798</v>
+        <v>816</v>
       </c>
       <c r="C3" s="110" t="s">
         <v>95</v>
       </c>
       <c r="D3" s="110" t="s">
-        <v>799</v>
+        <v>817</v>
       </c>
       <c r="E3" s="114" t="s">
         <v>101</v>
@@ -24234,13 +24432,13 @@
         <v>113</v>
       </c>
       <c r="I3" s="115" t="s">
-        <v>296</v>
+        <v>314</v>
       </c>
       <c r="J3" s="110" t="s">
-        <v>297</v>
+        <v>315</v>
       </c>
       <c r="K3" s="110" t="s">
-        <v>298</v>
+        <v>316</v>
       </c>
       <c r="L3" s="110" t="s">
         <v>126</v>
@@ -25993,10 +26191,10 @@
   <dimension ref="A1:Y1000"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="AV12 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.77734375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="39.14"/>
@@ -26090,7 +26288,7 @@
         <v>194</v>
       </c>
       <c r="B3" s="119" t="s">
-        <v>798</v>
+        <v>816</v>
       </c>
       <c r="C3" s="127" t="s">
         <v>158</v>

</xml_diff>